<commit_message>
renommage de la page 2 et modification de son titre pour qu il soit unique et precis
</commit_message>
<xml_diff>
--- a/Maquette-Sources/Modèle-audit-SEO.xlsx
+++ b/Maquette-Sources/Modèle-audit-SEO.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$H$34</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -100,6 +103,21 @@
     <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast</t>
   </si>
   <si>
+    <t xml:space="preserve">pour les liens du footer : couleur : #3B3B3B minimum pour AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">texte dans les images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inaccessible par les lecteurs d’écran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">préférer écrire les textes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">contenu des attributs alt utilisé pour des keywords pas pour des textes alternatifs</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO</t>
   </si>
   <si>
@@ -170,6 +188,69 @@
   </si>
   <si>
     <t xml:space="preserve">nom de fichiers image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise meta keywords, div keywords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">methode de black hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les supprimer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Learn/HTML/Introduction_to_HTML/The_head_metadata_in_HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mis en commentaire à nettoyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise meta description vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la balise description est utilisée par les moteurs de recherche pour l’indexation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter une description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image 1à4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images non significatives </t>
+  </si>
+  <si>
+    <t xml:space="preserve">à mettre en background image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image 1/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plus qrande que la zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adapter le contenu au contenant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les retailler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image 3/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">format BMP / format lourd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pour du background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les compresser en png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO /CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abus du !important ?</t>
   </si>
 </sst>
 </file>
@@ -179,7 +260,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -231,12 +312,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -286,7 +361,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,12 +386,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -391,6 +470,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -399,17 +482,19 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="57.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="57.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="1" width="10.57"/>
@@ -516,7 +601,7 @@
       <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -529,24 +614,45 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="E6" s="5"/>
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="0"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="G9" s="0"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E10" s="5"/>
@@ -575,19 +681,19 @@
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>13</v>
@@ -595,13 +701,13 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>13</v>
@@ -609,76 +715,161 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="35.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="0"/>
+      <c r="E31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="57.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1645,6 +1836,7 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A1:H34"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
@@ -1656,5 +1848,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modification des images du carrousel et de leur description
</commit_message>
<xml_diff>
--- a/Maquette-Sources/Modèle-audit-SEO.xlsx
+++ b/Maquette-Sources/Modèle-audit-SEO.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$H$34</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -52,19 +52,28 @@
     <t xml:space="preserve">(SEO ou accessiblité ?)</t>
   </si>
   <si>
+    <t xml:space="preserve">(à faire ou non)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdn, article spécialisé, cours</t>
+  </si>
+  <si>
     <t xml:space="preserve">accessibilité</t>
   </si>
   <si>
     <t xml:space="preserve">Langue absente (default)</t>
   </si>
   <si>
-    <t xml:space="preserve">les dispositifs d’assistance vocale ne reconnaîtrons pas la langue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ajouter lang=’fr’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fait</t>
+    <t xml:space="preserve">Avec lang=default, les dispositifs d’assistance vocale ne reconnaîtrons pas la langue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indiquer la langue dans laquelle est rédigée la page (c’est-à-dire : fr pour français). Pour éviter les problèmes de prononciation on peut même préciser fr-fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"></t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/International/questions/qa-lang-why.fr</t>
   </si>
   <si>
     <t xml:space="preserve">Lien des réseau sociaux sans texte</t>
@@ -73,10 +82,10 @@
     <t xml:space="preserve">les dispositifs d’assistance vocale ne pourront pas indiquer la destination du lien</t>
   </si>
   <si>
-    <t xml:space="preserve">ajouter un texte alternatif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ajouter du texte sous forme de ‘title’</t>
+    <t xml:space="preserve">ajouter du texte sous forme de ‘title’ et d’un aria-label dans le lien le contenant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fontawesome.com/v5.15/how-to-use/on-the-web/other-topics/accessibility</t>
   </si>
   <si>
     <t xml:space="preserve">contraste de couleurs</t>
@@ -88,7 +97,7 @@
     <t xml:space="preserve">augmenter le contraste des couleurs</t>
   </si>
   <si>
-    <t xml:space="preserve">modifier la couleur </t>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Learn/Accessibility/CSS_and_JavaScript#couleur_et_contraste_de_couleur</t>
@@ -118,78 +127,108 @@
     <t xml:space="preserve">contenu des attributs alt utilisé pour des keywords pas pour des textes alternatifs</t>
   </si>
   <si>
+    <t xml:space="preserve">accessibilité /référencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hiérarchie des titres non respaectée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1→H6 alors que h1→h3→h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter un titre h2 nos activités</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO + Bonne pratique SASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Présence d’attribut style dans les balises HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour simplifier le référencement du site, il faut simplifier le travail des BOT Google et ne pas éparpiller le CSS dans de nombreux fichiers. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il est préférable de le mettre que dans 1 ou 2 fichiers. De plus, il rendra le site plus facilement maintenable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ornitorinc.com/blog/referencement/10-bonnes-pratiques-referencement-seo/</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO</t>
   </si>
   <si>
-    <t xml:space="preserve">du style dans les balises HTML</t>
+    <t xml:space="preserve">title de la page index ‘.’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problème d’indexation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La balise &lt;title&gt; indique aux internautes et aux moteurs de recherche le sujet d'une page spécifique. Insérez la balise &lt;title&gt; dans l'élément &lt;head&gt; du document HTML et créez un titre unique pour chaque page du site. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nom de la page2+title → contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donner un nom de page unique et précis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">renommer la page en contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developers.google.com/search/docs/beginner/seo-starter-guide?hl=fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le bouton contact est en 2 exemplaires + 2 liens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le dédoublonner : 1 lien en haut (page 2&gt;) retirer le bouton du haut mettre celui du bas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer le bouton du bas car il y a déjà ceux des réseaux sociaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">à revoir car lien aussi en haut dans ul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SASS : bonne pratique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class white, bgc-white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">probleme pour la mise à jour si on change la couleur.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre un nom de class significatif sans référence de couleur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pas de h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le W3C demande à respecter la progression des titres et de ne pas sauter de niveau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ne pas sauter de niveau de titre h1→h3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplacer le h3 par h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/Heading_Elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remarque à revoir car h2 aprés h3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nom de fichiers image</t>
   </si>
   <si>
     <t xml:space="preserve">difficulté de mise à jour</t>
   </si>
   <si>
-    <t xml:space="preserve">mettre le css dans le fichier CSS pour améliorer la facilité de MAJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nettoyer les fichier HTML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title de la page index ‘.’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">problème d’indexation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le bouton contact est en 2 exemplaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le dédoublonner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supprimer le bouton du bas car il y a déjà ceux des réseaux sociaux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">à revoir car lien aussi en haut dans ul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEO /SASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class white, bgc-white</t>
-  </si>
-  <si>
-    <t xml:space="preserve">probleme pour la mise à jour si on change la couleur.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre un nom de class significatif sans référence de couleur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">renommer la classe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pas de h2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le W3C demande à respecter la progression des titres et de ne pas sauter de niveau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ne pas sauter de niveau de titre h1→h3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remplacer le h3 par h2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/Heading_Elements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remarque à revoir car h2 aprés h3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nom de fichiers image</t>
-  </si>
-  <si>
     <t xml:space="preserve">balise meta keywords, div keywords</t>
   </si>
   <si>
@@ -214,13 +253,22 @@
     <t xml:space="preserve">ajouter une description</t>
   </si>
   <si>
+    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agence de web design</t>
+  </si>
+  <si>
     <t xml:space="preserve">image 1à4</t>
   </si>
   <si>
-    <t xml:space="preserve">images non significatives </t>
-  </si>
-  <si>
-    <t xml:space="preserve">à mettre en background image</t>
+    <t xml:space="preserve">les renommer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nom de fichier parlant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.codeur.com/blog/seo-image-google/</t>
   </si>
   <si>
     <t xml:space="preserve">Image 1/2</t>
@@ -247,10 +295,19 @@
     <t xml:space="preserve">les compresser en png</t>
   </si>
   <si>
-    <t xml:space="preserve">SEO /CSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abus du !important ?</t>
+    <t xml:space="preserve">utiliser balises sémantique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problème de référencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex bloc-0 →nav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annuaire liste 1 et 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soit à mettre dans une page ‘annuaire’ soit supprimer les 404</t>
   </si>
 </sst>
 </file>
@@ -260,7 +317,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -312,8 +369,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Symbol"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,8 +392,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -336,7 +418,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -360,8 +442,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -370,7 +455,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -386,6 +471,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -398,15 +487,44 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Sans nom1" xfId="20"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="12"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF81D41A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -451,7 +569,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -479,19 +597,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="57.97"/>
@@ -549,110 +667,127 @@
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="66.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>18</v>
+      <c r="A5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
       <c r="E6" s="5"/>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="8"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="G9" s="8"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E10" s="5"/>
@@ -679,200 +814,255 @@
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="133.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="58.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" s="12" customFormat="true" ht="116.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="35.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="35.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="0"/>
+        <v>69</v>
+      </c>
       <c r="E31" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="57.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+      <c r="D32" s="0"/>
+      <c r="E32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="57.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>86</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+    </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1835,12 +2025,18 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:H34"/>
+  <autoFilter ref="A1:H35"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
   </mergeCells>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula></formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
nettoyage des logos de l'agence + suppression de l'image title2 remplacée par un paragraphe de texte
</commit_message>
<xml_diff>
--- a/Maquette-Sources/Modèle-audit-SEO.xlsx
+++ b/Maquette-Sources/Modèle-audit-SEO.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$H$35</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -127,16 +127,19 @@
     <t xml:space="preserve">contenu des attributs alt utilisé pour des keywords pas pour des textes alternatifs</t>
   </si>
   <si>
-    <t xml:space="preserve">accessibilité /référencement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hiérarchie des titres non respaectée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h1→H6 alors que h1→h3→h2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ajouter un titre h2 nos activités</t>
+    <t xml:space="preserve">SEO et accesibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il y a un saut de h1 à h3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le W3C demande à respecter la progression des titres et de ne pas sauter de niveau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on peut ajouter un h2 entre le h1 et le h3 ex : nos activités</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/Heading_Elements</t>
   </si>
   <si>
     <t xml:space="preserve">SEO + Bonne pratique SASS</t>
@@ -205,30 +208,6 @@
     <t xml:space="preserve">mettre un nom de class significatif sans référence de couleur</t>
   </si>
   <si>
-    <t xml:space="preserve">pas de h2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le W3C demande à respecter la progression des titres et de ne pas sauter de niveau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ne pas sauter de niveau de titre h1→h3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remplacer le h3 par h2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/Heading_Elements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remarque à revoir car h2 aprés h3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nom de fichiers image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">difficulté de mise à jour</t>
-  </si>
-  <si>
     <t xml:space="preserve">balise meta keywords, div keywords</t>
   </si>
   <si>
@@ -250,64 +229,73 @@
     <t xml:space="preserve">la balise description est utilisée par les moteurs de recherche pour l’indexation</t>
   </si>
   <si>
-    <t xml:space="preserve">ajouter une description</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages</t>
   </si>
   <si>
-    <t xml:space="preserve">agence de web design</t>
-  </si>
-  <si>
     <t xml:space="preserve">image 1à4</t>
   </si>
   <si>
-    <t xml:space="preserve">les renommer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nom de fichier parlant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.codeur.com/blog/seo-image-google/</t>
+    <t xml:space="preserve">des noms vagues et non-significatifs et leur attributs alt répétitifs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le nom des images et leur balises alt aide google pour le référencement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.codeur.com/blog/seo-image-google/ + https://www.anthedesign.fr/referencement/seo-comment-optimiser-le-referencement-des-images/</t>
   </si>
   <si>
     <t xml:space="preserve">Image 1/2</t>
   </si>
   <si>
-    <t xml:space="preserve">plus qrande que la zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adapter le contenu au contenant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">les retailler</t>
+    <t xml:space="preserve">les images sont plus grandes que la zone d’affichage. Elles ont un poids qui augmente le temps de chargement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il faut dans la mesure du possible avoir des images à la taille de l’affichage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.anthedesign.fr/referencement/seo-comment-optimiser-le-referencement-des-images/</t>
   </si>
   <si>
     <t xml:space="preserve">Image 3/4</t>
   </si>
   <si>
-    <t xml:space="preserve">format BMP / format lourd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pour du background</t>
-  </si>
-  <si>
-    <t xml:space="preserve">les compresser en png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">utiliser balises sémantique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">problème de référencement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ex bloc-0 →nav</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annuaire liste 1 et 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soit à mettre dans une page ‘annuaire’ soit supprimer les 404</t>
+    <t xml:space="preserve">le format BMP est un format lourd qui n’est pas forcément lu par les moteurs de recherche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les convertir en PNG et les retailler à la bonne taille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image_de_presenation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l’image de fond est au format BMP qui est un format lourd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utiliser de préférence des images plus légères comme des format PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les liens du footer sont nombreux et renvoient vers des pages 404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vu le nombre de lien, il aurait été interressant de créer une page dédiée. Mais vu qu’ils renvoie tous vers des pages 404, il faut les supprimer sous peine que le site soit considéré comme non mis régulièrement à jour et améliorer l’expérience utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il faut supprimer tous les liens 404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.leptidigital.fr/webmarketing/seo/erreurs-404-seo-16902/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images inutiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il n’y a que des div bloc xx, pas de réel header / footer /main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les blocs header / footer / main permet aux robot de connaître le rôle de chaque partie de la page et leur signifier où se trouve le contenu important</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/</t>
   </si>
 </sst>
 </file>
@@ -446,7 +434,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -488,10 +476,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -597,12 +581,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -764,7 +748,9 @@
       <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
@@ -773,7 +759,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -786,8 +772,12 @@
       <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="G9" s="9"/>
+      <c r="E9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E10" s="5"/>
@@ -816,252 +806,1285 @@
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="133.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="58.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="27" s="12" customFormat="true" ht="116.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="12" t="s">
+    <row r="27" s="11" customFormat="true" ht="116.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>59</v>
       </c>
+      <c r="D27" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="28" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>65</v>
-      </c>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="I28" s="0"/>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+      <c r="M28" s="0"/>
+      <c r="N28" s="0"/>
+      <c r="O28" s="0"/>
+      <c r="P28" s="0"/>
+      <c r="Q28" s="0"/>
+      <c r="R28" s="0"/>
+      <c r="S28" s="0"/>
+      <c r="T28" s="0"/>
+      <c r="U28" s="0"/>
+      <c r="V28" s="0"/>
+      <c r="W28" s="0"/>
+      <c r="X28" s="0"/>
+      <c r="Y28" s="0"/>
+      <c r="Z28" s="0"/>
+      <c r="AA28" s="0"/>
+      <c r="AB28" s="0"/>
+      <c r="AC28" s="0"/>
+      <c r="AD28" s="0"/>
+      <c r="AE28" s="0"/>
+      <c r="AF28" s="0"/>
+      <c r="AG28" s="0"/>
+      <c r="AH28" s="0"/>
+      <c r="AI28" s="0"/>
+      <c r="AJ28" s="0"/>
+      <c r="AK28" s="0"/>
+      <c r="AL28" s="0"/>
+      <c r="AM28" s="0"/>
+      <c r="AN28" s="0"/>
+      <c r="AO28" s="0"/>
+      <c r="AP28" s="0"/>
+      <c r="AQ28" s="0"/>
+      <c r="AR28" s="0"/>
+      <c r="AS28" s="0"/>
+      <c r="AT28" s="0"/>
+      <c r="AU28" s="0"/>
+      <c r="AV28" s="0"/>
+      <c r="AW28" s="0"/>
+      <c r="AX28" s="0"/>
+      <c r="AY28" s="0"/>
+      <c r="AZ28" s="0"/>
+      <c r="BA28" s="0"/>
+      <c r="BB28" s="0"/>
+      <c r="BC28" s="0"/>
+      <c r="BD28" s="0"/>
+      <c r="BE28" s="0"/>
+      <c r="BF28" s="0"/>
+      <c r="BG28" s="0"/>
+      <c r="BH28" s="0"/>
+      <c r="BI28" s="0"/>
+      <c r="BJ28" s="0"/>
+      <c r="BK28" s="0"/>
+      <c r="BL28" s="0"/>
+      <c r="BM28" s="0"/>
+      <c r="BN28" s="0"/>
+      <c r="BO28" s="0"/>
+      <c r="BP28" s="0"/>
+      <c r="BQ28" s="0"/>
+      <c r="BR28" s="0"/>
+      <c r="BS28" s="0"/>
+      <c r="BT28" s="0"/>
+      <c r="BU28" s="0"/>
+      <c r="BV28" s="0"/>
+      <c r="BW28" s="0"/>
+      <c r="BX28" s="0"/>
+      <c r="BY28" s="0"/>
+      <c r="BZ28" s="0"/>
+      <c r="CA28" s="0"/>
+      <c r="CB28" s="0"/>
+      <c r="CC28" s="0"/>
+      <c r="CD28" s="0"/>
+      <c r="CE28" s="0"/>
+      <c r="CF28" s="0"/>
+      <c r="CG28" s="0"/>
+      <c r="CH28" s="0"/>
+      <c r="CI28" s="0"/>
+      <c r="CJ28" s="0"/>
+      <c r="CK28" s="0"/>
+      <c r="CL28" s="0"/>
+      <c r="CM28" s="0"/>
+      <c r="CN28" s="0"/>
+      <c r="CO28" s="0"/>
+      <c r="CP28" s="0"/>
+      <c r="CQ28" s="0"/>
+      <c r="CR28" s="0"/>
+      <c r="CS28" s="0"/>
+      <c r="CT28" s="0"/>
+      <c r="CU28" s="0"/>
+      <c r="CV28" s="0"/>
+      <c r="CW28" s="0"/>
+      <c r="CX28" s="0"/>
+      <c r="CY28" s="0"/>
+      <c r="CZ28" s="0"/>
+      <c r="DA28" s="0"/>
+      <c r="DB28" s="0"/>
+      <c r="DC28" s="0"/>
+      <c r="DD28" s="0"/>
+      <c r="DE28" s="0"/>
+      <c r="DF28" s="0"/>
+      <c r="DG28" s="0"/>
+      <c r="DH28" s="0"/>
+      <c r="DI28" s="0"/>
+      <c r="DJ28" s="0"/>
+      <c r="DK28" s="0"/>
+      <c r="DL28" s="0"/>
+      <c r="DM28" s="0"/>
+      <c r="DN28" s="0"/>
+      <c r="DO28" s="0"/>
+      <c r="DP28" s="0"/>
+      <c r="DQ28" s="0"/>
+      <c r="DR28" s="0"/>
+      <c r="DS28" s="0"/>
+      <c r="DT28" s="0"/>
+      <c r="DU28" s="0"/>
+      <c r="DV28" s="0"/>
+      <c r="DW28" s="0"/>
+      <c r="DX28" s="0"/>
+      <c r="DY28" s="0"/>
+      <c r="DZ28" s="0"/>
+      <c r="EA28" s="0"/>
+      <c r="EB28" s="0"/>
+      <c r="EC28" s="0"/>
+      <c r="ED28" s="0"/>
+      <c r="EE28" s="0"/>
+      <c r="EF28" s="0"/>
+      <c r="EG28" s="0"/>
+      <c r="EH28" s="0"/>
+      <c r="EI28" s="0"/>
+      <c r="EJ28" s="0"/>
+      <c r="EK28" s="0"/>
+      <c r="EL28" s="0"/>
+      <c r="EM28" s="0"/>
+      <c r="EN28" s="0"/>
+      <c r="EO28" s="0"/>
+      <c r="EP28" s="0"/>
+      <c r="EQ28" s="0"/>
+      <c r="ER28" s="0"/>
+      <c r="ES28" s="0"/>
+      <c r="ET28" s="0"/>
+      <c r="EU28" s="0"/>
+      <c r="EV28" s="0"/>
+      <c r="EW28" s="0"/>
+      <c r="EX28" s="0"/>
+      <c r="EY28" s="0"/>
+      <c r="EZ28" s="0"/>
+      <c r="FA28" s="0"/>
+      <c r="FB28" s="0"/>
+      <c r="FC28" s="0"/>
+      <c r="FD28" s="0"/>
+      <c r="FE28" s="0"/>
+      <c r="FF28" s="0"/>
+      <c r="FG28" s="0"/>
+      <c r="FH28" s="0"/>
+      <c r="FI28" s="0"/>
+      <c r="FJ28" s="0"/>
+      <c r="FK28" s="0"/>
+      <c r="FL28" s="0"/>
+      <c r="FM28" s="0"/>
+      <c r="FN28" s="0"/>
+      <c r="FO28" s="0"/>
+      <c r="FP28" s="0"/>
+      <c r="FQ28" s="0"/>
+      <c r="FR28" s="0"/>
+      <c r="FS28" s="0"/>
+      <c r="FT28" s="0"/>
+      <c r="FU28" s="0"/>
+      <c r="FV28" s="0"/>
+      <c r="FW28" s="0"/>
+      <c r="FX28" s="0"/>
+      <c r="FY28" s="0"/>
+      <c r="FZ28" s="0"/>
+      <c r="GA28" s="0"/>
+      <c r="GB28" s="0"/>
+      <c r="GC28" s="0"/>
+      <c r="GD28" s="0"/>
+      <c r="GE28" s="0"/>
+      <c r="GF28" s="0"/>
+      <c r="GG28" s="0"/>
+      <c r="GH28" s="0"/>
+      <c r="GI28" s="0"/>
+      <c r="GJ28" s="0"/>
+      <c r="GK28" s="0"/>
+      <c r="GL28" s="0"/>
+      <c r="GM28" s="0"/>
+      <c r="GN28" s="0"/>
+      <c r="GO28" s="0"/>
+      <c r="GP28" s="0"/>
+      <c r="GQ28" s="0"/>
+      <c r="GR28" s="0"/>
+      <c r="GS28" s="0"/>
+      <c r="GT28" s="0"/>
+      <c r="GU28" s="0"/>
+      <c r="GV28" s="0"/>
+      <c r="GW28" s="0"/>
+      <c r="GX28" s="0"/>
+      <c r="GY28" s="0"/>
+      <c r="GZ28" s="0"/>
+      <c r="HA28" s="0"/>
+      <c r="HB28" s="0"/>
+      <c r="HC28" s="0"/>
+      <c r="HD28" s="0"/>
+      <c r="HE28" s="0"/>
+      <c r="HF28" s="0"/>
+      <c r="HG28" s="0"/>
+      <c r="HH28" s="0"/>
+      <c r="HI28" s="0"/>
+      <c r="HJ28" s="0"/>
+      <c r="HK28" s="0"/>
+      <c r="HL28" s="0"/>
+      <c r="HM28" s="0"/>
+      <c r="HN28" s="0"/>
+      <c r="HO28" s="0"/>
+      <c r="HP28" s="0"/>
+      <c r="HQ28" s="0"/>
+      <c r="HR28" s="0"/>
+      <c r="HS28" s="0"/>
+      <c r="HT28" s="0"/>
+      <c r="HU28" s="0"/>
+      <c r="HV28" s="0"/>
+      <c r="HW28" s="0"/>
+      <c r="HX28" s="0"/>
+      <c r="HY28" s="0"/>
+      <c r="HZ28" s="0"/>
+      <c r="IA28" s="0"/>
+      <c r="IB28" s="0"/>
+      <c r="IC28" s="0"/>
+      <c r="ID28" s="0"/>
+      <c r="IE28" s="0"/>
+      <c r="IF28" s="0"/>
+      <c r="IG28" s="0"/>
+      <c r="IH28" s="0"/>
+      <c r="II28" s="0"/>
+      <c r="IJ28" s="0"/>
+      <c r="IK28" s="0"/>
+      <c r="IL28" s="0"/>
+      <c r="IM28" s="0"/>
+      <c r="IN28" s="0"/>
+      <c r="IO28" s="0"/>
+      <c r="IP28" s="0"/>
+      <c r="IQ28" s="0"/>
+      <c r="IR28" s="0"/>
+      <c r="IS28" s="0"/>
+      <c r="IT28" s="0"/>
+      <c r="IU28" s="0"/>
+      <c r="IV28" s="0"/>
+      <c r="IW28" s="0"/>
+      <c r="IX28" s="0"/>
+      <c r="IY28" s="0"/>
+      <c r="IZ28" s="0"/>
+      <c r="JA28" s="0"/>
+      <c r="JB28" s="0"/>
+      <c r="JC28" s="0"/>
+      <c r="JD28" s="0"/>
+      <c r="JE28" s="0"/>
+      <c r="JF28" s="0"/>
+      <c r="JG28" s="0"/>
+      <c r="JH28" s="0"/>
+      <c r="JI28" s="0"/>
+      <c r="JJ28" s="0"/>
+      <c r="JK28" s="0"/>
+      <c r="JL28" s="0"/>
+      <c r="JM28" s="0"/>
+      <c r="JN28" s="0"/>
+      <c r="JO28" s="0"/>
+      <c r="JP28" s="0"/>
+      <c r="JQ28" s="0"/>
+      <c r="JR28" s="0"/>
+      <c r="JS28" s="0"/>
+      <c r="JT28" s="0"/>
+      <c r="JU28" s="0"/>
+      <c r="JV28" s="0"/>
+      <c r="JW28" s="0"/>
+      <c r="JX28" s="0"/>
+      <c r="JY28" s="0"/>
+      <c r="JZ28" s="0"/>
+      <c r="KA28" s="0"/>
+      <c r="KB28" s="0"/>
+      <c r="KC28" s="0"/>
+      <c r="KD28" s="0"/>
+      <c r="KE28" s="0"/>
+      <c r="KF28" s="0"/>
+      <c r="KG28" s="0"/>
+      <c r="KH28" s="0"/>
+      <c r="KI28" s="0"/>
+      <c r="KJ28" s="0"/>
+      <c r="KK28" s="0"/>
+      <c r="KL28" s="0"/>
+      <c r="KM28" s="0"/>
+      <c r="KN28" s="0"/>
+      <c r="KO28" s="0"/>
+      <c r="KP28" s="0"/>
+      <c r="KQ28" s="0"/>
+      <c r="KR28" s="0"/>
+      <c r="KS28" s="0"/>
+      <c r="KT28" s="0"/>
+      <c r="KU28" s="0"/>
+      <c r="KV28" s="0"/>
+      <c r="KW28" s="0"/>
+      <c r="KX28" s="0"/>
+      <c r="KY28" s="0"/>
+      <c r="KZ28" s="0"/>
+      <c r="LA28" s="0"/>
+      <c r="LB28" s="0"/>
+      <c r="LC28" s="0"/>
+      <c r="LD28" s="0"/>
+      <c r="LE28" s="0"/>
+      <c r="LF28" s="0"/>
+      <c r="LG28" s="0"/>
+      <c r="LH28" s="0"/>
+      <c r="LI28" s="0"/>
+      <c r="LJ28" s="0"/>
+      <c r="LK28" s="0"/>
+      <c r="LL28" s="0"/>
+      <c r="LM28" s="0"/>
+      <c r="LN28" s="0"/>
+      <c r="LO28" s="0"/>
+      <c r="LP28" s="0"/>
+      <c r="LQ28" s="0"/>
+      <c r="LR28" s="0"/>
+      <c r="LS28" s="0"/>
+      <c r="LT28" s="0"/>
+      <c r="LU28" s="0"/>
+      <c r="LV28" s="0"/>
+      <c r="LW28" s="0"/>
+      <c r="LX28" s="0"/>
+      <c r="LY28" s="0"/>
+      <c r="LZ28" s="0"/>
+      <c r="MA28" s="0"/>
+      <c r="MB28" s="0"/>
+      <c r="MC28" s="0"/>
+      <c r="MD28" s="0"/>
+      <c r="ME28" s="0"/>
+      <c r="MF28" s="0"/>
+      <c r="MG28" s="0"/>
+      <c r="MH28" s="0"/>
+      <c r="MI28" s="0"/>
+      <c r="MJ28" s="0"/>
+      <c r="MK28" s="0"/>
+      <c r="ML28" s="0"/>
+      <c r="MM28" s="0"/>
+      <c r="MN28" s="0"/>
+      <c r="MO28" s="0"/>
+      <c r="MP28" s="0"/>
+      <c r="MQ28" s="0"/>
+      <c r="MR28" s="0"/>
+      <c r="MS28" s="0"/>
+      <c r="MT28" s="0"/>
+      <c r="MU28" s="0"/>
+      <c r="MV28" s="0"/>
+      <c r="MW28" s="0"/>
+      <c r="MX28" s="0"/>
+      <c r="MY28" s="0"/>
+      <c r="MZ28" s="0"/>
+      <c r="NA28" s="0"/>
+      <c r="NB28" s="0"/>
+      <c r="NC28" s="0"/>
+      <c r="ND28" s="0"/>
+      <c r="NE28" s="0"/>
+      <c r="NF28" s="0"/>
+      <c r="NG28" s="0"/>
+      <c r="NH28" s="0"/>
+      <c r="NI28" s="0"/>
+      <c r="NJ28" s="0"/>
+      <c r="NK28" s="0"/>
+      <c r="NL28" s="0"/>
+      <c r="NM28" s="0"/>
+      <c r="NN28" s="0"/>
+      <c r="NO28" s="0"/>
+      <c r="NP28" s="0"/>
+      <c r="NQ28" s="0"/>
+      <c r="NR28" s="0"/>
+      <c r="NS28" s="0"/>
+      <c r="NT28" s="0"/>
+      <c r="NU28" s="0"/>
+      <c r="NV28" s="0"/>
+      <c r="NW28" s="0"/>
+      <c r="NX28" s="0"/>
+      <c r="NY28" s="0"/>
+      <c r="NZ28" s="0"/>
+      <c r="OA28" s="0"/>
+      <c r="OB28" s="0"/>
+      <c r="OC28" s="0"/>
+      <c r="OD28" s="0"/>
+      <c r="OE28" s="0"/>
+      <c r="OF28" s="0"/>
+      <c r="OG28" s="0"/>
+      <c r="OH28" s="0"/>
+      <c r="OI28" s="0"/>
+      <c r="OJ28" s="0"/>
+      <c r="OK28" s="0"/>
+      <c r="OL28" s="0"/>
+      <c r="OM28" s="0"/>
+      <c r="ON28" s="0"/>
+      <c r="OO28" s="0"/>
+      <c r="OP28" s="0"/>
+      <c r="OQ28" s="0"/>
+      <c r="OR28" s="0"/>
+      <c r="OS28" s="0"/>
+      <c r="OT28" s="0"/>
+      <c r="OU28" s="0"/>
+      <c r="OV28" s="0"/>
+      <c r="OW28" s="0"/>
+      <c r="OX28" s="0"/>
+      <c r="OY28" s="0"/>
+      <c r="OZ28" s="0"/>
+      <c r="PA28" s="0"/>
+      <c r="PB28" s="0"/>
+      <c r="PC28" s="0"/>
+      <c r="PD28" s="0"/>
+      <c r="PE28" s="0"/>
+      <c r="PF28" s="0"/>
+      <c r="PG28" s="0"/>
+      <c r="PH28" s="0"/>
+      <c r="PI28" s="0"/>
+      <c r="PJ28" s="0"/>
+      <c r="PK28" s="0"/>
+      <c r="PL28" s="0"/>
+      <c r="PM28" s="0"/>
+      <c r="PN28" s="0"/>
+      <c r="PO28" s="0"/>
+      <c r="PP28" s="0"/>
+      <c r="PQ28" s="0"/>
+      <c r="PR28" s="0"/>
+      <c r="PS28" s="0"/>
+      <c r="PT28" s="0"/>
+      <c r="PU28" s="0"/>
+      <c r="PV28" s="0"/>
+      <c r="PW28" s="0"/>
+      <c r="PX28" s="0"/>
+      <c r="PY28" s="0"/>
+      <c r="PZ28" s="0"/>
+      <c r="QA28" s="0"/>
+      <c r="QB28" s="0"/>
+      <c r="QC28" s="0"/>
+      <c r="QD28" s="0"/>
+      <c r="QE28" s="0"/>
+      <c r="QF28" s="0"/>
+      <c r="QG28" s="0"/>
+      <c r="QH28" s="0"/>
+      <c r="QI28" s="0"/>
+      <c r="QJ28" s="0"/>
+      <c r="QK28" s="0"/>
+      <c r="QL28" s="0"/>
+      <c r="QM28" s="0"/>
+      <c r="QN28" s="0"/>
+      <c r="QO28" s="0"/>
+      <c r="QP28" s="0"/>
+      <c r="QQ28" s="0"/>
+      <c r="QR28" s="0"/>
+      <c r="QS28" s="0"/>
+      <c r="QT28" s="0"/>
+      <c r="QU28" s="0"/>
+      <c r="QV28" s="0"/>
+      <c r="QW28" s="0"/>
+      <c r="QX28" s="0"/>
+      <c r="QY28" s="0"/>
+      <c r="QZ28" s="0"/>
+      <c r="RA28" s="0"/>
+      <c r="RB28" s="0"/>
+      <c r="RC28" s="0"/>
+      <c r="RD28" s="0"/>
+      <c r="RE28" s="0"/>
+      <c r="RF28" s="0"/>
+      <c r="RG28" s="0"/>
+      <c r="RH28" s="0"/>
+      <c r="RI28" s="0"/>
+      <c r="RJ28" s="0"/>
+      <c r="RK28" s="0"/>
+      <c r="RL28" s="0"/>
+      <c r="RM28" s="0"/>
+      <c r="RN28" s="0"/>
+      <c r="RO28" s="0"/>
+      <c r="RP28" s="0"/>
+      <c r="RQ28" s="0"/>
+      <c r="RR28" s="0"/>
+      <c r="RS28" s="0"/>
+      <c r="RT28" s="0"/>
+      <c r="RU28" s="0"/>
+      <c r="RV28" s="0"/>
+      <c r="RW28" s="0"/>
+      <c r="RX28" s="0"/>
+      <c r="RY28" s="0"/>
+      <c r="RZ28" s="0"/>
+      <c r="SA28" s="0"/>
+      <c r="SB28" s="0"/>
+      <c r="SC28" s="0"/>
+      <c r="SD28" s="0"/>
+      <c r="SE28" s="0"/>
+      <c r="SF28" s="0"/>
+      <c r="SG28" s="0"/>
+      <c r="SH28" s="0"/>
+      <c r="SI28" s="0"/>
+      <c r="SJ28" s="0"/>
+      <c r="SK28" s="0"/>
+      <c r="SL28" s="0"/>
+      <c r="SM28" s="0"/>
+      <c r="SN28" s="0"/>
+      <c r="SO28" s="0"/>
+      <c r="SP28" s="0"/>
+      <c r="SQ28" s="0"/>
+      <c r="SR28" s="0"/>
+      <c r="SS28" s="0"/>
+      <c r="ST28" s="0"/>
+      <c r="SU28" s="0"/>
+      <c r="SV28" s="0"/>
+      <c r="SW28" s="0"/>
+      <c r="SX28" s="0"/>
+      <c r="SY28" s="0"/>
+      <c r="SZ28" s="0"/>
+      <c r="TA28" s="0"/>
+      <c r="TB28" s="0"/>
+      <c r="TC28" s="0"/>
+      <c r="TD28" s="0"/>
+      <c r="TE28" s="0"/>
+      <c r="TF28" s="0"/>
+      <c r="TG28" s="0"/>
+      <c r="TH28" s="0"/>
+      <c r="TI28" s="0"/>
+      <c r="TJ28" s="0"/>
+      <c r="TK28" s="0"/>
+      <c r="TL28" s="0"/>
+      <c r="TM28" s="0"/>
+      <c r="TN28" s="0"/>
+      <c r="TO28" s="0"/>
+      <c r="TP28" s="0"/>
+      <c r="TQ28" s="0"/>
+      <c r="TR28" s="0"/>
+      <c r="TS28" s="0"/>
+      <c r="TT28" s="0"/>
+      <c r="TU28" s="0"/>
+      <c r="TV28" s="0"/>
+      <c r="TW28" s="0"/>
+      <c r="TX28" s="0"/>
+      <c r="TY28" s="0"/>
+      <c r="TZ28" s="0"/>
+      <c r="UA28" s="0"/>
+      <c r="UB28" s="0"/>
+      <c r="UC28" s="0"/>
+      <c r="UD28" s="0"/>
+      <c r="UE28" s="0"/>
+      <c r="UF28" s="0"/>
+      <c r="UG28" s="0"/>
+      <c r="UH28" s="0"/>
+      <c r="UI28" s="0"/>
+      <c r="UJ28" s="0"/>
+      <c r="UK28" s="0"/>
+      <c r="UL28" s="0"/>
+      <c r="UM28" s="0"/>
+      <c r="UN28" s="0"/>
+      <c r="UO28" s="0"/>
+      <c r="UP28" s="0"/>
+      <c r="UQ28" s="0"/>
+      <c r="UR28" s="0"/>
+      <c r="US28" s="0"/>
+      <c r="UT28" s="0"/>
+      <c r="UU28" s="0"/>
+      <c r="UV28" s="0"/>
+      <c r="UW28" s="0"/>
+      <c r="UX28" s="0"/>
+      <c r="UY28" s="0"/>
+      <c r="UZ28" s="0"/>
+      <c r="VA28" s="0"/>
+      <c r="VB28" s="0"/>
+      <c r="VC28" s="0"/>
+      <c r="VD28" s="0"/>
+      <c r="VE28" s="0"/>
+      <c r="VF28" s="0"/>
+      <c r="VG28" s="0"/>
+      <c r="VH28" s="0"/>
+      <c r="VI28" s="0"/>
+      <c r="VJ28" s="0"/>
+      <c r="VK28" s="0"/>
+      <c r="VL28" s="0"/>
+      <c r="VM28" s="0"/>
+      <c r="VN28" s="0"/>
+      <c r="VO28" s="0"/>
+      <c r="VP28" s="0"/>
+      <c r="VQ28" s="0"/>
+      <c r="VR28" s="0"/>
+      <c r="VS28" s="0"/>
+      <c r="VT28" s="0"/>
+      <c r="VU28" s="0"/>
+      <c r="VV28" s="0"/>
+      <c r="VW28" s="0"/>
+      <c r="VX28" s="0"/>
+      <c r="VY28" s="0"/>
+      <c r="VZ28" s="0"/>
+      <c r="WA28" s="0"/>
+      <c r="WB28" s="0"/>
+      <c r="WC28" s="0"/>
+      <c r="WD28" s="0"/>
+      <c r="WE28" s="0"/>
+      <c r="WF28" s="0"/>
+      <c r="WG28" s="0"/>
+      <c r="WH28" s="0"/>
+      <c r="WI28" s="0"/>
+      <c r="WJ28" s="0"/>
+      <c r="WK28" s="0"/>
+      <c r="WL28" s="0"/>
+      <c r="WM28" s="0"/>
+      <c r="WN28" s="0"/>
+      <c r="WO28" s="0"/>
+      <c r="WP28" s="0"/>
+      <c r="WQ28" s="0"/>
+      <c r="WR28" s="0"/>
+      <c r="WS28" s="0"/>
+      <c r="WT28" s="0"/>
+      <c r="WU28" s="0"/>
+      <c r="WV28" s="0"/>
+      <c r="WW28" s="0"/>
+      <c r="WX28" s="0"/>
+      <c r="WY28" s="0"/>
+      <c r="WZ28" s="0"/>
+      <c r="XA28" s="0"/>
+      <c r="XB28" s="0"/>
+      <c r="XC28" s="0"/>
+      <c r="XD28" s="0"/>
+      <c r="XE28" s="0"/>
+      <c r="XF28" s="0"/>
+      <c r="XG28" s="0"/>
+      <c r="XH28" s="0"/>
+      <c r="XI28" s="0"/>
+      <c r="XJ28" s="0"/>
+      <c r="XK28" s="0"/>
+      <c r="XL28" s="0"/>
+      <c r="XM28" s="0"/>
+      <c r="XN28" s="0"/>
+      <c r="XO28" s="0"/>
+      <c r="XP28" s="0"/>
+      <c r="XQ28" s="0"/>
+      <c r="XR28" s="0"/>
+      <c r="XS28" s="0"/>
+      <c r="XT28" s="0"/>
+      <c r="XU28" s="0"/>
+      <c r="XV28" s="0"/>
+      <c r="XW28" s="0"/>
+      <c r="XX28" s="0"/>
+      <c r="XY28" s="0"/>
+      <c r="XZ28" s="0"/>
+      <c r="YA28" s="0"/>
+      <c r="YB28" s="0"/>
+      <c r="YC28" s="0"/>
+      <c r="YD28" s="0"/>
+      <c r="YE28" s="0"/>
+      <c r="YF28" s="0"/>
+      <c r="YG28" s="0"/>
+      <c r="YH28" s="0"/>
+      <c r="YI28" s="0"/>
+      <c r="YJ28" s="0"/>
+      <c r="YK28" s="0"/>
+      <c r="YL28" s="0"/>
+      <c r="YM28" s="0"/>
+      <c r="YN28" s="0"/>
+      <c r="YO28" s="0"/>
+      <c r="YP28" s="0"/>
+      <c r="YQ28" s="0"/>
+      <c r="YR28" s="0"/>
+      <c r="YS28" s="0"/>
+      <c r="YT28" s="0"/>
+      <c r="YU28" s="0"/>
+      <c r="YV28" s="0"/>
+      <c r="YW28" s="0"/>
+      <c r="YX28" s="0"/>
+      <c r="YY28" s="0"/>
+      <c r="YZ28" s="0"/>
+      <c r="ZA28" s="0"/>
+      <c r="ZB28" s="0"/>
+      <c r="ZC28" s="0"/>
+      <c r="ZD28" s="0"/>
+      <c r="ZE28" s="0"/>
+      <c r="ZF28" s="0"/>
+      <c r="ZG28" s="0"/>
+      <c r="ZH28" s="0"/>
+      <c r="ZI28" s="0"/>
+      <c r="ZJ28" s="0"/>
+      <c r="ZK28" s="0"/>
+      <c r="ZL28" s="0"/>
+      <c r="ZM28" s="0"/>
+      <c r="ZN28" s="0"/>
+      <c r="ZO28" s="0"/>
+      <c r="ZP28" s="0"/>
+      <c r="ZQ28" s="0"/>
+      <c r="ZR28" s="0"/>
+      <c r="ZS28" s="0"/>
+      <c r="ZT28" s="0"/>
+      <c r="ZU28" s="0"/>
+      <c r="ZV28" s="0"/>
+      <c r="ZW28" s="0"/>
+      <c r="ZX28" s="0"/>
+      <c r="ZY28" s="0"/>
+      <c r="ZZ28" s="0"/>
+      <c r="AAA28" s="0"/>
+      <c r="AAB28" s="0"/>
+      <c r="AAC28" s="0"/>
+      <c r="AAD28" s="0"/>
+      <c r="AAE28" s="0"/>
+      <c r="AAF28" s="0"/>
+      <c r="AAG28" s="0"/>
+      <c r="AAH28" s="0"/>
+      <c r="AAI28" s="0"/>
+      <c r="AAJ28" s="0"/>
+      <c r="AAK28" s="0"/>
+      <c r="AAL28" s="0"/>
+      <c r="AAM28" s="0"/>
+      <c r="AAN28" s="0"/>
+      <c r="AAO28" s="0"/>
+      <c r="AAP28" s="0"/>
+      <c r="AAQ28" s="0"/>
+      <c r="AAR28" s="0"/>
+      <c r="AAS28" s="0"/>
+      <c r="AAT28" s="0"/>
+      <c r="AAU28" s="0"/>
+      <c r="AAV28" s="0"/>
+      <c r="AAW28" s="0"/>
+      <c r="AAX28" s="0"/>
+      <c r="AAY28" s="0"/>
+      <c r="AAZ28" s="0"/>
+      <c r="ABA28" s="0"/>
+      <c r="ABB28" s="0"/>
+      <c r="ABC28" s="0"/>
+      <c r="ABD28" s="0"/>
+      <c r="ABE28" s="0"/>
+      <c r="ABF28" s="0"/>
+      <c r="ABG28" s="0"/>
+      <c r="ABH28" s="0"/>
+      <c r="ABI28" s="0"/>
+      <c r="ABJ28" s="0"/>
+      <c r="ABK28" s="0"/>
+      <c r="ABL28" s="0"/>
+      <c r="ABM28" s="0"/>
+      <c r="ABN28" s="0"/>
+      <c r="ABO28" s="0"/>
+      <c r="ABP28" s="0"/>
+      <c r="ABQ28" s="0"/>
+      <c r="ABR28" s="0"/>
+      <c r="ABS28" s="0"/>
+      <c r="ABT28" s="0"/>
+      <c r="ABU28" s="0"/>
+      <c r="ABV28" s="0"/>
+      <c r="ABW28" s="0"/>
+      <c r="ABX28" s="0"/>
+      <c r="ABY28" s="0"/>
+      <c r="ABZ28" s="0"/>
+      <c r="ACA28" s="0"/>
+      <c r="ACB28" s="0"/>
+      <c r="ACC28" s="0"/>
+      <c r="ACD28" s="0"/>
+      <c r="ACE28" s="0"/>
+      <c r="ACF28" s="0"/>
+      <c r="ACG28" s="0"/>
+      <c r="ACH28" s="0"/>
+      <c r="ACI28" s="0"/>
+      <c r="ACJ28" s="0"/>
+      <c r="ACK28" s="0"/>
+      <c r="ACL28" s="0"/>
+      <c r="ACM28" s="0"/>
+      <c r="ACN28" s="0"/>
+      <c r="ACO28" s="0"/>
+      <c r="ACP28" s="0"/>
+      <c r="ACQ28" s="0"/>
+      <c r="ACR28" s="0"/>
+      <c r="ACS28" s="0"/>
+      <c r="ACT28" s="0"/>
+      <c r="ACU28" s="0"/>
+      <c r="ACV28" s="0"/>
+      <c r="ACW28" s="0"/>
+      <c r="ACX28" s="0"/>
+      <c r="ACY28" s="0"/>
+      <c r="ACZ28" s="0"/>
+      <c r="ADA28" s="0"/>
+      <c r="ADB28" s="0"/>
+      <c r="ADC28" s="0"/>
+      <c r="ADD28" s="0"/>
+      <c r="ADE28" s="0"/>
+      <c r="ADF28" s="0"/>
+      <c r="ADG28" s="0"/>
+      <c r="ADH28" s="0"/>
+      <c r="ADI28" s="0"/>
+      <c r="ADJ28" s="0"/>
+      <c r="ADK28" s="0"/>
+      <c r="ADL28" s="0"/>
+      <c r="ADM28" s="0"/>
+      <c r="ADN28" s="0"/>
+      <c r="ADO28" s="0"/>
+      <c r="ADP28" s="0"/>
+      <c r="ADQ28" s="0"/>
+      <c r="ADR28" s="0"/>
+      <c r="ADS28" s="0"/>
+      <c r="ADT28" s="0"/>
+      <c r="ADU28" s="0"/>
+      <c r="ADV28" s="0"/>
+      <c r="ADW28" s="0"/>
+      <c r="ADX28" s="0"/>
+      <c r="ADY28" s="0"/>
+      <c r="ADZ28" s="0"/>
+      <c r="AEA28" s="0"/>
+      <c r="AEB28" s="0"/>
+      <c r="AEC28" s="0"/>
+      <c r="AED28" s="0"/>
+      <c r="AEE28" s="0"/>
+      <c r="AEF28" s="0"/>
+      <c r="AEG28" s="0"/>
+      <c r="AEH28" s="0"/>
+      <c r="AEI28" s="0"/>
+      <c r="AEJ28" s="0"/>
+      <c r="AEK28" s="0"/>
+      <c r="AEL28" s="0"/>
+      <c r="AEM28" s="0"/>
+      <c r="AEN28" s="0"/>
+      <c r="AEO28" s="0"/>
+      <c r="AEP28" s="0"/>
+      <c r="AEQ28" s="0"/>
+      <c r="AER28" s="0"/>
+      <c r="AES28" s="0"/>
+      <c r="AET28" s="0"/>
+      <c r="AEU28" s="0"/>
+      <c r="AEV28" s="0"/>
+      <c r="AEW28" s="0"/>
+      <c r="AEX28" s="0"/>
+      <c r="AEY28" s="0"/>
+      <c r="AEZ28" s="0"/>
+      <c r="AFA28" s="0"/>
+      <c r="AFB28" s="0"/>
+      <c r="AFC28" s="0"/>
+      <c r="AFD28" s="0"/>
+      <c r="AFE28" s="0"/>
+      <c r="AFF28" s="0"/>
+      <c r="AFG28" s="0"/>
+      <c r="AFH28" s="0"/>
+      <c r="AFI28" s="0"/>
+      <c r="AFJ28" s="0"/>
+      <c r="AFK28" s="0"/>
+      <c r="AFL28" s="0"/>
+      <c r="AFM28" s="0"/>
+      <c r="AFN28" s="0"/>
+      <c r="AFO28" s="0"/>
+      <c r="AFP28" s="0"/>
+      <c r="AFQ28" s="0"/>
+      <c r="AFR28" s="0"/>
+      <c r="AFS28" s="0"/>
+      <c r="AFT28" s="0"/>
+      <c r="AFU28" s="0"/>
+      <c r="AFV28" s="0"/>
+      <c r="AFW28" s="0"/>
+      <c r="AFX28" s="0"/>
+      <c r="AFY28" s="0"/>
+      <c r="AFZ28" s="0"/>
+      <c r="AGA28" s="0"/>
+      <c r="AGB28" s="0"/>
+      <c r="AGC28" s="0"/>
+      <c r="AGD28" s="0"/>
+      <c r="AGE28" s="0"/>
+      <c r="AGF28" s="0"/>
+      <c r="AGG28" s="0"/>
+      <c r="AGH28" s="0"/>
+      <c r="AGI28" s="0"/>
+      <c r="AGJ28" s="0"/>
+      <c r="AGK28" s="0"/>
+      <c r="AGL28" s="0"/>
+      <c r="AGM28" s="0"/>
+      <c r="AGN28" s="0"/>
+      <c r="AGO28" s="0"/>
+      <c r="AGP28" s="0"/>
+      <c r="AGQ28" s="0"/>
+      <c r="AGR28" s="0"/>
+      <c r="AGS28" s="0"/>
+      <c r="AGT28" s="0"/>
+      <c r="AGU28" s="0"/>
+      <c r="AGV28" s="0"/>
+      <c r="AGW28" s="0"/>
+      <c r="AGX28" s="0"/>
+      <c r="AGY28" s="0"/>
+      <c r="AGZ28" s="0"/>
+      <c r="AHA28" s="0"/>
+      <c r="AHB28" s="0"/>
+      <c r="AHC28" s="0"/>
+      <c r="AHD28" s="0"/>
+      <c r="AHE28" s="0"/>
+      <c r="AHF28" s="0"/>
+      <c r="AHG28" s="0"/>
+      <c r="AHH28" s="0"/>
+      <c r="AHI28" s="0"/>
+      <c r="AHJ28" s="0"/>
+      <c r="AHK28" s="0"/>
+      <c r="AHL28" s="0"/>
+      <c r="AHM28" s="0"/>
+      <c r="AHN28" s="0"/>
+      <c r="AHO28" s="0"/>
+      <c r="AHP28" s="0"/>
+      <c r="AHQ28" s="0"/>
+      <c r="AHR28" s="0"/>
+      <c r="AHS28" s="0"/>
+      <c r="AHT28" s="0"/>
+      <c r="AHU28" s="0"/>
+      <c r="AHV28" s="0"/>
+      <c r="AHW28" s="0"/>
+      <c r="AHX28" s="0"/>
+      <c r="AHY28" s="0"/>
+      <c r="AHZ28" s="0"/>
+      <c r="AIA28" s="0"/>
+      <c r="AIB28" s="0"/>
+      <c r="AIC28" s="0"/>
+      <c r="AID28" s="0"/>
+      <c r="AIE28" s="0"/>
+      <c r="AIF28" s="0"/>
+      <c r="AIG28" s="0"/>
+      <c r="AIH28" s="0"/>
+      <c r="AII28" s="0"/>
+      <c r="AIJ28" s="0"/>
+      <c r="AIK28" s="0"/>
+      <c r="AIL28" s="0"/>
+      <c r="AIM28" s="0"/>
+      <c r="AIN28" s="0"/>
+      <c r="AIO28" s="0"/>
+      <c r="AIP28" s="0"/>
+      <c r="AIQ28" s="0"/>
+      <c r="AIR28" s="0"/>
+      <c r="AIS28" s="0"/>
+      <c r="AIT28" s="0"/>
+      <c r="AIU28" s="0"/>
+      <c r="AIV28" s="0"/>
+      <c r="AIW28" s="0"/>
+      <c r="AIX28" s="0"/>
+      <c r="AIY28" s="0"/>
+      <c r="AIZ28" s="0"/>
+      <c r="AJA28" s="0"/>
+      <c r="AJB28" s="0"/>
+      <c r="AJC28" s="0"/>
+      <c r="AJD28" s="0"/>
+      <c r="AJE28" s="0"/>
+      <c r="AJF28" s="0"/>
+      <c r="AJG28" s="0"/>
+      <c r="AJH28" s="0"/>
+      <c r="AJI28" s="0"/>
+      <c r="AJJ28" s="0"/>
+      <c r="AJK28" s="0"/>
+      <c r="AJL28" s="0"/>
+      <c r="AJM28" s="0"/>
+      <c r="AJN28" s="0"/>
+      <c r="AJO28" s="0"/>
+      <c r="AJP28" s="0"/>
+      <c r="AJQ28" s="0"/>
+      <c r="AJR28" s="0"/>
+      <c r="AJS28" s="0"/>
+      <c r="AJT28" s="0"/>
+      <c r="AJU28" s="0"/>
+      <c r="AJV28" s="0"/>
+      <c r="AJW28" s="0"/>
+      <c r="AJX28" s="0"/>
+      <c r="AJY28" s="0"/>
+      <c r="AJZ28" s="0"/>
+      <c r="AKA28" s="0"/>
+      <c r="AKB28" s="0"/>
+      <c r="AKC28" s="0"/>
+      <c r="AKD28" s="0"/>
+      <c r="AKE28" s="0"/>
+      <c r="AKF28" s="0"/>
+      <c r="AKG28" s="0"/>
+      <c r="AKH28" s="0"/>
+      <c r="AKI28" s="0"/>
+      <c r="AKJ28" s="0"/>
+      <c r="AKK28" s="0"/>
+      <c r="AKL28" s="0"/>
+      <c r="AKM28" s="0"/>
+      <c r="AKN28" s="0"/>
+      <c r="AKO28" s="0"/>
+      <c r="AKP28" s="0"/>
+      <c r="AKQ28" s="0"/>
+      <c r="AKR28" s="0"/>
+      <c r="AKS28" s="0"/>
+      <c r="AKT28" s="0"/>
+      <c r="AKU28" s="0"/>
+      <c r="AKV28" s="0"/>
+      <c r="AKW28" s="0"/>
+      <c r="AKX28" s="0"/>
+      <c r="AKY28" s="0"/>
+      <c r="AKZ28" s="0"/>
+      <c r="ALA28" s="0"/>
+      <c r="ALB28" s="0"/>
+      <c r="ALC28" s="0"/>
+      <c r="ALD28" s="0"/>
+      <c r="ALE28" s="0"/>
+      <c r="ALF28" s="0"/>
+      <c r="ALG28" s="0"/>
+      <c r="ALH28" s="0"/>
+      <c r="ALI28" s="0"/>
+      <c r="ALJ28" s="0"/>
+      <c r="ALK28" s="0"/>
+      <c r="ALL28" s="0"/>
+      <c r="ALM28" s="0"/>
+      <c r="ALN28" s="0"/>
+      <c r="ALO28" s="0"/>
+      <c r="ALP28" s="0"/>
+      <c r="ALQ28" s="0"/>
+      <c r="ALR28" s="0"/>
+      <c r="ALS28" s="0"/>
+      <c r="ALT28" s="0"/>
+      <c r="ALU28" s="0"/>
+      <c r="ALV28" s="0"/>
+      <c r="ALW28" s="0"/>
+      <c r="ALX28" s="0"/>
+      <c r="ALY28" s="0"/>
+      <c r="ALZ28" s="0"/>
+      <c r="AMA28" s="0"/>
+      <c r="AMB28" s="0"/>
+      <c r="AMC28" s="0"/>
+      <c r="AMD28" s="0"/>
+      <c r="AME28" s="0"/>
+      <c r="AMF28" s="0"/>
+      <c r="AMG28" s="0"/>
+      <c r="AMH28" s="0"/>
+      <c r="AMI28" s="0"/>
+      <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="35.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="D31" s="0"/>
+      <c r="E31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="31" customFormat="false" ht="35.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="1" t="s">
+    <row r="32" customFormat="false" ht="57.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="E32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="0"/>
-      <c r="E32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="E33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="57.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="1" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="E38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
-      <c r="D38" s="0"/>
-      <c r="E38" s="0"/>
-      <c r="F38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2025,9 +3048,9 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:H35"/>
+  <autoFilter ref="A1:H34"/>
   <mergeCells count="2">
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
@@ -2037,6 +3060,12 @@
       <formula></formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="F33" r:id="rId1" display="https://www.anthedesign.fr/referencement/seo-comment-optimiser-le-referencement-des-images/"/>
+    <hyperlink ref="F34" r:id="rId2" display="https://www.anthedesign.fr/referencement/seo-comment-optimiser-le-referencement-des-images/"/>
+    <hyperlink ref="F35" r:id="rId3" display="https://www.anthedesign.fr/referencement/seo-comment-optimiser-le-referencement-des-images/"/>
+    <hyperlink ref="F38" r:id="rId4" display="https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2044,6 +3073,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout de balise canonical
</commit_message>
<xml_diff>
--- a/Maquette-Sources/Modèle-audit-SEO.xlsx
+++ b/Maquette-Sources/Modèle-audit-SEO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -142,6 +142,33 @@
     <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Element/Heading_Elements</t>
   </si>
   <si>
+    <t xml:space="preserve">SEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">problème de structure de contenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les mots clés doivents y être présent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modification des titres pour y ajouter des mots clés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le titre col-sm-12 h2 est trop long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un titre doit résumer en 5 à 8 mots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifier le h2 en un h2 + paragraphe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.referenseo.com/guide-seo/balises-h1-h2-h3/#:~:text=Contrairement%20au%20titre%20h1%2C%20les,clés%20secondaires%20de%20votre%20page.</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO + Bonne pratique SASS</t>
   </si>
   <si>
@@ -157,9 +184,6 @@
     <t xml:space="preserve">https://www.ornitorinc.com/blog/referencement/10-bonnes-pratiques-referencement-seo/</t>
   </si>
   <si>
-    <t xml:space="preserve">SEO</t>
-  </si>
-  <si>
     <t xml:space="preserve">title de la page index ‘.’</t>
   </si>
   <si>
@@ -227,9 +251,6 @@
   </si>
   <si>
     <t xml:space="preserve">la balise description est utilisée par les moteurs de recherche pour l’indexation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages</t>
   </si>
   <si>
     <t xml:space="preserve">image 1à4</t>
@@ -305,7 +326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -363,12 +384,6 @@
       <name val="Symbol"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -434,7 +449,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -463,19 +478,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -581,12 +592,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="E10" activeCellId="0" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -674,7 +685,7 @@
       <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -688,7 +699,7 @@
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -699,10 +710,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -711,7 +722,7 @@
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -725,8 +736,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="E6" s="5"/>
       <c r="F6" s="1" t="s">
         <v>28</v>
@@ -757,7 +768,7 @@
         <v>33</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -779,11 +790,45 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E10" s="5"/>
+    <row r="10" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E11" s="5"/>
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E12" s="5"/>
@@ -806,1284 +851,259 @@
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="133.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="58.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" s="11" customFormat="true" ht="116.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
-      <c r="B28" s="0"/>
-      <c r="C28" s="0"/>
-      <c r="D28" s="0"/>
-      <c r="E28" s="0"/>
-      <c r="F28" s="0"/>
-      <c r="G28" s="0"/>
-      <c r="H28" s="0"/>
-      <c r="I28" s="0"/>
-      <c r="J28" s="0"/>
-      <c r="K28" s="0"/>
-      <c r="L28" s="0"/>
-      <c r="M28" s="0"/>
-      <c r="N28" s="0"/>
-      <c r="O28" s="0"/>
-      <c r="P28" s="0"/>
-      <c r="Q28" s="0"/>
-      <c r="R28" s="0"/>
-      <c r="S28" s="0"/>
-      <c r="T28" s="0"/>
-      <c r="U28" s="0"/>
-      <c r="V28" s="0"/>
-      <c r="W28" s="0"/>
-      <c r="X28" s="0"/>
-      <c r="Y28" s="0"/>
-      <c r="Z28" s="0"/>
-      <c r="AA28" s="0"/>
-      <c r="AB28" s="0"/>
-      <c r="AC28" s="0"/>
-      <c r="AD28" s="0"/>
-      <c r="AE28" s="0"/>
-      <c r="AF28" s="0"/>
-      <c r="AG28" s="0"/>
-      <c r="AH28" s="0"/>
-      <c r="AI28" s="0"/>
-      <c r="AJ28" s="0"/>
-      <c r="AK28" s="0"/>
-      <c r="AL28" s="0"/>
-      <c r="AM28" s="0"/>
-      <c r="AN28" s="0"/>
-      <c r="AO28" s="0"/>
-      <c r="AP28" s="0"/>
-      <c r="AQ28" s="0"/>
-      <c r="AR28" s="0"/>
-      <c r="AS28" s="0"/>
-      <c r="AT28" s="0"/>
-      <c r="AU28" s="0"/>
-      <c r="AV28" s="0"/>
-      <c r="AW28" s="0"/>
-      <c r="AX28" s="0"/>
-      <c r="AY28" s="0"/>
-      <c r="AZ28" s="0"/>
-      <c r="BA28" s="0"/>
-      <c r="BB28" s="0"/>
-      <c r="BC28" s="0"/>
-      <c r="BD28" s="0"/>
-      <c r="BE28" s="0"/>
-      <c r="BF28" s="0"/>
-      <c r="BG28" s="0"/>
-      <c r="BH28" s="0"/>
-      <c r="BI28" s="0"/>
-      <c r="BJ28" s="0"/>
-      <c r="BK28" s="0"/>
-      <c r="BL28" s="0"/>
-      <c r="BM28" s="0"/>
-      <c r="BN28" s="0"/>
-      <c r="BO28" s="0"/>
-      <c r="BP28" s="0"/>
-      <c r="BQ28" s="0"/>
-      <c r="BR28" s="0"/>
-      <c r="BS28" s="0"/>
-      <c r="BT28" s="0"/>
-      <c r="BU28" s="0"/>
-      <c r="BV28" s="0"/>
-      <c r="BW28" s="0"/>
-      <c r="BX28" s="0"/>
-      <c r="BY28" s="0"/>
-      <c r="BZ28" s="0"/>
-      <c r="CA28" s="0"/>
-      <c r="CB28" s="0"/>
-      <c r="CC28" s="0"/>
-      <c r="CD28" s="0"/>
-      <c r="CE28" s="0"/>
-      <c r="CF28" s="0"/>
-      <c r="CG28" s="0"/>
-      <c r="CH28" s="0"/>
-      <c r="CI28" s="0"/>
-      <c r="CJ28" s="0"/>
-      <c r="CK28" s="0"/>
-      <c r="CL28" s="0"/>
-      <c r="CM28" s="0"/>
-      <c r="CN28" s="0"/>
-      <c r="CO28" s="0"/>
-      <c r="CP28" s="0"/>
-      <c r="CQ28" s="0"/>
-      <c r="CR28" s="0"/>
-      <c r="CS28" s="0"/>
-      <c r="CT28" s="0"/>
-      <c r="CU28" s="0"/>
-      <c r="CV28" s="0"/>
-      <c r="CW28" s="0"/>
-      <c r="CX28" s="0"/>
-      <c r="CY28" s="0"/>
-      <c r="CZ28" s="0"/>
-      <c r="DA28" s="0"/>
-      <c r="DB28" s="0"/>
-      <c r="DC28" s="0"/>
-      <c r="DD28" s="0"/>
-      <c r="DE28" s="0"/>
-      <c r="DF28" s="0"/>
-      <c r="DG28" s="0"/>
-      <c r="DH28" s="0"/>
-      <c r="DI28" s="0"/>
-      <c r="DJ28" s="0"/>
-      <c r="DK28" s="0"/>
-      <c r="DL28" s="0"/>
-      <c r="DM28" s="0"/>
-      <c r="DN28" s="0"/>
-      <c r="DO28" s="0"/>
-      <c r="DP28" s="0"/>
-      <c r="DQ28" s="0"/>
-      <c r="DR28" s="0"/>
-      <c r="DS28" s="0"/>
-      <c r="DT28" s="0"/>
-      <c r="DU28" s="0"/>
-      <c r="DV28" s="0"/>
-      <c r="DW28" s="0"/>
-      <c r="DX28" s="0"/>
-      <c r="DY28" s="0"/>
-      <c r="DZ28" s="0"/>
-      <c r="EA28" s="0"/>
-      <c r="EB28" s="0"/>
-      <c r="EC28" s="0"/>
-      <c r="ED28" s="0"/>
-      <c r="EE28" s="0"/>
-      <c r="EF28" s="0"/>
-      <c r="EG28" s="0"/>
-      <c r="EH28" s="0"/>
-      <c r="EI28" s="0"/>
-      <c r="EJ28" s="0"/>
-      <c r="EK28" s="0"/>
-      <c r="EL28" s="0"/>
-      <c r="EM28" s="0"/>
-      <c r="EN28" s="0"/>
-      <c r="EO28" s="0"/>
-      <c r="EP28" s="0"/>
-      <c r="EQ28" s="0"/>
-      <c r="ER28" s="0"/>
-      <c r="ES28" s="0"/>
-      <c r="ET28" s="0"/>
-      <c r="EU28" s="0"/>
-      <c r="EV28" s="0"/>
-      <c r="EW28" s="0"/>
-      <c r="EX28" s="0"/>
-      <c r="EY28" s="0"/>
-      <c r="EZ28" s="0"/>
-      <c r="FA28" s="0"/>
-      <c r="FB28" s="0"/>
-      <c r="FC28" s="0"/>
-      <c r="FD28" s="0"/>
-      <c r="FE28" s="0"/>
-      <c r="FF28" s="0"/>
-      <c r="FG28" s="0"/>
-      <c r="FH28" s="0"/>
-      <c r="FI28" s="0"/>
-      <c r="FJ28" s="0"/>
-      <c r="FK28" s="0"/>
-      <c r="FL28" s="0"/>
-      <c r="FM28" s="0"/>
-      <c r="FN28" s="0"/>
-      <c r="FO28" s="0"/>
-      <c r="FP28" s="0"/>
-      <c r="FQ28" s="0"/>
-      <c r="FR28" s="0"/>
-      <c r="FS28" s="0"/>
-      <c r="FT28" s="0"/>
-      <c r="FU28" s="0"/>
-      <c r="FV28" s="0"/>
-      <c r="FW28" s="0"/>
-      <c r="FX28" s="0"/>
-      <c r="FY28" s="0"/>
-      <c r="FZ28" s="0"/>
-      <c r="GA28" s="0"/>
-      <c r="GB28" s="0"/>
-      <c r="GC28" s="0"/>
-      <c r="GD28" s="0"/>
-      <c r="GE28" s="0"/>
-      <c r="GF28" s="0"/>
-      <c r="GG28" s="0"/>
-      <c r="GH28" s="0"/>
-      <c r="GI28" s="0"/>
-      <c r="GJ28" s="0"/>
-      <c r="GK28" s="0"/>
-      <c r="GL28" s="0"/>
-      <c r="GM28" s="0"/>
-      <c r="GN28" s="0"/>
-      <c r="GO28" s="0"/>
-      <c r="GP28" s="0"/>
-      <c r="GQ28" s="0"/>
-      <c r="GR28" s="0"/>
-      <c r="GS28" s="0"/>
-      <c r="GT28" s="0"/>
-      <c r="GU28" s="0"/>
-      <c r="GV28" s="0"/>
-      <c r="GW28" s="0"/>
-      <c r="GX28" s="0"/>
-      <c r="GY28" s="0"/>
-      <c r="GZ28" s="0"/>
-      <c r="HA28" s="0"/>
-      <c r="HB28" s="0"/>
-      <c r="HC28" s="0"/>
-      <c r="HD28" s="0"/>
-      <c r="HE28" s="0"/>
-      <c r="HF28" s="0"/>
-      <c r="HG28" s="0"/>
-      <c r="HH28" s="0"/>
-      <c r="HI28" s="0"/>
-      <c r="HJ28" s="0"/>
-      <c r="HK28" s="0"/>
-      <c r="HL28" s="0"/>
-      <c r="HM28" s="0"/>
-      <c r="HN28" s="0"/>
-      <c r="HO28" s="0"/>
-      <c r="HP28" s="0"/>
-      <c r="HQ28" s="0"/>
-      <c r="HR28" s="0"/>
-      <c r="HS28" s="0"/>
-      <c r="HT28" s="0"/>
-      <c r="HU28" s="0"/>
-      <c r="HV28" s="0"/>
-      <c r="HW28" s="0"/>
-      <c r="HX28" s="0"/>
-      <c r="HY28" s="0"/>
-      <c r="HZ28" s="0"/>
-      <c r="IA28" s="0"/>
-      <c r="IB28" s="0"/>
-      <c r="IC28" s="0"/>
-      <c r="ID28" s="0"/>
-      <c r="IE28" s="0"/>
-      <c r="IF28" s="0"/>
-      <c r="IG28" s="0"/>
-      <c r="IH28" s="0"/>
-      <c r="II28" s="0"/>
-      <c r="IJ28" s="0"/>
-      <c r="IK28" s="0"/>
-      <c r="IL28" s="0"/>
-      <c r="IM28" s="0"/>
-      <c r="IN28" s="0"/>
-      <c r="IO28" s="0"/>
-      <c r="IP28" s="0"/>
-      <c r="IQ28" s="0"/>
-      <c r="IR28" s="0"/>
-      <c r="IS28" s="0"/>
-      <c r="IT28" s="0"/>
-      <c r="IU28" s="0"/>
-      <c r="IV28" s="0"/>
-      <c r="IW28" s="0"/>
-      <c r="IX28" s="0"/>
-      <c r="IY28" s="0"/>
-      <c r="IZ28" s="0"/>
-      <c r="JA28" s="0"/>
-      <c r="JB28" s="0"/>
-      <c r="JC28" s="0"/>
-      <c r="JD28" s="0"/>
-      <c r="JE28" s="0"/>
-      <c r="JF28" s="0"/>
-      <c r="JG28" s="0"/>
-      <c r="JH28" s="0"/>
-      <c r="JI28" s="0"/>
-      <c r="JJ28" s="0"/>
-      <c r="JK28" s="0"/>
-      <c r="JL28" s="0"/>
-      <c r="JM28" s="0"/>
-      <c r="JN28" s="0"/>
-      <c r="JO28" s="0"/>
-      <c r="JP28" s="0"/>
-      <c r="JQ28" s="0"/>
-      <c r="JR28" s="0"/>
-      <c r="JS28" s="0"/>
-      <c r="JT28" s="0"/>
-      <c r="JU28" s="0"/>
-      <c r="JV28" s="0"/>
-      <c r="JW28" s="0"/>
-      <c r="JX28" s="0"/>
-      <c r="JY28" s="0"/>
-      <c r="JZ28" s="0"/>
-      <c r="KA28" s="0"/>
-      <c r="KB28" s="0"/>
-      <c r="KC28" s="0"/>
-      <c r="KD28" s="0"/>
-      <c r="KE28" s="0"/>
-      <c r="KF28" s="0"/>
-      <c r="KG28" s="0"/>
-      <c r="KH28" s="0"/>
-      <c r="KI28" s="0"/>
-      <c r="KJ28" s="0"/>
-      <c r="KK28" s="0"/>
-      <c r="KL28" s="0"/>
-      <c r="KM28" s="0"/>
-      <c r="KN28" s="0"/>
-      <c r="KO28" s="0"/>
-      <c r="KP28" s="0"/>
-      <c r="KQ28" s="0"/>
-      <c r="KR28" s="0"/>
-      <c r="KS28" s="0"/>
-      <c r="KT28" s="0"/>
-      <c r="KU28" s="0"/>
-      <c r="KV28" s="0"/>
-      <c r="KW28" s="0"/>
-      <c r="KX28" s="0"/>
-      <c r="KY28" s="0"/>
-      <c r="KZ28" s="0"/>
-      <c r="LA28" s="0"/>
-      <c r="LB28" s="0"/>
-      <c r="LC28" s="0"/>
-      <c r="LD28" s="0"/>
-      <c r="LE28" s="0"/>
-      <c r="LF28" s="0"/>
-      <c r="LG28" s="0"/>
-      <c r="LH28" s="0"/>
-      <c r="LI28" s="0"/>
-      <c r="LJ28" s="0"/>
-      <c r="LK28" s="0"/>
-      <c r="LL28" s="0"/>
-      <c r="LM28" s="0"/>
-      <c r="LN28" s="0"/>
-      <c r="LO28" s="0"/>
-      <c r="LP28" s="0"/>
-      <c r="LQ28" s="0"/>
-      <c r="LR28" s="0"/>
-      <c r="LS28" s="0"/>
-      <c r="LT28" s="0"/>
-      <c r="LU28" s="0"/>
-      <c r="LV28" s="0"/>
-      <c r="LW28" s="0"/>
-      <c r="LX28" s="0"/>
-      <c r="LY28" s="0"/>
-      <c r="LZ28" s="0"/>
-      <c r="MA28" s="0"/>
-      <c r="MB28" s="0"/>
-      <c r="MC28" s="0"/>
-      <c r="MD28" s="0"/>
-      <c r="ME28" s="0"/>
-      <c r="MF28" s="0"/>
-      <c r="MG28" s="0"/>
-      <c r="MH28" s="0"/>
-      <c r="MI28" s="0"/>
-      <c r="MJ28" s="0"/>
-      <c r="MK28" s="0"/>
-      <c r="ML28" s="0"/>
-      <c r="MM28" s="0"/>
-      <c r="MN28" s="0"/>
-      <c r="MO28" s="0"/>
-      <c r="MP28" s="0"/>
-      <c r="MQ28" s="0"/>
-      <c r="MR28" s="0"/>
-      <c r="MS28" s="0"/>
-      <c r="MT28" s="0"/>
-      <c r="MU28" s="0"/>
-      <c r="MV28" s="0"/>
-      <c r="MW28" s="0"/>
-      <c r="MX28" s="0"/>
-      <c r="MY28" s="0"/>
-      <c r="MZ28" s="0"/>
-      <c r="NA28" s="0"/>
-      <c r="NB28" s="0"/>
-      <c r="NC28" s="0"/>
-      <c r="ND28" s="0"/>
-      <c r="NE28" s="0"/>
-      <c r="NF28" s="0"/>
-      <c r="NG28" s="0"/>
-      <c r="NH28" s="0"/>
-      <c r="NI28" s="0"/>
-      <c r="NJ28" s="0"/>
-      <c r="NK28" s="0"/>
-      <c r="NL28" s="0"/>
-      <c r="NM28" s="0"/>
-      <c r="NN28" s="0"/>
-      <c r="NO28" s="0"/>
-      <c r="NP28" s="0"/>
-      <c r="NQ28" s="0"/>
-      <c r="NR28" s="0"/>
-      <c r="NS28" s="0"/>
-      <c r="NT28" s="0"/>
-      <c r="NU28" s="0"/>
-      <c r="NV28" s="0"/>
-      <c r="NW28" s="0"/>
-      <c r="NX28" s="0"/>
-      <c r="NY28" s="0"/>
-      <c r="NZ28" s="0"/>
-      <c r="OA28" s="0"/>
-      <c r="OB28" s="0"/>
-      <c r="OC28" s="0"/>
-      <c r="OD28" s="0"/>
-      <c r="OE28" s="0"/>
-      <c r="OF28" s="0"/>
-      <c r="OG28" s="0"/>
-      <c r="OH28" s="0"/>
-      <c r="OI28" s="0"/>
-      <c r="OJ28" s="0"/>
-      <c r="OK28" s="0"/>
-      <c r="OL28" s="0"/>
-      <c r="OM28" s="0"/>
-      <c r="ON28" s="0"/>
-      <c r="OO28" s="0"/>
-      <c r="OP28" s="0"/>
-      <c r="OQ28" s="0"/>
-      <c r="OR28" s="0"/>
-      <c r="OS28" s="0"/>
-      <c r="OT28" s="0"/>
-      <c r="OU28" s="0"/>
-      <c r="OV28" s="0"/>
-      <c r="OW28" s="0"/>
-      <c r="OX28" s="0"/>
-      <c r="OY28" s="0"/>
-      <c r="OZ28" s="0"/>
-      <c r="PA28" s="0"/>
-      <c r="PB28" s="0"/>
-      <c r="PC28" s="0"/>
-      <c r="PD28" s="0"/>
-      <c r="PE28" s="0"/>
-      <c r="PF28" s="0"/>
-      <c r="PG28" s="0"/>
-      <c r="PH28" s="0"/>
-      <c r="PI28" s="0"/>
-      <c r="PJ28" s="0"/>
-      <c r="PK28" s="0"/>
-      <c r="PL28" s="0"/>
-      <c r="PM28" s="0"/>
-      <c r="PN28" s="0"/>
-      <c r="PO28" s="0"/>
-      <c r="PP28" s="0"/>
-      <c r="PQ28" s="0"/>
-      <c r="PR28" s="0"/>
-      <c r="PS28" s="0"/>
-      <c r="PT28" s="0"/>
-      <c r="PU28" s="0"/>
-      <c r="PV28" s="0"/>
-      <c r="PW28" s="0"/>
-      <c r="PX28" s="0"/>
-      <c r="PY28" s="0"/>
-      <c r="PZ28" s="0"/>
-      <c r="QA28" s="0"/>
-      <c r="QB28" s="0"/>
-      <c r="QC28" s="0"/>
-      <c r="QD28" s="0"/>
-      <c r="QE28" s="0"/>
-      <c r="QF28" s="0"/>
-      <c r="QG28" s="0"/>
-      <c r="QH28" s="0"/>
-      <c r="QI28" s="0"/>
-      <c r="QJ28" s="0"/>
-      <c r="QK28" s="0"/>
-      <c r="QL28" s="0"/>
-      <c r="QM28" s="0"/>
-      <c r="QN28" s="0"/>
-      <c r="QO28" s="0"/>
-      <c r="QP28" s="0"/>
-      <c r="QQ28" s="0"/>
-      <c r="QR28" s="0"/>
-      <c r="QS28" s="0"/>
-      <c r="QT28" s="0"/>
-      <c r="QU28" s="0"/>
-      <c r="QV28" s="0"/>
-      <c r="QW28" s="0"/>
-      <c r="QX28" s="0"/>
-      <c r="QY28" s="0"/>
-      <c r="QZ28" s="0"/>
-      <c r="RA28" s="0"/>
-      <c r="RB28" s="0"/>
-      <c r="RC28" s="0"/>
-      <c r="RD28" s="0"/>
-      <c r="RE28" s="0"/>
-      <c r="RF28" s="0"/>
-      <c r="RG28" s="0"/>
-      <c r="RH28" s="0"/>
-      <c r="RI28" s="0"/>
-      <c r="RJ28" s="0"/>
-      <c r="RK28" s="0"/>
-      <c r="RL28" s="0"/>
-      <c r="RM28" s="0"/>
-      <c r="RN28" s="0"/>
-      <c r="RO28" s="0"/>
-      <c r="RP28" s="0"/>
-      <c r="RQ28" s="0"/>
-      <c r="RR28" s="0"/>
-      <c r="RS28" s="0"/>
-      <c r="RT28" s="0"/>
-      <c r="RU28" s="0"/>
-      <c r="RV28" s="0"/>
-      <c r="RW28" s="0"/>
-      <c r="RX28" s="0"/>
-      <c r="RY28" s="0"/>
-      <c r="RZ28" s="0"/>
-      <c r="SA28" s="0"/>
-      <c r="SB28" s="0"/>
-      <c r="SC28" s="0"/>
-      <c r="SD28" s="0"/>
-      <c r="SE28" s="0"/>
-      <c r="SF28" s="0"/>
-      <c r="SG28" s="0"/>
-      <c r="SH28" s="0"/>
-      <c r="SI28" s="0"/>
-      <c r="SJ28" s="0"/>
-      <c r="SK28" s="0"/>
-      <c r="SL28" s="0"/>
-      <c r="SM28" s="0"/>
-      <c r="SN28" s="0"/>
-      <c r="SO28" s="0"/>
-      <c r="SP28" s="0"/>
-      <c r="SQ28" s="0"/>
-      <c r="SR28" s="0"/>
-      <c r="SS28" s="0"/>
-      <c r="ST28" s="0"/>
-      <c r="SU28" s="0"/>
-      <c r="SV28" s="0"/>
-      <c r="SW28" s="0"/>
-      <c r="SX28" s="0"/>
-      <c r="SY28" s="0"/>
-      <c r="SZ28" s="0"/>
-      <c r="TA28" s="0"/>
-      <c r="TB28" s="0"/>
-      <c r="TC28" s="0"/>
-      <c r="TD28" s="0"/>
-      <c r="TE28" s="0"/>
-      <c r="TF28" s="0"/>
-      <c r="TG28" s="0"/>
-      <c r="TH28" s="0"/>
-      <c r="TI28" s="0"/>
-      <c r="TJ28" s="0"/>
-      <c r="TK28" s="0"/>
-      <c r="TL28" s="0"/>
-      <c r="TM28" s="0"/>
-      <c r="TN28" s="0"/>
-      <c r="TO28" s="0"/>
-      <c r="TP28" s="0"/>
-      <c r="TQ28" s="0"/>
-      <c r="TR28" s="0"/>
-      <c r="TS28" s="0"/>
-      <c r="TT28" s="0"/>
-      <c r="TU28" s="0"/>
-      <c r="TV28" s="0"/>
-      <c r="TW28" s="0"/>
-      <c r="TX28" s="0"/>
-      <c r="TY28" s="0"/>
-      <c r="TZ28" s="0"/>
-      <c r="UA28" s="0"/>
-      <c r="UB28" s="0"/>
-      <c r="UC28" s="0"/>
-      <c r="UD28" s="0"/>
-      <c r="UE28" s="0"/>
-      <c r="UF28" s="0"/>
-      <c r="UG28" s="0"/>
-      <c r="UH28" s="0"/>
-      <c r="UI28" s="0"/>
-      <c r="UJ28" s="0"/>
-      <c r="UK28" s="0"/>
-      <c r="UL28" s="0"/>
-      <c r="UM28" s="0"/>
-      <c r="UN28" s="0"/>
-      <c r="UO28" s="0"/>
-      <c r="UP28" s="0"/>
-      <c r="UQ28" s="0"/>
-      <c r="UR28" s="0"/>
-      <c r="US28" s="0"/>
-      <c r="UT28" s="0"/>
-      <c r="UU28" s="0"/>
-      <c r="UV28" s="0"/>
-      <c r="UW28" s="0"/>
-      <c r="UX28" s="0"/>
-      <c r="UY28" s="0"/>
-      <c r="UZ28" s="0"/>
-      <c r="VA28" s="0"/>
-      <c r="VB28" s="0"/>
-      <c r="VC28" s="0"/>
-      <c r="VD28" s="0"/>
-      <c r="VE28" s="0"/>
-      <c r="VF28" s="0"/>
-      <c r="VG28" s="0"/>
-      <c r="VH28" s="0"/>
-      <c r="VI28" s="0"/>
-      <c r="VJ28" s="0"/>
-      <c r="VK28" s="0"/>
-      <c r="VL28" s="0"/>
-      <c r="VM28" s="0"/>
-      <c r="VN28" s="0"/>
-      <c r="VO28" s="0"/>
-      <c r="VP28" s="0"/>
-      <c r="VQ28" s="0"/>
-      <c r="VR28" s="0"/>
-      <c r="VS28" s="0"/>
-      <c r="VT28" s="0"/>
-      <c r="VU28" s="0"/>
-      <c r="VV28" s="0"/>
-      <c r="VW28" s="0"/>
-      <c r="VX28" s="0"/>
-      <c r="VY28" s="0"/>
-      <c r="VZ28" s="0"/>
-      <c r="WA28" s="0"/>
-      <c r="WB28" s="0"/>
-      <c r="WC28" s="0"/>
-      <c r="WD28" s="0"/>
-      <c r="WE28" s="0"/>
-      <c r="WF28" s="0"/>
-      <c r="WG28" s="0"/>
-      <c r="WH28" s="0"/>
-      <c r="WI28" s="0"/>
-      <c r="WJ28" s="0"/>
-      <c r="WK28" s="0"/>
-      <c r="WL28" s="0"/>
-      <c r="WM28" s="0"/>
-      <c r="WN28" s="0"/>
-      <c r="WO28" s="0"/>
-      <c r="WP28" s="0"/>
-      <c r="WQ28" s="0"/>
-      <c r="WR28" s="0"/>
-      <c r="WS28" s="0"/>
-      <c r="WT28" s="0"/>
-      <c r="WU28" s="0"/>
-      <c r="WV28" s="0"/>
-      <c r="WW28" s="0"/>
-      <c r="WX28" s="0"/>
-      <c r="WY28" s="0"/>
-      <c r="WZ28" s="0"/>
-      <c r="XA28" s="0"/>
-      <c r="XB28" s="0"/>
-      <c r="XC28" s="0"/>
-      <c r="XD28" s="0"/>
-      <c r="XE28" s="0"/>
-      <c r="XF28" s="0"/>
-      <c r="XG28" s="0"/>
-      <c r="XH28" s="0"/>
-      <c r="XI28" s="0"/>
-      <c r="XJ28" s="0"/>
-      <c r="XK28" s="0"/>
-      <c r="XL28" s="0"/>
-      <c r="XM28" s="0"/>
-      <c r="XN28" s="0"/>
-      <c r="XO28" s="0"/>
-      <c r="XP28" s="0"/>
-      <c r="XQ28" s="0"/>
-      <c r="XR28" s="0"/>
-      <c r="XS28" s="0"/>
-      <c r="XT28" s="0"/>
-      <c r="XU28" s="0"/>
-      <c r="XV28" s="0"/>
-      <c r="XW28" s="0"/>
-      <c r="XX28" s="0"/>
-      <c r="XY28" s="0"/>
-      <c r="XZ28" s="0"/>
-      <c r="YA28" s="0"/>
-      <c r="YB28" s="0"/>
-      <c r="YC28" s="0"/>
-      <c r="YD28" s="0"/>
-      <c r="YE28" s="0"/>
-      <c r="YF28" s="0"/>
-      <c r="YG28" s="0"/>
-      <c r="YH28" s="0"/>
-      <c r="YI28" s="0"/>
-      <c r="YJ28" s="0"/>
-      <c r="YK28" s="0"/>
-      <c r="YL28" s="0"/>
-      <c r="YM28" s="0"/>
-      <c r="YN28" s="0"/>
-      <c r="YO28" s="0"/>
-      <c r="YP28" s="0"/>
-      <c r="YQ28" s="0"/>
-      <c r="YR28" s="0"/>
-      <c r="YS28" s="0"/>
-      <c r="YT28" s="0"/>
-      <c r="YU28" s="0"/>
-      <c r="YV28" s="0"/>
-      <c r="YW28" s="0"/>
-      <c r="YX28" s="0"/>
-      <c r="YY28" s="0"/>
-      <c r="YZ28" s="0"/>
-      <c r="ZA28" s="0"/>
-      <c r="ZB28" s="0"/>
-      <c r="ZC28" s="0"/>
-      <c r="ZD28" s="0"/>
-      <c r="ZE28" s="0"/>
-      <c r="ZF28" s="0"/>
-      <c r="ZG28" s="0"/>
-      <c r="ZH28" s="0"/>
-      <c r="ZI28" s="0"/>
-      <c r="ZJ28" s="0"/>
-      <c r="ZK28" s="0"/>
-      <c r="ZL28" s="0"/>
-      <c r="ZM28" s="0"/>
-      <c r="ZN28" s="0"/>
-      <c r="ZO28" s="0"/>
-      <c r="ZP28" s="0"/>
-      <c r="ZQ28" s="0"/>
-      <c r="ZR28" s="0"/>
-      <c r="ZS28" s="0"/>
-      <c r="ZT28" s="0"/>
-      <c r="ZU28" s="0"/>
-      <c r="ZV28" s="0"/>
-      <c r="ZW28" s="0"/>
-      <c r="ZX28" s="0"/>
-      <c r="ZY28" s="0"/>
-      <c r="ZZ28" s="0"/>
-      <c r="AAA28" s="0"/>
-      <c r="AAB28" s="0"/>
-      <c r="AAC28" s="0"/>
-      <c r="AAD28" s="0"/>
-      <c r="AAE28" s="0"/>
-      <c r="AAF28" s="0"/>
-      <c r="AAG28" s="0"/>
-      <c r="AAH28" s="0"/>
-      <c r="AAI28" s="0"/>
-      <c r="AAJ28" s="0"/>
-      <c r="AAK28" s="0"/>
-      <c r="AAL28" s="0"/>
-      <c r="AAM28" s="0"/>
-      <c r="AAN28" s="0"/>
-      <c r="AAO28" s="0"/>
-      <c r="AAP28" s="0"/>
-      <c r="AAQ28" s="0"/>
-      <c r="AAR28" s="0"/>
-      <c r="AAS28" s="0"/>
-      <c r="AAT28" s="0"/>
-      <c r="AAU28" s="0"/>
-      <c r="AAV28" s="0"/>
-      <c r="AAW28" s="0"/>
-      <c r="AAX28" s="0"/>
-      <c r="AAY28" s="0"/>
-      <c r="AAZ28" s="0"/>
-      <c r="ABA28" s="0"/>
-      <c r="ABB28" s="0"/>
-      <c r="ABC28" s="0"/>
-      <c r="ABD28" s="0"/>
-      <c r="ABE28" s="0"/>
-      <c r="ABF28" s="0"/>
-      <c r="ABG28" s="0"/>
-      <c r="ABH28" s="0"/>
-      <c r="ABI28" s="0"/>
-      <c r="ABJ28" s="0"/>
-      <c r="ABK28" s="0"/>
-      <c r="ABL28" s="0"/>
-      <c r="ABM28" s="0"/>
-      <c r="ABN28" s="0"/>
-      <c r="ABO28" s="0"/>
-      <c r="ABP28" s="0"/>
-      <c r="ABQ28" s="0"/>
-      <c r="ABR28" s="0"/>
-      <c r="ABS28" s="0"/>
-      <c r="ABT28" s="0"/>
-      <c r="ABU28" s="0"/>
-      <c r="ABV28" s="0"/>
-      <c r="ABW28" s="0"/>
-      <c r="ABX28" s="0"/>
-      <c r="ABY28" s="0"/>
-      <c r="ABZ28" s="0"/>
-      <c r="ACA28" s="0"/>
-      <c r="ACB28" s="0"/>
-      <c r="ACC28" s="0"/>
-      <c r="ACD28" s="0"/>
-      <c r="ACE28" s="0"/>
-      <c r="ACF28" s="0"/>
-      <c r="ACG28" s="0"/>
-      <c r="ACH28" s="0"/>
-      <c r="ACI28" s="0"/>
-      <c r="ACJ28" s="0"/>
-      <c r="ACK28" s="0"/>
-      <c r="ACL28" s="0"/>
-      <c r="ACM28" s="0"/>
-      <c r="ACN28" s="0"/>
-      <c r="ACO28" s="0"/>
-      <c r="ACP28" s="0"/>
-      <c r="ACQ28" s="0"/>
-      <c r="ACR28" s="0"/>
-      <c r="ACS28" s="0"/>
-      <c r="ACT28" s="0"/>
-      <c r="ACU28" s="0"/>
-      <c r="ACV28" s="0"/>
-      <c r="ACW28" s="0"/>
-      <c r="ACX28" s="0"/>
-      <c r="ACY28" s="0"/>
-      <c r="ACZ28" s="0"/>
-      <c r="ADA28" s="0"/>
-      <c r="ADB28" s="0"/>
-      <c r="ADC28" s="0"/>
-      <c r="ADD28" s="0"/>
-      <c r="ADE28" s="0"/>
-      <c r="ADF28" s="0"/>
-      <c r="ADG28" s="0"/>
-      <c r="ADH28" s="0"/>
-      <c r="ADI28" s="0"/>
-      <c r="ADJ28" s="0"/>
-      <c r="ADK28" s="0"/>
-      <c r="ADL28" s="0"/>
-      <c r="ADM28" s="0"/>
-      <c r="ADN28" s="0"/>
-      <c r="ADO28" s="0"/>
-      <c r="ADP28" s="0"/>
-      <c r="ADQ28" s="0"/>
-      <c r="ADR28" s="0"/>
-      <c r="ADS28" s="0"/>
-      <c r="ADT28" s="0"/>
-      <c r="ADU28" s="0"/>
-      <c r="ADV28" s="0"/>
-      <c r="ADW28" s="0"/>
-      <c r="ADX28" s="0"/>
-      <c r="ADY28" s="0"/>
-      <c r="ADZ28" s="0"/>
-      <c r="AEA28" s="0"/>
-      <c r="AEB28" s="0"/>
-      <c r="AEC28" s="0"/>
-      <c r="AED28" s="0"/>
-      <c r="AEE28" s="0"/>
-      <c r="AEF28" s="0"/>
-      <c r="AEG28" s="0"/>
-      <c r="AEH28" s="0"/>
-      <c r="AEI28" s="0"/>
-      <c r="AEJ28" s="0"/>
-      <c r="AEK28" s="0"/>
-      <c r="AEL28" s="0"/>
-      <c r="AEM28" s="0"/>
-      <c r="AEN28" s="0"/>
-      <c r="AEO28" s="0"/>
-      <c r="AEP28" s="0"/>
-      <c r="AEQ28" s="0"/>
-      <c r="AER28" s="0"/>
-      <c r="AES28" s="0"/>
-      <c r="AET28" s="0"/>
-      <c r="AEU28" s="0"/>
-      <c r="AEV28" s="0"/>
-      <c r="AEW28" s="0"/>
-      <c r="AEX28" s="0"/>
-      <c r="AEY28" s="0"/>
-      <c r="AEZ28" s="0"/>
-      <c r="AFA28" s="0"/>
-      <c r="AFB28" s="0"/>
-      <c r="AFC28" s="0"/>
-      <c r="AFD28" s="0"/>
-      <c r="AFE28" s="0"/>
-      <c r="AFF28" s="0"/>
-      <c r="AFG28" s="0"/>
-      <c r="AFH28" s="0"/>
-      <c r="AFI28" s="0"/>
-      <c r="AFJ28" s="0"/>
-      <c r="AFK28" s="0"/>
-      <c r="AFL28" s="0"/>
-      <c r="AFM28" s="0"/>
-      <c r="AFN28" s="0"/>
-      <c r="AFO28" s="0"/>
-      <c r="AFP28" s="0"/>
-      <c r="AFQ28" s="0"/>
-      <c r="AFR28" s="0"/>
-      <c r="AFS28" s="0"/>
-      <c r="AFT28" s="0"/>
-      <c r="AFU28" s="0"/>
-      <c r="AFV28" s="0"/>
-      <c r="AFW28" s="0"/>
-      <c r="AFX28" s="0"/>
-      <c r="AFY28" s="0"/>
-      <c r="AFZ28" s="0"/>
-      <c r="AGA28" s="0"/>
-      <c r="AGB28" s="0"/>
-      <c r="AGC28" s="0"/>
-      <c r="AGD28" s="0"/>
-      <c r="AGE28" s="0"/>
-      <c r="AGF28" s="0"/>
-      <c r="AGG28" s="0"/>
-      <c r="AGH28" s="0"/>
-      <c r="AGI28" s="0"/>
-      <c r="AGJ28" s="0"/>
-      <c r="AGK28" s="0"/>
-      <c r="AGL28" s="0"/>
-      <c r="AGM28" s="0"/>
-      <c r="AGN28" s="0"/>
-      <c r="AGO28" s="0"/>
-      <c r="AGP28" s="0"/>
-      <c r="AGQ28" s="0"/>
-      <c r="AGR28" s="0"/>
-      <c r="AGS28" s="0"/>
-      <c r="AGT28" s="0"/>
-      <c r="AGU28" s="0"/>
-      <c r="AGV28" s="0"/>
-      <c r="AGW28" s="0"/>
-      <c r="AGX28" s="0"/>
-      <c r="AGY28" s="0"/>
-      <c r="AGZ28" s="0"/>
-      <c r="AHA28" s="0"/>
-      <c r="AHB28" s="0"/>
-      <c r="AHC28" s="0"/>
-      <c r="AHD28" s="0"/>
-      <c r="AHE28" s="0"/>
-      <c r="AHF28" s="0"/>
-      <c r="AHG28" s="0"/>
-      <c r="AHH28" s="0"/>
-      <c r="AHI28" s="0"/>
-      <c r="AHJ28" s="0"/>
-      <c r="AHK28" s="0"/>
-      <c r="AHL28" s="0"/>
-      <c r="AHM28" s="0"/>
-      <c r="AHN28" s="0"/>
-      <c r="AHO28" s="0"/>
-      <c r="AHP28" s="0"/>
-      <c r="AHQ28" s="0"/>
-      <c r="AHR28" s="0"/>
-      <c r="AHS28" s="0"/>
-      <c r="AHT28" s="0"/>
-      <c r="AHU28" s="0"/>
-      <c r="AHV28" s="0"/>
-      <c r="AHW28" s="0"/>
-      <c r="AHX28" s="0"/>
-      <c r="AHY28" s="0"/>
-      <c r="AHZ28" s="0"/>
-      <c r="AIA28" s="0"/>
-      <c r="AIB28" s="0"/>
-      <c r="AIC28" s="0"/>
-      <c r="AID28" s="0"/>
-      <c r="AIE28" s="0"/>
-      <c r="AIF28" s="0"/>
-      <c r="AIG28" s="0"/>
-      <c r="AIH28" s="0"/>
-      <c r="AII28" s="0"/>
-      <c r="AIJ28" s="0"/>
-      <c r="AIK28" s="0"/>
-      <c r="AIL28" s="0"/>
-      <c r="AIM28" s="0"/>
-      <c r="AIN28" s="0"/>
-      <c r="AIO28" s="0"/>
-      <c r="AIP28" s="0"/>
-      <c r="AIQ28" s="0"/>
-      <c r="AIR28" s="0"/>
-      <c r="AIS28" s="0"/>
-      <c r="AIT28" s="0"/>
-      <c r="AIU28" s="0"/>
-      <c r="AIV28" s="0"/>
-      <c r="AIW28" s="0"/>
-      <c r="AIX28" s="0"/>
-      <c r="AIY28" s="0"/>
-      <c r="AIZ28" s="0"/>
-      <c r="AJA28" s="0"/>
-      <c r="AJB28" s="0"/>
-      <c r="AJC28" s="0"/>
-      <c r="AJD28" s="0"/>
-      <c r="AJE28" s="0"/>
-      <c r="AJF28" s="0"/>
-      <c r="AJG28" s="0"/>
-      <c r="AJH28" s="0"/>
-      <c r="AJI28" s="0"/>
-      <c r="AJJ28" s="0"/>
-      <c r="AJK28" s="0"/>
-      <c r="AJL28" s="0"/>
-      <c r="AJM28" s="0"/>
-      <c r="AJN28" s="0"/>
-      <c r="AJO28" s="0"/>
-      <c r="AJP28" s="0"/>
-      <c r="AJQ28" s="0"/>
-      <c r="AJR28" s="0"/>
-      <c r="AJS28" s="0"/>
-      <c r="AJT28" s="0"/>
-      <c r="AJU28" s="0"/>
-      <c r="AJV28" s="0"/>
-      <c r="AJW28" s="0"/>
-      <c r="AJX28" s="0"/>
-      <c r="AJY28" s="0"/>
-      <c r="AJZ28" s="0"/>
-      <c r="AKA28" s="0"/>
-      <c r="AKB28" s="0"/>
-      <c r="AKC28" s="0"/>
-      <c r="AKD28" s="0"/>
-      <c r="AKE28" s="0"/>
-      <c r="AKF28" s="0"/>
-      <c r="AKG28" s="0"/>
-      <c r="AKH28" s="0"/>
-      <c r="AKI28" s="0"/>
-      <c r="AKJ28" s="0"/>
-      <c r="AKK28" s="0"/>
-      <c r="AKL28" s="0"/>
-      <c r="AKM28" s="0"/>
-      <c r="AKN28" s="0"/>
-      <c r="AKO28" s="0"/>
-      <c r="AKP28" s="0"/>
-      <c r="AKQ28" s="0"/>
-      <c r="AKR28" s="0"/>
-      <c r="AKS28" s="0"/>
-      <c r="AKT28" s="0"/>
-      <c r="AKU28" s="0"/>
-      <c r="AKV28" s="0"/>
-      <c r="AKW28" s="0"/>
-      <c r="AKX28" s="0"/>
-      <c r="AKY28" s="0"/>
-      <c r="AKZ28" s="0"/>
-      <c r="ALA28" s="0"/>
-      <c r="ALB28" s="0"/>
-      <c r="ALC28" s="0"/>
-      <c r="ALD28" s="0"/>
-      <c r="ALE28" s="0"/>
-      <c r="ALF28" s="0"/>
-      <c r="ALG28" s="0"/>
-      <c r="ALH28" s="0"/>
-      <c r="ALI28" s="0"/>
-      <c r="ALJ28" s="0"/>
-      <c r="ALK28" s="0"/>
-      <c r="ALL28" s="0"/>
-      <c r="ALM28" s="0"/>
-      <c r="ALN28" s="0"/>
-      <c r="ALO28" s="0"/>
-      <c r="ALP28" s="0"/>
-      <c r="ALQ28" s="0"/>
-      <c r="ALR28" s="0"/>
-      <c r="ALS28" s="0"/>
-      <c r="ALT28" s="0"/>
-      <c r="ALU28" s="0"/>
-      <c r="ALV28" s="0"/>
-      <c r="ALW28" s="0"/>
-      <c r="ALX28" s="0"/>
-      <c r="ALY28" s="0"/>
-      <c r="ALZ28" s="0"/>
-      <c r="AMA28" s="0"/>
-      <c r="AMB28" s="0"/>
-      <c r="AMC28" s="0"/>
-      <c r="AMD28" s="0"/>
-      <c r="AME28" s="0"/>
-      <c r="AMF28" s="0"/>
-      <c r="AMG28" s="0"/>
-      <c r="AMH28" s="0"/>
-      <c r="AMI28" s="0"/>
-      <c r="AMJ28" s="0"/>
-    </row>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" s="10" customFormat="true" ht="116.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="35.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="0"/>
+        <v>75</v>
+      </c>
+      <c r="D31" s="7"/>
       <c r="E31" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="57.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="0"/>
-      <c r="D37" s="0"/>
-      <c r="E37" s="0"/>
-      <c r="F37" s="0"/>
+      <c r="A37" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
ajout de la classe lyon
</commit_message>
<xml_diff>
--- a/Maquette-Sources/Modèle-audit-SEO.xlsx
+++ b/Maquette-Sources/Modèle-audit-SEO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -235,7 +235,7 @@
     <t xml:space="preserve">balise meta keywords, div keywords</t>
   </si>
   <si>
-    <t xml:space="preserve">methode de black hat</t>
+    <t xml:space="preserve">Le fait de multiplier les mots clés fait parti des methode de black hat</t>
   </si>
   <si>
     <t xml:space="preserve">les supprimer</t>
@@ -298,7 +298,7 @@
     <t xml:space="preserve">les liens du footer sont nombreux et renvoient vers des pages 404</t>
   </si>
   <si>
-    <t xml:space="preserve">Vu le nombre de lien, il aurait été interressant de créer une page dédiée. Mais vu qu’ils renvoie tous vers des pages 404, il faut les supprimer sous peine que le site soit considéré comme non mis régulièrement à jour et améliorer l’expérience utilisateur</t>
+    <t xml:space="preserve">Vu qu’ils renvoie tous vers des pages 404, il faut les supprimer sous peine que le site soit considéré comme non mis régulièrement à jour et améliorer l’expérience utilisateur</t>
   </si>
   <si>
     <t xml:space="preserve">Il faut supprimer tous les liens 404</t>
@@ -317,6 +317,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter la balise canonical dans l’entête</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t>
   </si>
 </sst>
 </file>
@@ -595,9 +601,9 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E10" activeCellId="0" sqref="E10:E11"/>
+      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -794,7 +800,7 @@
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -949,8 +955,11 @@
       <c r="C30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>71</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>72</v>
@@ -1057,7 +1066,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1106,7 +1115,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2085,6 +2104,7 @@
     <hyperlink ref="F34" r:id="rId2" display="https://www.anthedesign.fr/referencement/seo-comment-optimiser-le-referencement-des-images/"/>
     <hyperlink ref="F35" r:id="rId3" display="https://www.anthedesign.fr/referencement/seo-comment-optimiser-le-referencement-des-images/"/>
     <hyperlink ref="F38" r:id="rId4" display="https://fr.oncrawl.com/seo-technique/contenu-page-avec-balises-semantiques-html5/"/>
+    <hyperlink ref="F39" r:id="rId5" display="https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2093,6 +2113,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correction des erreurs de css de style.css
</commit_message>
<xml_diff>
--- a/Maquette-Sources/Modèle-audit-SEO.xlsx
+++ b/Maquette-Sources/Modèle-audit-SEO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="148">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -166,6 +166,18 @@
     <t xml:space="preserve">icones réseau sociaux non visible</t>
   </si>
   <si>
+    <t xml:space="preserve">des balises li vides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les balises vides peuvent pertuber les lecteur d’écran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il ne faut pas utiliser de balises vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rapport </t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO + Bonne pratique SASS</t>
   </si>
   <si>
@@ -364,6 +376,18 @@
     <t xml:space="preserve">https://www.referenseo.com/guide-seo/balises-h1-h2-h3/#:~:text=Contrairement%20au%20titre%20h1%2C%20les,clés%20secondaires%20de%20votre%20page.</t>
   </si>
   <si>
+    <t xml:space="preserve">il n’y a pas de redirection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">une redirection sert à permettre à un internaute d’accéder à la page en tapant ou non les www</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il faut la mettre en place dans le fichier .htaccess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
     <t xml:space="preserve">Page 2</t>
   </si>
   <si>
@@ -403,7 +427,7 @@
     <t xml:space="preserve">le cache permet de charger plus rapidement la page lors de la prochaine visite</t>
   </si>
   <si>
-    <t xml:space="preserve">il faut mettre tous les gros fichiers (images…) en cache</t>
+    <t xml:space="preserve">il faut mettre tous les gros fichiers (images…) en cache. Il faut définir dans la durée de cache dans le fichier .htaccess</t>
   </si>
   <si>
     <t xml:space="preserve">https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055236-parametrez-le-cache-navigateur</t>
@@ -418,7 +442,31 @@
     <t xml:space="preserve">il faut l’alléger pour accèlerer la lecture par les bot</t>
   </si>
   <si>
-    <t xml:space="preserve">Il faut linter linter, minifier le code</t>
+    <t xml:space="preserve">Il faut linter linter, minifier, bundler le code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5543061-ecrivez-du-javascript-pour-le-web/5577726-optimisez-votre-code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dans le css présence d’un bloc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la taille du background est trop grand et donc trop lourd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">une image trop grande est lourde et nuit au référencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quand c’est possible comme dans le cas du background, prévoir des images de différentes tailles qui seront gérées par les media queries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.codeur.com/blog/seo-image-google/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taille du container non défini</t>
   </si>
 </sst>
 </file>
@@ -428,7 +476,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -487,8 +535,15 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,6 +566,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -551,13 +612,17 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -573,11 +638,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -588,8 +653,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -690,12 +775,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1004"/>
+  <dimension ref="A1:AMJ1006"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
+      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -704,7 +789,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="57.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.61"/>
@@ -712,55 +797,55 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="1" width="11.28"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="44.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -780,10 +865,10 @@
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -797,10 +882,10 @@
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -808,10 +893,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -820,7 +905,7 @@
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -829,14 +914,14 @@
       <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="E6" s="5"/>
+    <row r="6" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1" t="s">
         <v>28</v>
       </c>
@@ -857,97 +942,112 @@
       <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="128.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="44.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="72.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+    <row r="12" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E14" s="5"/>
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E15" s="5"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E16" s="5"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E17" s="5"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -958,296 +1058,299 @@
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="72.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="157.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="44.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="72.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="29" s="9" customFormat="true" ht="116.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>68</v>
-      </c>
+    <row r="29" s="12" customFormat="true" ht="116.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="13"/>
     </row>
-    <row r="30" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="10"/>
+    </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="35.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="57.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E35" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" s="6" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="58.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="114.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="A39" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E40" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E42" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="H42" s="0"/>
       <c r="I42" s="0"/>
@@ -2269,25 +2372,25 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>106</v>
+        <v>56</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E43" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H43" s="0"/>
       <c r="I43" s="0"/>
@@ -3309,25 +3412,25 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E44" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H44" s="0"/>
       <c r="I44" s="0"/>
@@ -4349,100 +4452,2190 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>113</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H45" s="0"/>
+      <c r="I45" s="0"/>
+      <c r="J45" s="0"/>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0"/>
+      <c r="N45" s="0"/>
+      <c r="O45" s="0"/>
+      <c r="P45" s="0"/>
+      <c r="Q45" s="0"/>
+      <c r="R45" s="0"/>
+      <c r="S45" s="0"/>
+      <c r="T45" s="0"/>
+      <c r="U45" s="0"/>
+      <c r="V45" s="0"/>
+      <c r="W45" s="0"/>
+      <c r="X45" s="0"/>
+      <c r="Y45" s="0"/>
+      <c r="Z45" s="0"/>
+      <c r="AA45" s="0"/>
+      <c r="AB45" s="0"/>
+      <c r="AC45" s="0"/>
+      <c r="AD45" s="0"/>
+      <c r="AE45" s="0"/>
+      <c r="AF45" s="0"/>
+      <c r="AG45" s="0"/>
+      <c r="AH45" s="0"/>
+      <c r="AI45" s="0"/>
+      <c r="AJ45" s="0"/>
+      <c r="AK45" s="0"/>
+      <c r="AL45" s="0"/>
+      <c r="AM45" s="0"/>
+      <c r="AN45" s="0"/>
+      <c r="AO45" s="0"/>
+      <c r="AP45" s="0"/>
+      <c r="AQ45" s="0"/>
+      <c r="AR45" s="0"/>
+      <c r="AS45" s="0"/>
+      <c r="AT45" s="0"/>
+      <c r="AU45" s="0"/>
+      <c r="AV45" s="0"/>
+      <c r="AW45" s="0"/>
+      <c r="AX45" s="0"/>
+      <c r="AY45" s="0"/>
+      <c r="AZ45" s="0"/>
+      <c r="BA45" s="0"/>
+      <c r="BB45" s="0"/>
+      <c r="BC45" s="0"/>
+      <c r="BD45" s="0"/>
+      <c r="BE45" s="0"/>
+      <c r="BF45" s="0"/>
+      <c r="BG45" s="0"/>
+      <c r="BH45" s="0"/>
+      <c r="BI45" s="0"/>
+      <c r="BJ45" s="0"/>
+      <c r="BK45" s="0"/>
+      <c r="BL45" s="0"/>
+      <c r="BM45" s="0"/>
+      <c r="BN45" s="0"/>
+      <c r="BO45" s="0"/>
+      <c r="BP45" s="0"/>
+      <c r="BQ45" s="0"/>
+      <c r="BR45" s="0"/>
+      <c r="BS45" s="0"/>
+      <c r="BT45" s="0"/>
+      <c r="BU45" s="0"/>
+      <c r="BV45" s="0"/>
+      <c r="BW45" s="0"/>
+      <c r="BX45" s="0"/>
+      <c r="BY45" s="0"/>
+      <c r="BZ45" s="0"/>
+      <c r="CA45" s="0"/>
+      <c r="CB45" s="0"/>
+      <c r="CC45" s="0"/>
+      <c r="CD45" s="0"/>
+      <c r="CE45" s="0"/>
+      <c r="CF45" s="0"/>
+      <c r="CG45" s="0"/>
+      <c r="CH45" s="0"/>
+      <c r="CI45" s="0"/>
+      <c r="CJ45" s="0"/>
+      <c r="CK45" s="0"/>
+      <c r="CL45" s="0"/>
+      <c r="CM45" s="0"/>
+      <c r="CN45" s="0"/>
+      <c r="CO45" s="0"/>
+      <c r="CP45" s="0"/>
+      <c r="CQ45" s="0"/>
+      <c r="CR45" s="0"/>
+      <c r="CS45" s="0"/>
+      <c r="CT45" s="0"/>
+      <c r="CU45" s="0"/>
+      <c r="CV45" s="0"/>
+      <c r="CW45" s="0"/>
+      <c r="CX45" s="0"/>
+      <c r="CY45" s="0"/>
+      <c r="CZ45" s="0"/>
+      <c r="DA45" s="0"/>
+      <c r="DB45" s="0"/>
+      <c r="DC45" s="0"/>
+      <c r="DD45" s="0"/>
+      <c r="DE45" s="0"/>
+      <c r="DF45" s="0"/>
+      <c r="DG45" s="0"/>
+      <c r="DH45" s="0"/>
+      <c r="DI45" s="0"/>
+      <c r="DJ45" s="0"/>
+      <c r="DK45" s="0"/>
+      <c r="DL45" s="0"/>
+      <c r="DM45" s="0"/>
+      <c r="DN45" s="0"/>
+      <c r="DO45" s="0"/>
+      <c r="DP45" s="0"/>
+      <c r="DQ45" s="0"/>
+      <c r="DR45" s="0"/>
+      <c r="DS45" s="0"/>
+      <c r="DT45" s="0"/>
+      <c r="DU45" s="0"/>
+      <c r="DV45" s="0"/>
+      <c r="DW45" s="0"/>
+      <c r="DX45" s="0"/>
+      <c r="DY45" s="0"/>
+      <c r="DZ45" s="0"/>
+      <c r="EA45" s="0"/>
+      <c r="EB45" s="0"/>
+      <c r="EC45" s="0"/>
+      <c r="ED45" s="0"/>
+      <c r="EE45" s="0"/>
+      <c r="EF45" s="0"/>
+      <c r="EG45" s="0"/>
+      <c r="EH45" s="0"/>
+      <c r="EI45" s="0"/>
+      <c r="EJ45" s="0"/>
+      <c r="EK45" s="0"/>
+      <c r="EL45" s="0"/>
+      <c r="EM45" s="0"/>
+      <c r="EN45" s="0"/>
+      <c r="EO45" s="0"/>
+      <c r="EP45" s="0"/>
+      <c r="EQ45" s="0"/>
+      <c r="ER45" s="0"/>
+      <c r="ES45" s="0"/>
+      <c r="ET45" s="0"/>
+      <c r="EU45" s="0"/>
+      <c r="EV45" s="0"/>
+      <c r="EW45" s="0"/>
+      <c r="EX45" s="0"/>
+      <c r="EY45" s="0"/>
+      <c r="EZ45" s="0"/>
+      <c r="FA45" s="0"/>
+      <c r="FB45" s="0"/>
+      <c r="FC45" s="0"/>
+      <c r="FD45" s="0"/>
+      <c r="FE45" s="0"/>
+      <c r="FF45" s="0"/>
+      <c r="FG45" s="0"/>
+      <c r="FH45" s="0"/>
+      <c r="FI45" s="0"/>
+      <c r="FJ45" s="0"/>
+      <c r="FK45" s="0"/>
+      <c r="FL45" s="0"/>
+      <c r="FM45" s="0"/>
+      <c r="FN45" s="0"/>
+      <c r="FO45" s="0"/>
+      <c r="FP45" s="0"/>
+      <c r="FQ45" s="0"/>
+      <c r="FR45" s="0"/>
+      <c r="FS45" s="0"/>
+      <c r="FT45" s="0"/>
+      <c r="FU45" s="0"/>
+      <c r="FV45" s="0"/>
+      <c r="FW45" s="0"/>
+      <c r="FX45" s="0"/>
+      <c r="FY45" s="0"/>
+      <c r="FZ45" s="0"/>
+      <c r="GA45" s="0"/>
+      <c r="GB45" s="0"/>
+      <c r="GC45" s="0"/>
+      <c r="GD45" s="0"/>
+      <c r="GE45" s="0"/>
+      <c r="GF45" s="0"/>
+      <c r="GG45" s="0"/>
+      <c r="GH45" s="0"/>
+      <c r="GI45" s="0"/>
+      <c r="GJ45" s="0"/>
+      <c r="GK45" s="0"/>
+      <c r="GL45" s="0"/>
+      <c r="GM45" s="0"/>
+      <c r="GN45" s="0"/>
+      <c r="GO45" s="0"/>
+      <c r="GP45" s="0"/>
+      <c r="GQ45" s="0"/>
+      <c r="GR45" s="0"/>
+      <c r="GS45" s="0"/>
+      <c r="GT45" s="0"/>
+      <c r="GU45" s="0"/>
+      <c r="GV45" s="0"/>
+      <c r="GW45" s="0"/>
+      <c r="GX45" s="0"/>
+      <c r="GY45" s="0"/>
+      <c r="GZ45" s="0"/>
+      <c r="HA45" s="0"/>
+      <c r="HB45" s="0"/>
+      <c r="HC45" s="0"/>
+      <c r="HD45" s="0"/>
+      <c r="HE45" s="0"/>
+      <c r="HF45" s="0"/>
+      <c r="HG45" s="0"/>
+      <c r="HH45" s="0"/>
+      <c r="HI45" s="0"/>
+      <c r="HJ45" s="0"/>
+      <c r="HK45" s="0"/>
+      <c r="HL45" s="0"/>
+      <c r="HM45" s="0"/>
+      <c r="HN45" s="0"/>
+      <c r="HO45" s="0"/>
+      <c r="HP45" s="0"/>
+      <c r="HQ45" s="0"/>
+      <c r="HR45" s="0"/>
+      <c r="HS45" s="0"/>
+      <c r="HT45" s="0"/>
+      <c r="HU45" s="0"/>
+      <c r="HV45" s="0"/>
+      <c r="HW45" s="0"/>
+      <c r="HX45" s="0"/>
+      <c r="HY45" s="0"/>
+      <c r="HZ45" s="0"/>
+      <c r="IA45" s="0"/>
+      <c r="IB45" s="0"/>
+      <c r="IC45" s="0"/>
+      <c r="ID45" s="0"/>
+      <c r="IE45" s="0"/>
+      <c r="IF45" s="0"/>
+      <c r="IG45" s="0"/>
+      <c r="IH45" s="0"/>
+      <c r="II45" s="0"/>
+      <c r="IJ45" s="0"/>
+      <c r="IK45" s="0"/>
+      <c r="IL45" s="0"/>
+      <c r="IM45" s="0"/>
+      <c r="IN45" s="0"/>
+      <c r="IO45" s="0"/>
+      <c r="IP45" s="0"/>
+      <c r="IQ45" s="0"/>
+      <c r="IR45" s="0"/>
+      <c r="IS45" s="0"/>
+      <c r="IT45" s="0"/>
+      <c r="IU45" s="0"/>
+      <c r="IV45" s="0"/>
+      <c r="IW45" s="0"/>
+      <c r="IX45" s="0"/>
+      <c r="IY45" s="0"/>
+      <c r="IZ45" s="0"/>
+      <c r="JA45" s="0"/>
+      <c r="JB45" s="0"/>
+      <c r="JC45" s="0"/>
+      <c r="JD45" s="0"/>
+      <c r="JE45" s="0"/>
+      <c r="JF45" s="0"/>
+      <c r="JG45" s="0"/>
+      <c r="JH45" s="0"/>
+      <c r="JI45" s="0"/>
+      <c r="JJ45" s="0"/>
+      <c r="JK45" s="0"/>
+      <c r="JL45" s="0"/>
+      <c r="JM45" s="0"/>
+      <c r="JN45" s="0"/>
+      <c r="JO45" s="0"/>
+      <c r="JP45" s="0"/>
+      <c r="JQ45" s="0"/>
+      <c r="JR45" s="0"/>
+      <c r="JS45" s="0"/>
+      <c r="JT45" s="0"/>
+      <c r="JU45" s="0"/>
+      <c r="JV45" s="0"/>
+      <c r="JW45" s="0"/>
+      <c r="JX45" s="0"/>
+      <c r="JY45" s="0"/>
+      <c r="JZ45" s="0"/>
+      <c r="KA45" s="0"/>
+      <c r="KB45" s="0"/>
+      <c r="KC45" s="0"/>
+      <c r="KD45" s="0"/>
+      <c r="KE45" s="0"/>
+      <c r="KF45" s="0"/>
+      <c r="KG45" s="0"/>
+      <c r="KH45" s="0"/>
+      <c r="KI45" s="0"/>
+      <c r="KJ45" s="0"/>
+      <c r="KK45" s="0"/>
+      <c r="KL45" s="0"/>
+      <c r="KM45" s="0"/>
+      <c r="KN45" s="0"/>
+      <c r="KO45" s="0"/>
+      <c r="KP45" s="0"/>
+      <c r="KQ45" s="0"/>
+      <c r="KR45" s="0"/>
+      <c r="KS45" s="0"/>
+      <c r="KT45" s="0"/>
+      <c r="KU45" s="0"/>
+      <c r="KV45" s="0"/>
+      <c r="KW45" s="0"/>
+      <c r="KX45" s="0"/>
+      <c r="KY45" s="0"/>
+      <c r="KZ45" s="0"/>
+      <c r="LA45" s="0"/>
+      <c r="LB45" s="0"/>
+      <c r="LC45" s="0"/>
+      <c r="LD45" s="0"/>
+      <c r="LE45" s="0"/>
+      <c r="LF45" s="0"/>
+      <c r="LG45" s="0"/>
+      <c r="LH45" s="0"/>
+      <c r="LI45" s="0"/>
+      <c r="LJ45" s="0"/>
+      <c r="LK45" s="0"/>
+      <c r="LL45" s="0"/>
+      <c r="LM45" s="0"/>
+      <c r="LN45" s="0"/>
+      <c r="LO45" s="0"/>
+      <c r="LP45" s="0"/>
+      <c r="LQ45" s="0"/>
+      <c r="LR45" s="0"/>
+      <c r="LS45" s="0"/>
+      <c r="LT45" s="0"/>
+      <c r="LU45" s="0"/>
+      <c r="LV45" s="0"/>
+      <c r="LW45" s="0"/>
+      <c r="LX45" s="0"/>
+      <c r="LY45" s="0"/>
+      <c r="LZ45" s="0"/>
+      <c r="MA45" s="0"/>
+      <c r="MB45" s="0"/>
+      <c r="MC45" s="0"/>
+      <c r="MD45" s="0"/>
+      <c r="ME45" s="0"/>
+      <c r="MF45" s="0"/>
+      <c r="MG45" s="0"/>
+      <c r="MH45" s="0"/>
+      <c r="MI45" s="0"/>
+      <c r="MJ45" s="0"/>
+      <c r="MK45" s="0"/>
+      <c r="ML45" s="0"/>
+      <c r="MM45" s="0"/>
+      <c r="MN45" s="0"/>
+      <c r="MO45" s="0"/>
+      <c r="MP45" s="0"/>
+      <c r="MQ45" s="0"/>
+      <c r="MR45" s="0"/>
+      <c r="MS45" s="0"/>
+      <c r="MT45" s="0"/>
+      <c r="MU45" s="0"/>
+      <c r="MV45" s="0"/>
+      <c r="MW45" s="0"/>
+      <c r="MX45" s="0"/>
+      <c r="MY45" s="0"/>
+      <c r="MZ45" s="0"/>
+      <c r="NA45" s="0"/>
+      <c r="NB45" s="0"/>
+      <c r="NC45" s="0"/>
+      <c r="ND45" s="0"/>
+      <c r="NE45" s="0"/>
+      <c r="NF45" s="0"/>
+      <c r="NG45" s="0"/>
+      <c r="NH45" s="0"/>
+      <c r="NI45" s="0"/>
+      <c r="NJ45" s="0"/>
+      <c r="NK45" s="0"/>
+      <c r="NL45" s="0"/>
+      <c r="NM45" s="0"/>
+      <c r="NN45" s="0"/>
+      <c r="NO45" s="0"/>
+      <c r="NP45" s="0"/>
+      <c r="NQ45" s="0"/>
+      <c r="NR45" s="0"/>
+      <c r="NS45" s="0"/>
+      <c r="NT45" s="0"/>
+      <c r="NU45" s="0"/>
+      <c r="NV45" s="0"/>
+      <c r="NW45" s="0"/>
+      <c r="NX45" s="0"/>
+      <c r="NY45" s="0"/>
+      <c r="NZ45" s="0"/>
+      <c r="OA45" s="0"/>
+      <c r="OB45" s="0"/>
+      <c r="OC45" s="0"/>
+      <c r="OD45" s="0"/>
+      <c r="OE45" s="0"/>
+      <c r="OF45" s="0"/>
+      <c r="OG45" s="0"/>
+      <c r="OH45" s="0"/>
+      <c r="OI45" s="0"/>
+      <c r="OJ45" s="0"/>
+      <c r="OK45" s="0"/>
+      <c r="OL45" s="0"/>
+      <c r="OM45" s="0"/>
+      <c r="ON45" s="0"/>
+      <c r="OO45" s="0"/>
+      <c r="OP45" s="0"/>
+      <c r="OQ45" s="0"/>
+      <c r="OR45" s="0"/>
+      <c r="OS45" s="0"/>
+      <c r="OT45" s="0"/>
+      <c r="OU45" s="0"/>
+      <c r="OV45" s="0"/>
+      <c r="OW45" s="0"/>
+      <c r="OX45" s="0"/>
+      <c r="OY45" s="0"/>
+      <c r="OZ45" s="0"/>
+      <c r="PA45" s="0"/>
+      <c r="PB45" s="0"/>
+      <c r="PC45" s="0"/>
+      <c r="PD45" s="0"/>
+      <c r="PE45" s="0"/>
+      <c r="PF45" s="0"/>
+      <c r="PG45" s="0"/>
+      <c r="PH45" s="0"/>
+      <c r="PI45" s="0"/>
+      <c r="PJ45" s="0"/>
+      <c r="PK45" s="0"/>
+      <c r="PL45" s="0"/>
+      <c r="PM45" s="0"/>
+      <c r="PN45" s="0"/>
+      <c r="PO45" s="0"/>
+      <c r="PP45" s="0"/>
+      <c r="PQ45" s="0"/>
+      <c r="PR45" s="0"/>
+      <c r="PS45" s="0"/>
+      <c r="PT45" s="0"/>
+      <c r="PU45" s="0"/>
+      <c r="PV45" s="0"/>
+      <c r="PW45" s="0"/>
+      <c r="PX45" s="0"/>
+      <c r="PY45" s="0"/>
+      <c r="PZ45" s="0"/>
+      <c r="QA45" s="0"/>
+      <c r="QB45" s="0"/>
+      <c r="QC45" s="0"/>
+      <c r="QD45" s="0"/>
+      <c r="QE45" s="0"/>
+      <c r="QF45" s="0"/>
+      <c r="QG45" s="0"/>
+      <c r="QH45" s="0"/>
+      <c r="QI45" s="0"/>
+      <c r="QJ45" s="0"/>
+      <c r="QK45" s="0"/>
+      <c r="QL45" s="0"/>
+      <c r="QM45" s="0"/>
+      <c r="QN45" s="0"/>
+      <c r="QO45" s="0"/>
+      <c r="QP45" s="0"/>
+      <c r="QQ45" s="0"/>
+      <c r="QR45" s="0"/>
+      <c r="QS45" s="0"/>
+      <c r="QT45" s="0"/>
+      <c r="QU45" s="0"/>
+      <c r="QV45" s="0"/>
+      <c r="QW45" s="0"/>
+      <c r="QX45" s="0"/>
+      <c r="QY45" s="0"/>
+      <c r="QZ45" s="0"/>
+      <c r="RA45" s="0"/>
+      <c r="RB45" s="0"/>
+      <c r="RC45" s="0"/>
+      <c r="RD45" s="0"/>
+      <c r="RE45" s="0"/>
+      <c r="RF45" s="0"/>
+      <c r="RG45" s="0"/>
+      <c r="RH45" s="0"/>
+      <c r="RI45" s="0"/>
+      <c r="RJ45" s="0"/>
+      <c r="RK45" s="0"/>
+      <c r="RL45" s="0"/>
+      <c r="RM45" s="0"/>
+      <c r="RN45" s="0"/>
+      <c r="RO45" s="0"/>
+      <c r="RP45" s="0"/>
+      <c r="RQ45" s="0"/>
+      <c r="RR45" s="0"/>
+      <c r="RS45" s="0"/>
+      <c r="RT45" s="0"/>
+      <c r="RU45" s="0"/>
+      <c r="RV45" s="0"/>
+      <c r="RW45" s="0"/>
+      <c r="RX45" s="0"/>
+      <c r="RY45" s="0"/>
+      <c r="RZ45" s="0"/>
+      <c r="SA45" s="0"/>
+      <c r="SB45" s="0"/>
+      <c r="SC45" s="0"/>
+      <c r="SD45" s="0"/>
+      <c r="SE45" s="0"/>
+      <c r="SF45" s="0"/>
+      <c r="SG45" s="0"/>
+      <c r="SH45" s="0"/>
+      <c r="SI45" s="0"/>
+      <c r="SJ45" s="0"/>
+      <c r="SK45" s="0"/>
+      <c r="SL45" s="0"/>
+      <c r="SM45" s="0"/>
+      <c r="SN45" s="0"/>
+      <c r="SO45" s="0"/>
+      <c r="SP45" s="0"/>
+      <c r="SQ45" s="0"/>
+      <c r="SR45" s="0"/>
+      <c r="SS45" s="0"/>
+      <c r="ST45" s="0"/>
+      <c r="SU45" s="0"/>
+      <c r="SV45" s="0"/>
+      <c r="SW45" s="0"/>
+      <c r="SX45" s="0"/>
+      <c r="SY45" s="0"/>
+      <c r="SZ45" s="0"/>
+      <c r="TA45" s="0"/>
+      <c r="TB45" s="0"/>
+      <c r="TC45" s="0"/>
+      <c r="TD45" s="0"/>
+      <c r="TE45" s="0"/>
+      <c r="TF45" s="0"/>
+      <c r="TG45" s="0"/>
+      <c r="TH45" s="0"/>
+      <c r="TI45" s="0"/>
+      <c r="TJ45" s="0"/>
+      <c r="TK45" s="0"/>
+      <c r="TL45" s="0"/>
+      <c r="TM45" s="0"/>
+      <c r="TN45" s="0"/>
+      <c r="TO45" s="0"/>
+      <c r="TP45" s="0"/>
+      <c r="TQ45" s="0"/>
+      <c r="TR45" s="0"/>
+      <c r="TS45" s="0"/>
+      <c r="TT45" s="0"/>
+      <c r="TU45" s="0"/>
+      <c r="TV45" s="0"/>
+      <c r="TW45" s="0"/>
+      <c r="TX45" s="0"/>
+      <c r="TY45" s="0"/>
+      <c r="TZ45" s="0"/>
+      <c r="UA45" s="0"/>
+      <c r="UB45" s="0"/>
+      <c r="UC45" s="0"/>
+      <c r="UD45" s="0"/>
+      <c r="UE45" s="0"/>
+      <c r="UF45" s="0"/>
+      <c r="UG45" s="0"/>
+      <c r="UH45" s="0"/>
+      <c r="UI45" s="0"/>
+      <c r="UJ45" s="0"/>
+      <c r="UK45" s="0"/>
+      <c r="UL45" s="0"/>
+      <c r="UM45" s="0"/>
+      <c r="UN45" s="0"/>
+      <c r="UO45" s="0"/>
+      <c r="UP45" s="0"/>
+      <c r="UQ45" s="0"/>
+      <c r="UR45" s="0"/>
+      <c r="US45" s="0"/>
+      <c r="UT45" s="0"/>
+      <c r="UU45" s="0"/>
+      <c r="UV45" s="0"/>
+      <c r="UW45" s="0"/>
+      <c r="UX45" s="0"/>
+      <c r="UY45" s="0"/>
+      <c r="UZ45" s="0"/>
+      <c r="VA45" s="0"/>
+      <c r="VB45" s="0"/>
+      <c r="VC45" s="0"/>
+      <c r="VD45" s="0"/>
+      <c r="VE45" s="0"/>
+      <c r="VF45" s="0"/>
+      <c r="VG45" s="0"/>
+      <c r="VH45" s="0"/>
+      <c r="VI45" s="0"/>
+      <c r="VJ45" s="0"/>
+      <c r="VK45" s="0"/>
+      <c r="VL45" s="0"/>
+      <c r="VM45" s="0"/>
+      <c r="VN45" s="0"/>
+      <c r="VO45" s="0"/>
+      <c r="VP45" s="0"/>
+      <c r="VQ45" s="0"/>
+      <c r="VR45" s="0"/>
+      <c r="VS45" s="0"/>
+      <c r="VT45" s="0"/>
+      <c r="VU45" s="0"/>
+      <c r="VV45" s="0"/>
+      <c r="VW45" s="0"/>
+      <c r="VX45" s="0"/>
+      <c r="VY45" s="0"/>
+      <c r="VZ45" s="0"/>
+      <c r="WA45" s="0"/>
+      <c r="WB45" s="0"/>
+      <c r="WC45" s="0"/>
+      <c r="WD45" s="0"/>
+      <c r="WE45" s="0"/>
+      <c r="WF45" s="0"/>
+      <c r="WG45" s="0"/>
+      <c r="WH45" s="0"/>
+      <c r="WI45" s="0"/>
+      <c r="WJ45" s="0"/>
+      <c r="WK45" s="0"/>
+      <c r="WL45" s="0"/>
+      <c r="WM45" s="0"/>
+      <c r="WN45" s="0"/>
+      <c r="WO45" s="0"/>
+      <c r="WP45" s="0"/>
+      <c r="WQ45" s="0"/>
+      <c r="WR45" s="0"/>
+      <c r="WS45" s="0"/>
+      <c r="WT45" s="0"/>
+      <c r="WU45" s="0"/>
+      <c r="WV45" s="0"/>
+      <c r="WW45" s="0"/>
+      <c r="WX45" s="0"/>
+      <c r="WY45" s="0"/>
+      <c r="WZ45" s="0"/>
+      <c r="XA45" s="0"/>
+      <c r="XB45" s="0"/>
+      <c r="XC45" s="0"/>
+      <c r="XD45" s="0"/>
+      <c r="XE45" s="0"/>
+      <c r="XF45" s="0"/>
+      <c r="XG45" s="0"/>
+      <c r="XH45" s="0"/>
+      <c r="XI45" s="0"/>
+      <c r="XJ45" s="0"/>
+      <c r="XK45" s="0"/>
+      <c r="XL45" s="0"/>
+      <c r="XM45" s="0"/>
+      <c r="XN45" s="0"/>
+      <c r="XO45" s="0"/>
+      <c r="XP45" s="0"/>
+      <c r="XQ45" s="0"/>
+      <c r="XR45" s="0"/>
+      <c r="XS45" s="0"/>
+      <c r="XT45" s="0"/>
+      <c r="XU45" s="0"/>
+      <c r="XV45" s="0"/>
+      <c r="XW45" s="0"/>
+      <c r="XX45" s="0"/>
+      <c r="XY45" s="0"/>
+      <c r="XZ45" s="0"/>
+      <c r="YA45" s="0"/>
+      <c r="YB45" s="0"/>
+      <c r="YC45" s="0"/>
+      <c r="YD45" s="0"/>
+      <c r="YE45" s="0"/>
+      <c r="YF45" s="0"/>
+      <c r="YG45" s="0"/>
+      <c r="YH45" s="0"/>
+      <c r="YI45" s="0"/>
+      <c r="YJ45" s="0"/>
+      <c r="YK45" s="0"/>
+      <c r="YL45" s="0"/>
+      <c r="YM45" s="0"/>
+      <c r="YN45" s="0"/>
+      <c r="YO45" s="0"/>
+      <c r="YP45" s="0"/>
+      <c r="YQ45" s="0"/>
+      <c r="YR45" s="0"/>
+      <c r="YS45" s="0"/>
+      <c r="YT45" s="0"/>
+      <c r="YU45" s="0"/>
+      <c r="YV45" s="0"/>
+      <c r="YW45" s="0"/>
+      <c r="YX45" s="0"/>
+      <c r="YY45" s="0"/>
+      <c r="YZ45" s="0"/>
+      <c r="ZA45" s="0"/>
+      <c r="ZB45" s="0"/>
+      <c r="ZC45" s="0"/>
+      <c r="ZD45" s="0"/>
+      <c r="ZE45" s="0"/>
+      <c r="ZF45" s="0"/>
+      <c r="ZG45" s="0"/>
+      <c r="ZH45" s="0"/>
+      <c r="ZI45" s="0"/>
+      <c r="ZJ45" s="0"/>
+      <c r="ZK45" s="0"/>
+      <c r="ZL45" s="0"/>
+      <c r="ZM45" s="0"/>
+      <c r="ZN45" s="0"/>
+      <c r="ZO45" s="0"/>
+      <c r="ZP45" s="0"/>
+      <c r="ZQ45" s="0"/>
+      <c r="ZR45" s="0"/>
+      <c r="ZS45" s="0"/>
+      <c r="ZT45" s="0"/>
+      <c r="ZU45" s="0"/>
+      <c r="ZV45" s="0"/>
+      <c r="ZW45" s="0"/>
+      <c r="ZX45" s="0"/>
+      <c r="ZY45" s="0"/>
+      <c r="ZZ45" s="0"/>
+      <c r="AAA45" s="0"/>
+      <c r="AAB45" s="0"/>
+      <c r="AAC45" s="0"/>
+      <c r="AAD45" s="0"/>
+      <c r="AAE45" s="0"/>
+      <c r="AAF45" s="0"/>
+      <c r="AAG45" s="0"/>
+      <c r="AAH45" s="0"/>
+      <c r="AAI45" s="0"/>
+      <c r="AAJ45" s="0"/>
+      <c r="AAK45" s="0"/>
+      <c r="AAL45" s="0"/>
+      <c r="AAM45" s="0"/>
+      <c r="AAN45" s="0"/>
+      <c r="AAO45" s="0"/>
+      <c r="AAP45" s="0"/>
+      <c r="AAQ45" s="0"/>
+      <c r="AAR45" s="0"/>
+      <c r="AAS45" s="0"/>
+      <c r="AAT45" s="0"/>
+      <c r="AAU45" s="0"/>
+      <c r="AAV45" s="0"/>
+      <c r="AAW45" s="0"/>
+      <c r="AAX45" s="0"/>
+      <c r="AAY45" s="0"/>
+      <c r="AAZ45" s="0"/>
+      <c r="ABA45" s="0"/>
+      <c r="ABB45" s="0"/>
+      <c r="ABC45" s="0"/>
+      <c r="ABD45" s="0"/>
+      <c r="ABE45" s="0"/>
+      <c r="ABF45" s="0"/>
+      <c r="ABG45" s="0"/>
+      <c r="ABH45" s="0"/>
+      <c r="ABI45" s="0"/>
+      <c r="ABJ45" s="0"/>
+      <c r="ABK45" s="0"/>
+      <c r="ABL45" s="0"/>
+      <c r="ABM45" s="0"/>
+      <c r="ABN45" s="0"/>
+      <c r="ABO45" s="0"/>
+      <c r="ABP45" s="0"/>
+      <c r="ABQ45" s="0"/>
+      <c r="ABR45" s="0"/>
+      <c r="ABS45" s="0"/>
+      <c r="ABT45" s="0"/>
+      <c r="ABU45" s="0"/>
+      <c r="ABV45" s="0"/>
+      <c r="ABW45" s="0"/>
+      <c r="ABX45" s="0"/>
+      <c r="ABY45" s="0"/>
+      <c r="ABZ45" s="0"/>
+      <c r="ACA45" s="0"/>
+      <c r="ACB45" s="0"/>
+      <c r="ACC45" s="0"/>
+      <c r="ACD45" s="0"/>
+      <c r="ACE45" s="0"/>
+      <c r="ACF45" s="0"/>
+      <c r="ACG45" s="0"/>
+      <c r="ACH45" s="0"/>
+      <c r="ACI45" s="0"/>
+      <c r="ACJ45" s="0"/>
+      <c r="ACK45" s="0"/>
+      <c r="ACL45" s="0"/>
+      <c r="ACM45" s="0"/>
+      <c r="ACN45" s="0"/>
+      <c r="ACO45" s="0"/>
+      <c r="ACP45" s="0"/>
+      <c r="ACQ45" s="0"/>
+      <c r="ACR45" s="0"/>
+      <c r="ACS45" s="0"/>
+      <c r="ACT45" s="0"/>
+      <c r="ACU45" s="0"/>
+      <c r="ACV45" s="0"/>
+      <c r="ACW45" s="0"/>
+      <c r="ACX45" s="0"/>
+      <c r="ACY45" s="0"/>
+      <c r="ACZ45" s="0"/>
+      <c r="ADA45" s="0"/>
+      <c r="ADB45" s="0"/>
+      <c r="ADC45" s="0"/>
+      <c r="ADD45" s="0"/>
+      <c r="ADE45" s="0"/>
+      <c r="ADF45" s="0"/>
+      <c r="ADG45" s="0"/>
+      <c r="ADH45" s="0"/>
+      <c r="ADI45" s="0"/>
+      <c r="ADJ45" s="0"/>
+      <c r="ADK45" s="0"/>
+      <c r="ADL45" s="0"/>
+      <c r="ADM45" s="0"/>
+      <c r="ADN45" s="0"/>
+      <c r="ADO45" s="0"/>
+      <c r="ADP45" s="0"/>
+      <c r="ADQ45" s="0"/>
+      <c r="ADR45" s="0"/>
+      <c r="ADS45" s="0"/>
+      <c r="ADT45" s="0"/>
+      <c r="ADU45" s="0"/>
+      <c r="ADV45" s="0"/>
+      <c r="ADW45" s="0"/>
+      <c r="ADX45" s="0"/>
+      <c r="ADY45" s="0"/>
+      <c r="ADZ45" s="0"/>
+      <c r="AEA45" s="0"/>
+      <c r="AEB45" s="0"/>
+      <c r="AEC45" s="0"/>
+      <c r="AED45" s="0"/>
+      <c r="AEE45" s="0"/>
+      <c r="AEF45" s="0"/>
+      <c r="AEG45" s="0"/>
+      <c r="AEH45" s="0"/>
+      <c r="AEI45" s="0"/>
+      <c r="AEJ45" s="0"/>
+      <c r="AEK45" s="0"/>
+      <c r="AEL45" s="0"/>
+      <c r="AEM45" s="0"/>
+      <c r="AEN45" s="0"/>
+      <c r="AEO45" s="0"/>
+      <c r="AEP45" s="0"/>
+      <c r="AEQ45" s="0"/>
+      <c r="AER45" s="0"/>
+      <c r="AES45" s="0"/>
+      <c r="AET45" s="0"/>
+      <c r="AEU45" s="0"/>
+      <c r="AEV45" s="0"/>
+      <c r="AEW45" s="0"/>
+      <c r="AEX45" s="0"/>
+      <c r="AEY45" s="0"/>
+      <c r="AEZ45" s="0"/>
+      <c r="AFA45" s="0"/>
+      <c r="AFB45" s="0"/>
+      <c r="AFC45" s="0"/>
+      <c r="AFD45" s="0"/>
+      <c r="AFE45" s="0"/>
+      <c r="AFF45" s="0"/>
+      <c r="AFG45" s="0"/>
+      <c r="AFH45" s="0"/>
+      <c r="AFI45" s="0"/>
+      <c r="AFJ45" s="0"/>
+      <c r="AFK45" s="0"/>
+      <c r="AFL45" s="0"/>
+      <c r="AFM45" s="0"/>
+      <c r="AFN45" s="0"/>
+      <c r="AFO45" s="0"/>
+      <c r="AFP45" s="0"/>
+      <c r="AFQ45" s="0"/>
+      <c r="AFR45" s="0"/>
+      <c r="AFS45" s="0"/>
+      <c r="AFT45" s="0"/>
+      <c r="AFU45" s="0"/>
+      <c r="AFV45" s="0"/>
+      <c r="AFW45" s="0"/>
+      <c r="AFX45" s="0"/>
+      <c r="AFY45" s="0"/>
+      <c r="AFZ45" s="0"/>
+      <c r="AGA45" s="0"/>
+      <c r="AGB45" s="0"/>
+      <c r="AGC45" s="0"/>
+      <c r="AGD45" s="0"/>
+      <c r="AGE45" s="0"/>
+      <c r="AGF45" s="0"/>
+      <c r="AGG45" s="0"/>
+      <c r="AGH45" s="0"/>
+      <c r="AGI45" s="0"/>
+      <c r="AGJ45" s="0"/>
+      <c r="AGK45" s="0"/>
+      <c r="AGL45" s="0"/>
+      <c r="AGM45" s="0"/>
+      <c r="AGN45" s="0"/>
+      <c r="AGO45" s="0"/>
+      <c r="AGP45" s="0"/>
+      <c r="AGQ45" s="0"/>
+      <c r="AGR45" s="0"/>
+      <c r="AGS45" s="0"/>
+      <c r="AGT45" s="0"/>
+      <c r="AGU45" s="0"/>
+      <c r="AGV45" s="0"/>
+      <c r="AGW45" s="0"/>
+      <c r="AGX45" s="0"/>
+      <c r="AGY45" s="0"/>
+      <c r="AGZ45" s="0"/>
+      <c r="AHA45" s="0"/>
+      <c r="AHB45" s="0"/>
+      <c r="AHC45" s="0"/>
+      <c r="AHD45" s="0"/>
+      <c r="AHE45" s="0"/>
+      <c r="AHF45" s="0"/>
+      <c r="AHG45" s="0"/>
+      <c r="AHH45" s="0"/>
+      <c r="AHI45" s="0"/>
+      <c r="AHJ45" s="0"/>
+      <c r="AHK45" s="0"/>
+      <c r="AHL45" s="0"/>
+      <c r="AHM45" s="0"/>
+      <c r="AHN45" s="0"/>
+      <c r="AHO45" s="0"/>
+      <c r="AHP45" s="0"/>
+      <c r="AHQ45" s="0"/>
+      <c r="AHR45" s="0"/>
+      <c r="AHS45" s="0"/>
+      <c r="AHT45" s="0"/>
+      <c r="AHU45" s="0"/>
+      <c r="AHV45" s="0"/>
+      <c r="AHW45" s="0"/>
+      <c r="AHX45" s="0"/>
+      <c r="AHY45" s="0"/>
+      <c r="AHZ45" s="0"/>
+      <c r="AIA45" s="0"/>
+      <c r="AIB45" s="0"/>
+      <c r="AIC45" s="0"/>
+      <c r="AID45" s="0"/>
+      <c r="AIE45" s="0"/>
+      <c r="AIF45" s="0"/>
+      <c r="AIG45" s="0"/>
+      <c r="AIH45" s="0"/>
+      <c r="AII45" s="0"/>
+      <c r="AIJ45" s="0"/>
+      <c r="AIK45" s="0"/>
+      <c r="AIL45" s="0"/>
+      <c r="AIM45" s="0"/>
+      <c r="AIN45" s="0"/>
+      <c r="AIO45" s="0"/>
+      <c r="AIP45" s="0"/>
+      <c r="AIQ45" s="0"/>
+      <c r="AIR45" s="0"/>
+      <c r="AIS45" s="0"/>
+      <c r="AIT45" s="0"/>
+      <c r="AIU45" s="0"/>
+      <c r="AIV45" s="0"/>
+      <c r="AIW45" s="0"/>
+      <c r="AIX45" s="0"/>
+      <c r="AIY45" s="0"/>
+      <c r="AIZ45" s="0"/>
+      <c r="AJA45" s="0"/>
+      <c r="AJB45" s="0"/>
+      <c r="AJC45" s="0"/>
+      <c r="AJD45" s="0"/>
+      <c r="AJE45" s="0"/>
+      <c r="AJF45" s="0"/>
+      <c r="AJG45" s="0"/>
+      <c r="AJH45" s="0"/>
+      <c r="AJI45" s="0"/>
+      <c r="AJJ45" s="0"/>
+      <c r="AJK45" s="0"/>
+      <c r="AJL45" s="0"/>
+      <c r="AJM45" s="0"/>
+      <c r="AJN45" s="0"/>
+      <c r="AJO45" s="0"/>
+      <c r="AJP45" s="0"/>
+      <c r="AJQ45" s="0"/>
+      <c r="AJR45" s="0"/>
+      <c r="AJS45" s="0"/>
+      <c r="AJT45" s="0"/>
+      <c r="AJU45" s="0"/>
+      <c r="AJV45" s="0"/>
+      <c r="AJW45" s="0"/>
+      <c r="AJX45" s="0"/>
+      <c r="AJY45" s="0"/>
+      <c r="AJZ45" s="0"/>
+      <c r="AKA45" s="0"/>
+      <c r="AKB45" s="0"/>
+      <c r="AKC45" s="0"/>
+      <c r="AKD45" s="0"/>
+      <c r="AKE45" s="0"/>
+      <c r="AKF45" s="0"/>
+      <c r="AKG45" s="0"/>
+      <c r="AKH45" s="0"/>
+      <c r="AKI45" s="0"/>
+      <c r="AKJ45" s="0"/>
+      <c r="AKK45" s="0"/>
+      <c r="AKL45" s="0"/>
+      <c r="AKM45" s="0"/>
+      <c r="AKN45" s="0"/>
+      <c r="AKO45" s="0"/>
+      <c r="AKP45" s="0"/>
+      <c r="AKQ45" s="0"/>
+      <c r="AKR45" s="0"/>
+      <c r="AKS45" s="0"/>
+      <c r="AKT45" s="0"/>
+      <c r="AKU45" s="0"/>
+      <c r="AKV45" s="0"/>
+      <c r="AKW45" s="0"/>
+      <c r="AKX45" s="0"/>
+      <c r="AKY45" s="0"/>
+      <c r="AKZ45" s="0"/>
+      <c r="ALA45" s="0"/>
+      <c r="ALB45" s="0"/>
+      <c r="ALC45" s="0"/>
+      <c r="ALD45" s="0"/>
+      <c r="ALE45" s="0"/>
+      <c r="ALF45" s="0"/>
+      <c r="ALG45" s="0"/>
+      <c r="ALH45" s="0"/>
+      <c r="ALI45" s="0"/>
+      <c r="ALJ45" s="0"/>
+      <c r="ALK45" s="0"/>
+      <c r="ALL45" s="0"/>
+      <c r="ALM45" s="0"/>
+      <c r="ALN45" s="0"/>
+      <c r="ALO45" s="0"/>
+      <c r="ALP45" s="0"/>
+      <c r="ALQ45" s="0"/>
+      <c r="ALR45" s="0"/>
+      <c r="ALS45" s="0"/>
+      <c r="ALT45" s="0"/>
+      <c r="ALU45" s="0"/>
+      <c r="ALV45" s="0"/>
+      <c r="ALW45" s="0"/>
+      <c r="ALX45" s="0"/>
+      <c r="ALY45" s="0"/>
+      <c r="ALZ45" s="0"/>
+      <c r="AMA45" s="0"/>
+      <c r="AMB45" s="0"/>
+      <c r="AMC45" s="0"/>
+      <c r="AMD45" s="0"/>
+      <c r="AME45" s="0"/>
+      <c r="AMF45" s="0"/>
+      <c r="AMG45" s="0"/>
+      <c r="AMH45" s="0"/>
+      <c r="AMI45" s="0"/>
+      <c r="AMJ45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="E46" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="J46" s="0"/>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
+      <c r="M46" s="0"/>
+      <c r="N46" s="0"/>
+      <c r="O46" s="0"/>
+      <c r="P46" s="0"/>
+      <c r="Q46" s="0"/>
+      <c r="R46" s="0"/>
+      <c r="S46" s="0"/>
+      <c r="T46" s="0"/>
+      <c r="U46" s="0"/>
+      <c r="V46" s="0"/>
+      <c r="W46" s="0"/>
+      <c r="X46" s="0"/>
+      <c r="Y46" s="0"/>
+      <c r="Z46" s="0"/>
+      <c r="AA46" s="0"/>
+      <c r="AB46" s="0"/>
+      <c r="AC46" s="0"/>
+      <c r="AD46" s="0"/>
+      <c r="AE46" s="0"/>
+      <c r="AF46" s="0"/>
+      <c r="AG46" s="0"/>
+      <c r="AH46" s="0"/>
+      <c r="AI46" s="0"/>
+      <c r="AJ46" s="0"/>
+      <c r="AK46" s="0"/>
+      <c r="AL46" s="0"/>
+      <c r="AM46" s="0"/>
+      <c r="AN46" s="0"/>
+      <c r="AO46" s="0"/>
+      <c r="AP46" s="0"/>
+      <c r="AQ46" s="0"/>
+      <c r="AR46" s="0"/>
+      <c r="AS46" s="0"/>
+      <c r="AT46" s="0"/>
+      <c r="AU46" s="0"/>
+      <c r="AV46" s="0"/>
+      <c r="AW46" s="0"/>
+      <c r="AX46" s="0"/>
+      <c r="AY46" s="0"/>
+      <c r="AZ46" s="0"/>
+      <c r="BA46" s="0"/>
+      <c r="BB46" s="0"/>
+      <c r="BC46" s="0"/>
+      <c r="BD46" s="0"/>
+      <c r="BE46" s="0"/>
+      <c r="BF46" s="0"/>
+      <c r="BG46" s="0"/>
+      <c r="BH46" s="0"/>
+      <c r="BI46" s="0"/>
+      <c r="BJ46" s="0"/>
+      <c r="BK46" s="0"/>
+      <c r="BL46" s="0"/>
+      <c r="BM46" s="0"/>
+      <c r="BN46" s="0"/>
+      <c r="BO46" s="0"/>
+      <c r="BP46" s="0"/>
+      <c r="BQ46" s="0"/>
+      <c r="BR46" s="0"/>
+      <c r="BS46" s="0"/>
+      <c r="BT46" s="0"/>
+      <c r="BU46" s="0"/>
+      <c r="BV46" s="0"/>
+      <c r="BW46" s="0"/>
+      <c r="BX46" s="0"/>
+      <c r="BY46" s="0"/>
+      <c r="BZ46" s="0"/>
+      <c r="CA46" s="0"/>
+      <c r="CB46" s="0"/>
+      <c r="CC46" s="0"/>
+      <c r="CD46" s="0"/>
+      <c r="CE46" s="0"/>
+      <c r="CF46" s="0"/>
+      <c r="CG46" s="0"/>
+      <c r="CH46" s="0"/>
+      <c r="CI46" s="0"/>
+      <c r="CJ46" s="0"/>
+      <c r="CK46" s="0"/>
+      <c r="CL46" s="0"/>
+      <c r="CM46" s="0"/>
+      <c r="CN46" s="0"/>
+      <c r="CO46" s="0"/>
+      <c r="CP46" s="0"/>
+      <c r="CQ46" s="0"/>
+      <c r="CR46" s="0"/>
+      <c r="CS46" s="0"/>
+      <c r="CT46" s="0"/>
+      <c r="CU46" s="0"/>
+      <c r="CV46" s="0"/>
+      <c r="CW46" s="0"/>
+      <c r="CX46" s="0"/>
+      <c r="CY46" s="0"/>
+      <c r="CZ46" s="0"/>
+      <c r="DA46" s="0"/>
+      <c r="DB46" s="0"/>
+      <c r="DC46" s="0"/>
+      <c r="DD46" s="0"/>
+      <c r="DE46" s="0"/>
+      <c r="DF46" s="0"/>
+      <c r="DG46" s="0"/>
+      <c r="DH46" s="0"/>
+      <c r="DI46" s="0"/>
+      <c r="DJ46" s="0"/>
+      <c r="DK46" s="0"/>
+      <c r="DL46" s="0"/>
+      <c r="DM46" s="0"/>
+      <c r="DN46" s="0"/>
+      <c r="DO46" s="0"/>
+      <c r="DP46" s="0"/>
+      <c r="DQ46" s="0"/>
+      <c r="DR46" s="0"/>
+      <c r="DS46" s="0"/>
+      <c r="DT46" s="0"/>
+      <c r="DU46" s="0"/>
+      <c r="DV46" s="0"/>
+      <c r="DW46" s="0"/>
+      <c r="DX46" s="0"/>
+      <c r="DY46" s="0"/>
+      <c r="DZ46" s="0"/>
+      <c r="EA46" s="0"/>
+      <c r="EB46" s="0"/>
+      <c r="EC46" s="0"/>
+      <c r="ED46" s="0"/>
+      <c r="EE46" s="0"/>
+      <c r="EF46" s="0"/>
+      <c r="EG46" s="0"/>
+      <c r="EH46" s="0"/>
+      <c r="EI46" s="0"/>
+      <c r="EJ46" s="0"/>
+      <c r="EK46" s="0"/>
+      <c r="EL46" s="0"/>
+      <c r="EM46" s="0"/>
+      <c r="EN46" s="0"/>
+      <c r="EO46" s="0"/>
+      <c r="EP46" s="0"/>
+      <c r="EQ46" s="0"/>
+      <c r="ER46" s="0"/>
+      <c r="ES46" s="0"/>
+      <c r="ET46" s="0"/>
+      <c r="EU46" s="0"/>
+      <c r="EV46" s="0"/>
+      <c r="EW46" s="0"/>
+      <c r="EX46" s="0"/>
+      <c r="EY46" s="0"/>
+      <c r="EZ46" s="0"/>
+      <c r="FA46" s="0"/>
+      <c r="FB46" s="0"/>
+      <c r="FC46" s="0"/>
+      <c r="FD46" s="0"/>
+      <c r="FE46" s="0"/>
+      <c r="FF46" s="0"/>
+      <c r="FG46" s="0"/>
+      <c r="FH46" s="0"/>
+      <c r="FI46" s="0"/>
+      <c r="FJ46" s="0"/>
+      <c r="FK46" s="0"/>
+      <c r="FL46" s="0"/>
+      <c r="FM46" s="0"/>
+      <c r="FN46" s="0"/>
+      <c r="FO46" s="0"/>
+      <c r="FP46" s="0"/>
+      <c r="FQ46" s="0"/>
+      <c r="FR46" s="0"/>
+      <c r="FS46" s="0"/>
+      <c r="FT46" s="0"/>
+      <c r="FU46" s="0"/>
+      <c r="FV46" s="0"/>
+      <c r="FW46" s="0"/>
+      <c r="FX46" s="0"/>
+      <c r="FY46" s="0"/>
+      <c r="FZ46" s="0"/>
+      <c r="GA46" s="0"/>
+      <c r="GB46" s="0"/>
+      <c r="GC46" s="0"/>
+      <c r="GD46" s="0"/>
+      <c r="GE46" s="0"/>
+      <c r="GF46" s="0"/>
+      <c r="GG46" s="0"/>
+      <c r="GH46" s="0"/>
+      <c r="GI46" s="0"/>
+      <c r="GJ46" s="0"/>
+      <c r="GK46" s="0"/>
+      <c r="GL46" s="0"/>
+      <c r="GM46" s="0"/>
+      <c r="GN46" s="0"/>
+      <c r="GO46" s="0"/>
+      <c r="GP46" s="0"/>
+      <c r="GQ46" s="0"/>
+      <c r="GR46" s="0"/>
+      <c r="GS46" s="0"/>
+      <c r="GT46" s="0"/>
+      <c r="GU46" s="0"/>
+      <c r="GV46" s="0"/>
+      <c r="GW46" s="0"/>
+      <c r="GX46" s="0"/>
+      <c r="GY46" s="0"/>
+      <c r="GZ46" s="0"/>
+      <c r="HA46" s="0"/>
+      <c r="HB46" s="0"/>
+      <c r="HC46" s="0"/>
+      <c r="HD46" s="0"/>
+      <c r="HE46" s="0"/>
+      <c r="HF46" s="0"/>
+      <c r="HG46" s="0"/>
+      <c r="HH46" s="0"/>
+      <c r="HI46" s="0"/>
+      <c r="HJ46" s="0"/>
+      <c r="HK46" s="0"/>
+      <c r="HL46" s="0"/>
+      <c r="HM46" s="0"/>
+      <c r="HN46" s="0"/>
+      <c r="HO46" s="0"/>
+      <c r="HP46" s="0"/>
+      <c r="HQ46" s="0"/>
+      <c r="HR46" s="0"/>
+      <c r="HS46" s="0"/>
+      <c r="HT46" s="0"/>
+      <c r="HU46" s="0"/>
+      <c r="HV46" s="0"/>
+      <c r="HW46" s="0"/>
+      <c r="HX46" s="0"/>
+      <c r="HY46" s="0"/>
+      <c r="HZ46" s="0"/>
+      <c r="IA46" s="0"/>
+      <c r="IB46" s="0"/>
+      <c r="IC46" s="0"/>
+      <c r="ID46" s="0"/>
+      <c r="IE46" s="0"/>
+      <c r="IF46" s="0"/>
+      <c r="IG46" s="0"/>
+      <c r="IH46" s="0"/>
+      <c r="II46" s="0"/>
+      <c r="IJ46" s="0"/>
+      <c r="IK46" s="0"/>
+      <c r="IL46" s="0"/>
+      <c r="IM46" s="0"/>
+      <c r="IN46" s="0"/>
+      <c r="IO46" s="0"/>
+      <c r="IP46" s="0"/>
+      <c r="IQ46" s="0"/>
+      <c r="IR46" s="0"/>
+      <c r="IS46" s="0"/>
+      <c r="IT46" s="0"/>
+      <c r="IU46" s="0"/>
+      <c r="IV46" s="0"/>
+      <c r="IW46" s="0"/>
+      <c r="IX46" s="0"/>
+      <c r="IY46" s="0"/>
+      <c r="IZ46" s="0"/>
+      <c r="JA46" s="0"/>
+      <c r="JB46" s="0"/>
+      <c r="JC46" s="0"/>
+      <c r="JD46" s="0"/>
+      <c r="JE46" s="0"/>
+      <c r="JF46" s="0"/>
+      <c r="JG46" s="0"/>
+      <c r="JH46" s="0"/>
+      <c r="JI46" s="0"/>
+      <c r="JJ46" s="0"/>
+      <c r="JK46" s="0"/>
+      <c r="JL46" s="0"/>
+      <c r="JM46" s="0"/>
+      <c r="JN46" s="0"/>
+      <c r="JO46" s="0"/>
+      <c r="JP46" s="0"/>
+      <c r="JQ46" s="0"/>
+      <c r="JR46" s="0"/>
+      <c r="JS46" s="0"/>
+      <c r="JT46" s="0"/>
+      <c r="JU46" s="0"/>
+      <c r="JV46" s="0"/>
+      <c r="JW46" s="0"/>
+      <c r="JX46" s="0"/>
+      <c r="JY46" s="0"/>
+      <c r="JZ46" s="0"/>
+      <c r="KA46" s="0"/>
+      <c r="KB46" s="0"/>
+      <c r="KC46" s="0"/>
+      <c r="KD46" s="0"/>
+      <c r="KE46" s="0"/>
+      <c r="KF46" s="0"/>
+      <c r="KG46" s="0"/>
+      <c r="KH46" s="0"/>
+      <c r="KI46" s="0"/>
+      <c r="KJ46" s="0"/>
+      <c r="KK46" s="0"/>
+      <c r="KL46" s="0"/>
+      <c r="KM46" s="0"/>
+      <c r="KN46" s="0"/>
+      <c r="KO46" s="0"/>
+      <c r="KP46" s="0"/>
+      <c r="KQ46" s="0"/>
+      <c r="KR46" s="0"/>
+      <c r="KS46" s="0"/>
+      <c r="KT46" s="0"/>
+      <c r="KU46" s="0"/>
+      <c r="KV46" s="0"/>
+      <c r="KW46" s="0"/>
+      <c r="KX46" s="0"/>
+      <c r="KY46" s="0"/>
+      <c r="KZ46" s="0"/>
+      <c r="LA46" s="0"/>
+      <c r="LB46" s="0"/>
+      <c r="LC46" s="0"/>
+      <c r="LD46" s="0"/>
+      <c r="LE46" s="0"/>
+      <c r="LF46" s="0"/>
+      <c r="LG46" s="0"/>
+      <c r="LH46" s="0"/>
+      <c r="LI46" s="0"/>
+      <c r="LJ46" s="0"/>
+      <c r="LK46" s="0"/>
+      <c r="LL46" s="0"/>
+      <c r="LM46" s="0"/>
+      <c r="LN46" s="0"/>
+      <c r="LO46" s="0"/>
+      <c r="LP46" s="0"/>
+      <c r="LQ46" s="0"/>
+      <c r="LR46" s="0"/>
+      <c r="LS46" s="0"/>
+      <c r="LT46" s="0"/>
+      <c r="LU46" s="0"/>
+      <c r="LV46" s="0"/>
+      <c r="LW46" s="0"/>
+      <c r="LX46" s="0"/>
+      <c r="LY46" s="0"/>
+      <c r="LZ46" s="0"/>
+      <c r="MA46" s="0"/>
+      <c r="MB46" s="0"/>
+      <c r="MC46" s="0"/>
+      <c r="MD46" s="0"/>
+      <c r="ME46" s="0"/>
+      <c r="MF46" s="0"/>
+      <c r="MG46" s="0"/>
+      <c r="MH46" s="0"/>
+      <c r="MI46" s="0"/>
+      <c r="MJ46" s="0"/>
+      <c r="MK46" s="0"/>
+      <c r="ML46" s="0"/>
+      <c r="MM46" s="0"/>
+      <c r="MN46" s="0"/>
+      <c r="MO46" s="0"/>
+      <c r="MP46" s="0"/>
+      <c r="MQ46" s="0"/>
+      <c r="MR46" s="0"/>
+      <c r="MS46" s="0"/>
+      <c r="MT46" s="0"/>
+      <c r="MU46" s="0"/>
+      <c r="MV46" s="0"/>
+      <c r="MW46" s="0"/>
+      <c r="MX46" s="0"/>
+      <c r="MY46" s="0"/>
+      <c r="MZ46" s="0"/>
+      <c r="NA46" s="0"/>
+      <c r="NB46" s="0"/>
+      <c r="NC46" s="0"/>
+      <c r="ND46" s="0"/>
+      <c r="NE46" s="0"/>
+      <c r="NF46" s="0"/>
+      <c r="NG46" s="0"/>
+      <c r="NH46" s="0"/>
+      <c r="NI46" s="0"/>
+      <c r="NJ46" s="0"/>
+      <c r="NK46" s="0"/>
+      <c r="NL46" s="0"/>
+      <c r="NM46" s="0"/>
+      <c r="NN46" s="0"/>
+      <c r="NO46" s="0"/>
+      <c r="NP46" s="0"/>
+      <c r="NQ46" s="0"/>
+      <c r="NR46" s="0"/>
+      <c r="NS46" s="0"/>
+      <c r="NT46" s="0"/>
+      <c r="NU46" s="0"/>
+      <c r="NV46" s="0"/>
+      <c r="NW46" s="0"/>
+      <c r="NX46" s="0"/>
+      <c r="NY46" s="0"/>
+      <c r="NZ46" s="0"/>
+      <c r="OA46" s="0"/>
+      <c r="OB46" s="0"/>
+      <c r="OC46" s="0"/>
+      <c r="OD46" s="0"/>
+      <c r="OE46" s="0"/>
+      <c r="OF46" s="0"/>
+      <c r="OG46" s="0"/>
+      <c r="OH46" s="0"/>
+      <c r="OI46" s="0"/>
+      <c r="OJ46" s="0"/>
+      <c r="OK46" s="0"/>
+      <c r="OL46" s="0"/>
+      <c r="OM46" s="0"/>
+      <c r="ON46" s="0"/>
+      <c r="OO46" s="0"/>
+      <c r="OP46" s="0"/>
+      <c r="OQ46" s="0"/>
+      <c r="OR46" s="0"/>
+      <c r="OS46" s="0"/>
+      <c r="OT46" s="0"/>
+      <c r="OU46" s="0"/>
+      <c r="OV46" s="0"/>
+      <c r="OW46" s="0"/>
+      <c r="OX46" s="0"/>
+      <c r="OY46" s="0"/>
+      <c r="OZ46" s="0"/>
+      <c r="PA46" s="0"/>
+      <c r="PB46" s="0"/>
+      <c r="PC46" s="0"/>
+      <c r="PD46" s="0"/>
+      <c r="PE46" s="0"/>
+      <c r="PF46" s="0"/>
+      <c r="PG46" s="0"/>
+      <c r="PH46" s="0"/>
+      <c r="PI46" s="0"/>
+      <c r="PJ46" s="0"/>
+      <c r="PK46" s="0"/>
+      <c r="PL46" s="0"/>
+      <c r="PM46" s="0"/>
+      <c r="PN46" s="0"/>
+      <c r="PO46" s="0"/>
+      <c r="PP46" s="0"/>
+      <c r="PQ46" s="0"/>
+      <c r="PR46" s="0"/>
+      <c r="PS46" s="0"/>
+      <c r="PT46" s="0"/>
+      <c r="PU46" s="0"/>
+      <c r="PV46" s="0"/>
+      <c r="PW46" s="0"/>
+      <c r="PX46" s="0"/>
+      <c r="PY46" s="0"/>
+      <c r="PZ46" s="0"/>
+      <c r="QA46" s="0"/>
+      <c r="QB46" s="0"/>
+      <c r="QC46" s="0"/>
+      <c r="QD46" s="0"/>
+      <c r="QE46" s="0"/>
+      <c r="QF46" s="0"/>
+      <c r="QG46" s="0"/>
+      <c r="QH46" s="0"/>
+      <c r="QI46" s="0"/>
+      <c r="QJ46" s="0"/>
+      <c r="QK46" s="0"/>
+      <c r="QL46" s="0"/>
+      <c r="QM46" s="0"/>
+      <c r="QN46" s="0"/>
+      <c r="QO46" s="0"/>
+      <c r="QP46" s="0"/>
+      <c r="QQ46" s="0"/>
+      <c r="QR46" s="0"/>
+      <c r="QS46" s="0"/>
+      <c r="QT46" s="0"/>
+      <c r="QU46" s="0"/>
+      <c r="QV46" s="0"/>
+      <c r="QW46" s="0"/>
+      <c r="QX46" s="0"/>
+      <c r="QY46" s="0"/>
+      <c r="QZ46" s="0"/>
+      <c r="RA46" s="0"/>
+      <c r="RB46" s="0"/>
+      <c r="RC46" s="0"/>
+      <c r="RD46" s="0"/>
+      <c r="RE46" s="0"/>
+      <c r="RF46" s="0"/>
+      <c r="RG46" s="0"/>
+      <c r="RH46" s="0"/>
+      <c r="RI46" s="0"/>
+      <c r="RJ46" s="0"/>
+      <c r="RK46" s="0"/>
+      <c r="RL46" s="0"/>
+      <c r="RM46" s="0"/>
+      <c r="RN46" s="0"/>
+      <c r="RO46" s="0"/>
+      <c r="RP46" s="0"/>
+      <c r="RQ46" s="0"/>
+      <c r="RR46" s="0"/>
+      <c r="RS46" s="0"/>
+      <c r="RT46" s="0"/>
+      <c r="RU46" s="0"/>
+      <c r="RV46" s="0"/>
+      <c r="RW46" s="0"/>
+      <c r="RX46" s="0"/>
+      <c r="RY46" s="0"/>
+      <c r="RZ46" s="0"/>
+      <c r="SA46" s="0"/>
+      <c r="SB46" s="0"/>
+      <c r="SC46" s="0"/>
+      <c r="SD46" s="0"/>
+      <c r="SE46" s="0"/>
+      <c r="SF46" s="0"/>
+      <c r="SG46" s="0"/>
+      <c r="SH46" s="0"/>
+      <c r="SI46" s="0"/>
+      <c r="SJ46" s="0"/>
+      <c r="SK46" s="0"/>
+      <c r="SL46" s="0"/>
+      <c r="SM46" s="0"/>
+      <c r="SN46" s="0"/>
+      <c r="SO46" s="0"/>
+      <c r="SP46" s="0"/>
+      <c r="SQ46" s="0"/>
+      <c r="SR46" s="0"/>
+      <c r="SS46" s="0"/>
+      <c r="ST46" s="0"/>
+      <c r="SU46" s="0"/>
+      <c r="SV46" s="0"/>
+      <c r="SW46" s="0"/>
+      <c r="SX46" s="0"/>
+      <c r="SY46" s="0"/>
+      <c r="SZ46" s="0"/>
+      <c r="TA46" s="0"/>
+      <c r="TB46" s="0"/>
+      <c r="TC46" s="0"/>
+      <c r="TD46" s="0"/>
+      <c r="TE46" s="0"/>
+      <c r="TF46" s="0"/>
+      <c r="TG46" s="0"/>
+      <c r="TH46" s="0"/>
+      <c r="TI46" s="0"/>
+      <c r="TJ46" s="0"/>
+      <c r="TK46" s="0"/>
+      <c r="TL46" s="0"/>
+      <c r="TM46" s="0"/>
+      <c r="TN46" s="0"/>
+      <c r="TO46" s="0"/>
+      <c r="TP46" s="0"/>
+      <c r="TQ46" s="0"/>
+      <c r="TR46" s="0"/>
+      <c r="TS46" s="0"/>
+      <c r="TT46" s="0"/>
+      <c r="TU46" s="0"/>
+      <c r="TV46" s="0"/>
+      <c r="TW46" s="0"/>
+      <c r="TX46" s="0"/>
+      <c r="TY46" s="0"/>
+      <c r="TZ46" s="0"/>
+      <c r="UA46" s="0"/>
+      <c r="UB46" s="0"/>
+      <c r="UC46" s="0"/>
+      <c r="UD46" s="0"/>
+      <c r="UE46" s="0"/>
+      <c r="UF46" s="0"/>
+      <c r="UG46" s="0"/>
+      <c r="UH46" s="0"/>
+      <c r="UI46" s="0"/>
+      <c r="UJ46" s="0"/>
+      <c r="UK46" s="0"/>
+      <c r="UL46" s="0"/>
+      <c r="UM46" s="0"/>
+      <c r="UN46" s="0"/>
+      <c r="UO46" s="0"/>
+      <c r="UP46" s="0"/>
+      <c r="UQ46" s="0"/>
+      <c r="UR46" s="0"/>
+      <c r="US46" s="0"/>
+      <c r="UT46" s="0"/>
+      <c r="UU46" s="0"/>
+      <c r="UV46" s="0"/>
+      <c r="UW46" s="0"/>
+      <c r="UX46" s="0"/>
+      <c r="UY46" s="0"/>
+      <c r="UZ46" s="0"/>
+      <c r="VA46" s="0"/>
+      <c r="VB46" s="0"/>
+      <c r="VC46" s="0"/>
+      <c r="VD46" s="0"/>
+      <c r="VE46" s="0"/>
+      <c r="VF46" s="0"/>
+      <c r="VG46" s="0"/>
+      <c r="VH46" s="0"/>
+      <c r="VI46" s="0"/>
+      <c r="VJ46" s="0"/>
+      <c r="VK46" s="0"/>
+      <c r="VL46" s="0"/>
+      <c r="VM46" s="0"/>
+      <c r="VN46" s="0"/>
+      <c r="VO46" s="0"/>
+      <c r="VP46" s="0"/>
+      <c r="VQ46" s="0"/>
+      <c r="VR46" s="0"/>
+      <c r="VS46" s="0"/>
+      <c r="VT46" s="0"/>
+      <c r="VU46" s="0"/>
+      <c r="VV46" s="0"/>
+      <c r="VW46" s="0"/>
+      <c r="VX46" s="0"/>
+      <c r="VY46" s="0"/>
+      <c r="VZ46" s="0"/>
+      <c r="WA46" s="0"/>
+      <c r="WB46" s="0"/>
+      <c r="WC46" s="0"/>
+      <c r="WD46" s="0"/>
+      <c r="WE46" s="0"/>
+      <c r="WF46" s="0"/>
+      <c r="WG46" s="0"/>
+      <c r="WH46" s="0"/>
+      <c r="WI46" s="0"/>
+      <c r="WJ46" s="0"/>
+      <c r="WK46" s="0"/>
+      <c r="WL46" s="0"/>
+      <c r="WM46" s="0"/>
+      <c r="WN46" s="0"/>
+      <c r="WO46" s="0"/>
+      <c r="WP46" s="0"/>
+      <c r="WQ46" s="0"/>
+      <c r="WR46" s="0"/>
+      <c r="WS46" s="0"/>
+      <c r="WT46" s="0"/>
+      <c r="WU46" s="0"/>
+      <c r="WV46" s="0"/>
+      <c r="WW46" s="0"/>
+      <c r="WX46" s="0"/>
+      <c r="WY46" s="0"/>
+      <c r="WZ46" s="0"/>
+      <c r="XA46" s="0"/>
+      <c r="XB46" s="0"/>
+      <c r="XC46" s="0"/>
+      <c r="XD46" s="0"/>
+      <c r="XE46" s="0"/>
+      <c r="XF46" s="0"/>
+      <c r="XG46" s="0"/>
+      <c r="XH46" s="0"/>
+      <c r="XI46" s="0"/>
+      <c r="XJ46" s="0"/>
+      <c r="XK46" s="0"/>
+      <c r="XL46" s="0"/>
+      <c r="XM46" s="0"/>
+      <c r="XN46" s="0"/>
+      <c r="XO46" s="0"/>
+      <c r="XP46" s="0"/>
+      <c r="XQ46" s="0"/>
+      <c r="XR46" s="0"/>
+      <c r="XS46" s="0"/>
+      <c r="XT46" s="0"/>
+      <c r="XU46" s="0"/>
+      <c r="XV46" s="0"/>
+      <c r="XW46" s="0"/>
+      <c r="XX46" s="0"/>
+      <c r="XY46" s="0"/>
+      <c r="XZ46" s="0"/>
+      <c r="YA46" s="0"/>
+      <c r="YB46" s="0"/>
+      <c r="YC46" s="0"/>
+      <c r="YD46" s="0"/>
+      <c r="YE46" s="0"/>
+      <c r="YF46" s="0"/>
+      <c r="YG46" s="0"/>
+      <c r="YH46" s="0"/>
+      <c r="YI46" s="0"/>
+      <c r="YJ46" s="0"/>
+      <c r="YK46" s="0"/>
+      <c r="YL46" s="0"/>
+      <c r="YM46" s="0"/>
+      <c r="YN46" s="0"/>
+      <c r="YO46" s="0"/>
+      <c r="YP46" s="0"/>
+      <c r="YQ46" s="0"/>
+      <c r="YR46" s="0"/>
+      <c r="YS46" s="0"/>
+      <c r="YT46" s="0"/>
+      <c r="YU46" s="0"/>
+      <c r="YV46" s="0"/>
+      <c r="YW46" s="0"/>
+      <c r="YX46" s="0"/>
+      <c r="YY46" s="0"/>
+      <c r="YZ46" s="0"/>
+      <c r="ZA46" s="0"/>
+      <c r="ZB46" s="0"/>
+      <c r="ZC46" s="0"/>
+      <c r="ZD46" s="0"/>
+      <c r="ZE46" s="0"/>
+      <c r="ZF46" s="0"/>
+      <c r="ZG46" s="0"/>
+      <c r="ZH46" s="0"/>
+      <c r="ZI46" s="0"/>
+      <c r="ZJ46" s="0"/>
+      <c r="ZK46" s="0"/>
+      <c r="ZL46" s="0"/>
+      <c r="ZM46" s="0"/>
+      <c r="ZN46" s="0"/>
+      <c r="ZO46" s="0"/>
+      <c r="ZP46" s="0"/>
+      <c r="ZQ46" s="0"/>
+      <c r="ZR46" s="0"/>
+      <c r="ZS46" s="0"/>
+      <c r="ZT46" s="0"/>
+      <c r="ZU46" s="0"/>
+      <c r="ZV46" s="0"/>
+      <c r="ZW46" s="0"/>
+      <c r="ZX46" s="0"/>
+      <c r="ZY46" s="0"/>
+      <c r="ZZ46" s="0"/>
+      <c r="AAA46" s="0"/>
+      <c r="AAB46" s="0"/>
+      <c r="AAC46" s="0"/>
+      <c r="AAD46" s="0"/>
+      <c r="AAE46" s="0"/>
+      <c r="AAF46" s="0"/>
+      <c r="AAG46" s="0"/>
+      <c r="AAH46" s="0"/>
+      <c r="AAI46" s="0"/>
+      <c r="AAJ46" s="0"/>
+      <c r="AAK46" s="0"/>
+      <c r="AAL46" s="0"/>
+      <c r="AAM46" s="0"/>
+      <c r="AAN46" s="0"/>
+      <c r="AAO46" s="0"/>
+      <c r="AAP46" s="0"/>
+      <c r="AAQ46" s="0"/>
+      <c r="AAR46" s="0"/>
+      <c r="AAS46" s="0"/>
+      <c r="AAT46" s="0"/>
+      <c r="AAU46" s="0"/>
+      <c r="AAV46" s="0"/>
+      <c r="AAW46" s="0"/>
+      <c r="AAX46" s="0"/>
+      <c r="AAY46" s="0"/>
+      <c r="AAZ46" s="0"/>
+      <c r="ABA46" s="0"/>
+      <c r="ABB46" s="0"/>
+      <c r="ABC46" s="0"/>
+      <c r="ABD46" s="0"/>
+      <c r="ABE46" s="0"/>
+      <c r="ABF46" s="0"/>
+      <c r="ABG46" s="0"/>
+      <c r="ABH46" s="0"/>
+      <c r="ABI46" s="0"/>
+      <c r="ABJ46" s="0"/>
+      <c r="ABK46" s="0"/>
+      <c r="ABL46" s="0"/>
+      <c r="ABM46" s="0"/>
+      <c r="ABN46" s="0"/>
+      <c r="ABO46" s="0"/>
+      <c r="ABP46" s="0"/>
+      <c r="ABQ46" s="0"/>
+      <c r="ABR46" s="0"/>
+      <c r="ABS46" s="0"/>
+      <c r="ABT46" s="0"/>
+      <c r="ABU46" s="0"/>
+      <c r="ABV46" s="0"/>
+      <c r="ABW46" s="0"/>
+      <c r="ABX46" s="0"/>
+      <c r="ABY46" s="0"/>
+      <c r="ABZ46" s="0"/>
+      <c r="ACA46" s="0"/>
+      <c r="ACB46" s="0"/>
+      <c r="ACC46" s="0"/>
+      <c r="ACD46" s="0"/>
+      <c r="ACE46" s="0"/>
+      <c r="ACF46" s="0"/>
+      <c r="ACG46" s="0"/>
+      <c r="ACH46" s="0"/>
+      <c r="ACI46" s="0"/>
+      <c r="ACJ46" s="0"/>
+      <c r="ACK46" s="0"/>
+      <c r="ACL46" s="0"/>
+      <c r="ACM46" s="0"/>
+      <c r="ACN46" s="0"/>
+      <c r="ACO46" s="0"/>
+      <c r="ACP46" s="0"/>
+      <c r="ACQ46" s="0"/>
+      <c r="ACR46" s="0"/>
+      <c r="ACS46" s="0"/>
+      <c r="ACT46" s="0"/>
+      <c r="ACU46" s="0"/>
+      <c r="ACV46" s="0"/>
+      <c r="ACW46" s="0"/>
+      <c r="ACX46" s="0"/>
+      <c r="ACY46" s="0"/>
+      <c r="ACZ46" s="0"/>
+      <c r="ADA46" s="0"/>
+      <c r="ADB46" s="0"/>
+      <c r="ADC46" s="0"/>
+      <c r="ADD46" s="0"/>
+      <c r="ADE46" s="0"/>
+      <c r="ADF46" s="0"/>
+      <c r="ADG46" s="0"/>
+      <c r="ADH46" s="0"/>
+      <c r="ADI46" s="0"/>
+      <c r="ADJ46" s="0"/>
+      <c r="ADK46" s="0"/>
+      <c r="ADL46" s="0"/>
+      <c r="ADM46" s="0"/>
+      <c r="ADN46" s="0"/>
+      <c r="ADO46" s="0"/>
+      <c r="ADP46" s="0"/>
+      <c r="ADQ46" s="0"/>
+      <c r="ADR46" s="0"/>
+      <c r="ADS46" s="0"/>
+      <c r="ADT46" s="0"/>
+      <c r="ADU46" s="0"/>
+      <c r="ADV46" s="0"/>
+      <c r="ADW46" s="0"/>
+      <c r="ADX46" s="0"/>
+      <c r="ADY46" s="0"/>
+      <c r="ADZ46" s="0"/>
+      <c r="AEA46" s="0"/>
+      <c r="AEB46" s="0"/>
+      <c r="AEC46" s="0"/>
+      <c r="AED46" s="0"/>
+      <c r="AEE46" s="0"/>
+      <c r="AEF46" s="0"/>
+      <c r="AEG46" s="0"/>
+      <c r="AEH46" s="0"/>
+      <c r="AEI46" s="0"/>
+      <c r="AEJ46" s="0"/>
+      <c r="AEK46" s="0"/>
+      <c r="AEL46" s="0"/>
+      <c r="AEM46" s="0"/>
+      <c r="AEN46" s="0"/>
+      <c r="AEO46" s="0"/>
+      <c r="AEP46" s="0"/>
+      <c r="AEQ46" s="0"/>
+      <c r="AER46" s="0"/>
+      <c r="AES46" s="0"/>
+      <c r="AET46" s="0"/>
+      <c r="AEU46" s="0"/>
+      <c r="AEV46" s="0"/>
+      <c r="AEW46" s="0"/>
+      <c r="AEX46" s="0"/>
+      <c r="AEY46" s="0"/>
+      <c r="AEZ46" s="0"/>
+      <c r="AFA46" s="0"/>
+      <c r="AFB46" s="0"/>
+      <c r="AFC46" s="0"/>
+      <c r="AFD46" s="0"/>
+      <c r="AFE46" s="0"/>
+      <c r="AFF46" s="0"/>
+      <c r="AFG46" s="0"/>
+      <c r="AFH46" s="0"/>
+      <c r="AFI46" s="0"/>
+      <c r="AFJ46" s="0"/>
+      <c r="AFK46" s="0"/>
+      <c r="AFL46" s="0"/>
+      <c r="AFM46" s="0"/>
+      <c r="AFN46" s="0"/>
+      <c r="AFO46" s="0"/>
+      <c r="AFP46" s="0"/>
+      <c r="AFQ46" s="0"/>
+      <c r="AFR46" s="0"/>
+      <c r="AFS46" s="0"/>
+      <c r="AFT46" s="0"/>
+      <c r="AFU46" s="0"/>
+      <c r="AFV46" s="0"/>
+      <c r="AFW46" s="0"/>
+      <c r="AFX46" s="0"/>
+      <c r="AFY46" s="0"/>
+      <c r="AFZ46" s="0"/>
+      <c r="AGA46" s="0"/>
+      <c r="AGB46" s="0"/>
+      <c r="AGC46" s="0"/>
+      <c r="AGD46" s="0"/>
+      <c r="AGE46" s="0"/>
+      <c r="AGF46" s="0"/>
+      <c r="AGG46" s="0"/>
+      <c r="AGH46" s="0"/>
+      <c r="AGI46" s="0"/>
+      <c r="AGJ46" s="0"/>
+      <c r="AGK46" s="0"/>
+      <c r="AGL46" s="0"/>
+      <c r="AGM46" s="0"/>
+      <c r="AGN46" s="0"/>
+      <c r="AGO46" s="0"/>
+      <c r="AGP46" s="0"/>
+      <c r="AGQ46" s="0"/>
+      <c r="AGR46" s="0"/>
+      <c r="AGS46" s="0"/>
+      <c r="AGT46" s="0"/>
+      <c r="AGU46" s="0"/>
+      <c r="AGV46" s="0"/>
+      <c r="AGW46" s="0"/>
+      <c r="AGX46" s="0"/>
+      <c r="AGY46" s="0"/>
+      <c r="AGZ46" s="0"/>
+      <c r="AHA46" s="0"/>
+      <c r="AHB46" s="0"/>
+      <c r="AHC46" s="0"/>
+      <c r="AHD46" s="0"/>
+      <c r="AHE46" s="0"/>
+      <c r="AHF46" s="0"/>
+      <c r="AHG46" s="0"/>
+      <c r="AHH46" s="0"/>
+      <c r="AHI46" s="0"/>
+      <c r="AHJ46" s="0"/>
+      <c r="AHK46" s="0"/>
+      <c r="AHL46" s="0"/>
+      <c r="AHM46" s="0"/>
+      <c r="AHN46" s="0"/>
+      <c r="AHO46" s="0"/>
+      <c r="AHP46" s="0"/>
+      <c r="AHQ46" s="0"/>
+      <c r="AHR46" s="0"/>
+      <c r="AHS46" s="0"/>
+      <c r="AHT46" s="0"/>
+      <c r="AHU46" s="0"/>
+      <c r="AHV46" s="0"/>
+      <c r="AHW46" s="0"/>
+      <c r="AHX46" s="0"/>
+      <c r="AHY46" s="0"/>
+      <c r="AHZ46" s="0"/>
+      <c r="AIA46" s="0"/>
+      <c r="AIB46" s="0"/>
+      <c r="AIC46" s="0"/>
+      <c r="AID46" s="0"/>
+      <c r="AIE46" s="0"/>
+      <c r="AIF46" s="0"/>
+      <c r="AIG46" s="0"/>
+      <c r="AIH46" s="0"/>
+      <c r="AII46" s="0"/>
+      <c r="AIJ46" s="0"/>
+      <c r="AIK46" s="0"/>
+      <c r="AIL46" s="0"/>
+      <c r="AIM46" s="0"/>
+      <c r="AIN46" s="0"/>
+      <c r="AIO46" s="0"/>
+      <c r="AIP46" s="0"/>
+      <c r="AIQ46" s="0"/>
+      <c r="AIR46" s="0"/>
+      <c r="AIS46" s="0"/>
+      <c r="AIT46" s="0"/>
+      <c r="AIU46" s="0"/>
+      <c r="AIV46" s="0"/>
+      <c r="AIW46" s="0"/>
+      <c r="AIX46" s="0"/>
+      <c r="AIY46" s="0"/>
+      <c r="AIZ46" s="0"/>
+      <c r="AJA46" s="0"/>
+      <c r="AJB46" s="0"/>
+      <c r="AJC46" s="0"/>
+      <c r="AJD46" s="0"/>
+      <c r="AJE46" s="0"/>
+      <c r="AJF46" s="0"/>
+      <c r="AJG46" s="0"/>
+      <c r="AJH46" s="0"/>
+      <c r="AJI46" s="0"/>
+      <c r="AJJ46" s="0"/>
+      <c r="AJK46" s="0"/>
+      <c r="AJL46" s="0"/>
+      <c r="AJM46" s="0"/>
+      <c r="AJN46" s="0"/>
+      <c r="AJO46" s="0"/>
+      <c r="AJP46" s="0"/>
+      <c r="AJQ46" s="0"/>
+      <c r="AJR46" s="0"/>
+      <c r="AJS46" s="0"/>
+      <c r="AJT46" s="0"/>
+      <c r="AJU46" s="0"/>
+      <c r="AJV46" s="0"/>
+      <c r="AJW46" s="0"/>
+      <c r="AJX46" s="0"/>
+      <c r="AJY46" s="0"/>
+      <c r="AJZ46" s="0"/>
+      <c r="AKA46" s="0"/>
+      <c r="AKB46" s="0"/>
+      <c r="AKC46" s="0"/>
+      <c r="AKD46" s="0"/>
+      <c r="AKE46" s="0"/>
+      <c r="AKF46" s="0"/>
+      <c r="AKG46" s="0"/>
+      <c r="AKH46" s="0"/>
+      <c r="AKI46" s="0"/>
+      <c r="AKJ46" s="0"/>
+      <c r="AKK46" s="0"/>
+      <c r="AKL46" s="0"/>
+      <c r="AKM46" s="0"/>
+      <c r="AKN46" s="0"/>
+      <c r="AKO46" s="0"/>
+      <c r="AKP46" s="0"/>
+      <c r="AKQ46" s="0"/>
+      <c r="AKR46" s="0"/>
+      <c r="AKS46" s="0"/>
+      <c r="AKT46" s="0"/>
+      <c r="AKU46" s="0"/>
+      <c r="AKV46" s="0"/>
+      <c r="AKW46" s="0"/>
+      <c r="AKX46" s="0"/>
+      <c r="AKY46" s="0"/>
+      <c r="AKZ46" s="0"/>
+      <c r="ALA46" s="0"/>
+      <c r="ALB46" s="0"/>
+      <c r="ALC46" s="0"/>
+      <c r="ALD46" s="0"/>
+      <c r="ALE46" s="0"/>
+      <c r="ALF46" s="0"/>
+      <c r="ALG46" s="0"/>
+      <c r="ALH46" s="0"/>
+      <c r="ALI46" s="0"/>
+      <c r="ALJ46" s="0"/>
+      <c r="ALK46" s="0"/>
+      <c r="ALL46" s="0"/>
+      <c r="ALM46" s="0"/>
+      <c r="ALN46" s="0"/>
+      <c r="ALO46" s="0"/>
+      <c r="ALP46" s="0"/>
+      <c r="ALQ46" s="0"/>
+      <c r="ALR46" s="0"/>
+      <c r="ALS46" s="0"/>
+      <c r="ALT46" s="0"/>
+      <c r="ALU46" s="0"/>
+      <c r="ALV46" s="0"/>
+      <c r="ALW46" s="0"/>
+      <c r="ALX46" s="0"/>
+      <c r="ALY46" s="0"/>
+      <c r="ALZ46" s="0"/>
+      <c r="AMA46" s="0"/>
+      <c r="AMB46" s="0"/>
+      <c r="AMC46" s="0"/>
+      <c r="AMD46" s="0"/>
+      <c r="AME46" s="0"/>
+      <c r="AMF46" s="0"/>
+      <c r="AMG46" s="0"/>
+      <c r="AMH46" s="0"/>
+      <c r="AMI46" s="0"/>
+      <c r="AMJ46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="1" t="s">
-        <v>116</v>
+      <c r="A47" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B48" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B49" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F50" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5389,6 +7582,8 @@
     <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:H36"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
ajout de version mobile de l image de presentation
</commit_message>
<xml_diff>
--- a/Maquette-Sources/Modèle-audit-SEO.xlsx
+++ b/Maquette-Sources/Modèle-audit-SEO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="161">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -467,6 +467,45 @@
   </si>
   <si>
     <t xml:space="preserve">taille du container non défini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO ? W3C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la valeur constant génère une erreur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contant n’existe pas en css</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bugherd.com/blog/why-we-need-localized-css-constants/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min-device-width et max-device-width sont déprécié</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la dépréciation est le fait qu’il ne soit plus recommandé de les utiliser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il est préférable d’utiliser car il n’est pas sur que les navigateurs les reconnaissent encore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/CSS/@media/device-width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speak:none n’est pas reconnu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speak a été modifié lors du passage à CSS3. Dorénavant ses valeur sont:auto / never always</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il faut remplacer la valeur de speak dans ce cas par never</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.css-faciles.com/liste-proprietes/speak.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/TR/css-speech-1/#speaking-props-speak</t>
   </si>
 </sst>
 </file>
@@ -778,9 +817,9 @@
   <dimension ref="A1:AMJ1006"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="F57" activeCellId="0" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6637,9 +6676,66 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
mise en auto de la hauteur du logo
</commit_message>
<xml_diff>
--- a/Maquette-Sources/Modèle-audit-SEO.xlsx
+++ b/Maquette-Sources/Modèle-audit-SEO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="168">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -388,6 +388,18 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
+    <t xml:space="preserve">les scripts sont mal placés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les bonnes pratiques de programmation veulent que les scripts soient placés juste avant la fermeture du body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il faut déplacer les scripts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://waytolearnx.com/2019/06/10-bonnes-pratiques-de-codage-en-javascript.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Page 2</t>
   </si>
   <si>
@@ -506,6 +518,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.w3.org/TR/css-speech-1/#speaking-props-speak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la page appelle des fichier css et js qui n’existent pas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">il y a des erreurs dans le nom des fichiers (.min a été ajouté)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il faut corriger le nom des fichiers</t>
   </si>
 </sst>
 </file>
@@ -814,12 +835,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1006"/>
+  <dimension ref="A1:AMJ1008"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F57" activeCellId="0" sqref="F57"/>
+      <selection pane="bottomLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5524,1077 +5545,2083 @@
       <c r="AMJ45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E46" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="H46" s="0"/>
-      <c r="I46" s="0"/>
-      <c r="J46" s="0"/>
-      <c r="K46" s="0"/>
-      <c r="L46" s="0"/>
-      <c r="M46" s="0"/>
-      <c r="N46" s="0"/>
-      <c r="O46" s="0"/>
-      <c r="P46" s="0"/>
-      <c r="Q46" s="0"/>
-      <c r="R46" s="0"/>
-      <c r="S46" s="0"/>
-      <c r="T46" s="0"/>
-      <c r="U46" s="0"/>
-      <c r="V46" s="0"/>
-      <c r="W46" s="0"/>
-      <c r="X46" s="0"/>
-      <c r="Y46" s="0"/>
-      <c r="Z46" s="0"/>
-      <c r="AA46" s="0"/>
-      <c r="AB46" s="0"/>
-      <c r="AC46" s="0"/>
-      <c r="AD46" s="0"/>
-      <c r="AE46" s="0"/>
-      <c r="AF46" s="0"/>
-      <c r="AG46" s="0"/>
-      <c r="AH46" s="0"/>
-      <c r="AI46" s="0"/>
-      <c r="AJ46" s="0"/>
-      <c r="AK46" s="0"/>
-      <c r="AL46" s="0"/>
-      <c r="AM46" s="0"/>
-      <c r="AN46" s="0"/>
-      <c r="AO46" s="0"/>
-      <c r="AP46" s="0"/>
-      <c r="AQ46" s="0"/>
-      <c r="AR46" s="0"/>
-      <c r="AS46" s="0"/>
-      <c r="AT46" s="0"/>
-      <c r="AU46" s="0"/>
-      <c r="AV46" s="0"/>
-      <c r="AW46" s="0"/>
-      <c r="AX46" s="0"/>
-      <c r="AY46" s="0"/>
-      <c r="AZ46" s="0"/>
-      <c r="BA46" s="0"/>
-      <c r="BB46" s="0"/>
-      <c r="BC46" s="0"/>
-      <c r="BD46" s="0"/>
-      <c r="BE46" s="0"/>
-      <c r="BF46" s="0"/>
-      <c r="BG46" s="0"/>
-      <c r="BH46" s="0"/>
-      <c r="BI46" s="0"/>
-      <c r="BJ46" s="0"/>
-      <c r="BK46" s="0"/>
-      <c r="BL46" s="0"/>
-      <c r="BM46" s="0"/>
-      <c r="BN46" s="0"/>
-      <c r="BO46" s="0"/>
-      <c r="BP46" s="0"/>
-      <c r="BQ46" s="0"/>
-      <c r="BR46" s="0"/>
-      <c r="BS46" s="0"/>
-      <c r="BT46" s="0"/>
-      <c r="BU46" s="0"/>
-      <c r="BV46" s="0"/>
-      <c r="BW46" s="0"/>
-      <c r="BX46" s="0"/>
-      <c r="BY46" s="0"/>
-      <c r="BZ46" s="0"/>
-      <c r="CA46" s="0"/>
-      <c r="CB46" s="0"/>
-      <c r="CC46" s="0"/>
-      <c r="CD46" s="0"/>
-      <c r="CE46" s="0"/>
-      <c r="CF46" s="0"/>
-      <c r="CG46" s="0"/>
-      <c r="CH46" s="0"/>
-      <c r="CI46" s="0"/>
-      <c r="CJ46" s="0"/>
-      <c r="CK46" s="0"/>
-      <c r="CL46" s="0"/>
-      <c r="CM46" s="0"/>
-      <c r="CN46" s="0"/>
-      <c r="CO46" s="0"/>
-      <c r="CP46" s="0"/>
-      <c r="CQ46" s="0"/>
-      <c r="CR46" s="0"/>
-      <c r="CS46" s="0"/>
-      <c r="CT46" s="0"/>
-      <c r="CU46" s="0"/>
-      <c r="CV46" s="0"/>
-      <c r="CW46" s="0"/>
-      <c r="CX46" s="0"/>
-      <c r="CY46" s="0"/>
-      <c r="CZ46" s="0"/>
-      <c r="DA46" s="0"/>
-      <c r="DB46" s="0"/>
-      <c r="DC46" s="0"/>
-      <c r="DD46" s="0"/>
-      <c r="DE46" s="0"/>
-      <c r="DF46" s="0"/>
-      <c r="DG46" s="0"/>
-      <c r="DH46" s="0"/>
-      <c r="DI46" s="0"/>
-      <c r="DJ46" s="0"/>
-      <c r="DK46" s="0"/>
-      <c r="DL46" s="0"/>
-      <c r="DM46" s="0"/>
-      <c r="DN46" s="0"/>
-      <c r="DO46" s="0"/>
-      <c r="DP46" s="0"/>
-      <c r="DQ46" s="0"/>
-      <c r="DR46" s="0"/>
-      <c r="DS46" s="0"/>
-      <c r="DT46" s="0"/>
-      <c r="DU46" s="0"/>
-      <c r="DV46" s="0"/>
-      <c r="DW46" s="0"/>
-      <c r="DX46" s="0"/>
-      <c r="DY46" s="0"/>
-      <c r="DZ46" s="0"/>
-      <c r="EA46" s="0"/>
-      <c r="EB46" s="0"/>
-      <c r="EC46" s="0"/>
-      <c r="ED46" s="0"/>
-      <c r="EE46" s="0"/>
-      <c r="EF46" s="0"/>
-      <c r="EG46" s="0"/>
-      <c r="EH46" s="0"/>
-      <c r="EI46" s="0"/>
-      <c r="EJ46" s="0"/>
-      <c r="EK46" s="0"/>
-      <c r="EL46" s="0"/>
-      <c r="EM46" s="0"/>
-      <c r="EN46" s="0"/>
-      <c r="EO46" s="0"/>
-      <c r="EP46" s="0"/>
-      <c r="EQ46" s="0"/>
-      <c r="ER46" s="0"/>
-      <c r="ES46" s="0"/>
-      <c r="ET46" s="0"/>
-      <c r="EU46" s="0"/>
-      <c r="EV46" s="0"/>
-      <c r="EW46" s="0"/>
-      <c r="EX46" s="0"/>
-      <c r="EY46" s="0"/>
-      <c r="EZ46" s="0"/>
-      <c r="FA46" s="0"/>
-      <c r="FB46" s="0"/>
-      <c r="FC46" s="0"/>
-      <c r="FD46" s="0"/>
-      <c r="FE46" s="0"/>
-      <c r="FF46" s="0"/>
-      <c r="FG46" s="0"/>
-      <c r="FH46" s="0"/>
-      <c r="FI46" s="0"/>
-      <c r="FJ46" s="0"/>
-      <c r="FK46" s="0"/>
-      <c r="FL46" s="0"/>
-      <c r="FM46" s="0"/>
-      <c r="FN46" s="0"/>
-      <c r="FO46" s="0"/>
-      <c r="FP46" s="0"/>
-      <c r="FQ46" s="0"/>
-      <c r="FR46" s="0"/>
-      <c r="FS46" s="0"/>
-      <c r="FT46" s="0"/>
-      <c r="FU46" s="0"/>
-      <c r="FV46" s="0"/>
-      <c r="FW46" s="0"/>
-      <c r="FX46" s="0"/>
-      <c r="FY46" s="0"/>
-      <c r="FZ46" s="0"/>
-      <c r="GA46" s="0"/>
-      <c r="GB46" s="0"/>
-      <c r="GC46" s="0"/>
-      <c r="GD46" s="0"/>
-      <c r="GE46" s="0"/>
-      <c r="GF46" s="0"/>
-      <c r="GG46" s="0"/>
-      <c r="GH46" s="0"/>
-      <c r="GI46" s="0"/>
-      <c r="GJ46" s="0"/>
-      <c r="GK46" s="0"/>
-      <c r="GL46" s="0"/>
-      <c r="GM46" s="0"/>
-      <c r="GN46" s="0"/>
-      <c r="GO46" s="0"/>
-      <c r="GP46" s="0"/>
-      <c r="GQ46" s="0"/>
-      <c r="GR46" s="0"/>
-      <c r="GS46" s="0"/>
-      <c r="GT46" s="0"/>
-      <c r="GU46" s="0"/>
-      <c r="GV46" s="0"/>
-      <c r="GW46" s="0"/>
-      <c r="GX46" s="0"/>
-      <c r="GY46" s="0"/>
-      <c r="GZ46" s="0"/>
-      <c r="HA46" s="0"/>
-      <c r="HB46" s="0"/>
-      <c r="HC46" s="0"/>
-      <c r="HD46" s="0"/>
-      <c r="HE46" s="0"/>
-      <c r="HF46" s="0"/>
-      <c r="HG46" s="0"/>
-      <c r="HH46" s="0"/>
-      <c r="HI46" s="0"/>
-      <c r="HJ46" s="0"/>
-      <c r="HK46" s="0"/>
-      <c r="HL46" s="0"/>
-      <c r="HM46" s="0"/>
-      <c r="HN46" s="0"/>
-      <c r="HO46" s="0"/>
-      <c r="HP46" s="0"/>
-      <c r="HQ46" s="0"/>
-      <c r="HR46" s="0"/>
-      <c r="HS46" s="0"/>
-      <c r="HT46" s="0"/>
-      <c r="HU46" s="0"/>
-      <c r="HV46" s="0"/>
-      <c r="HW46" s="0"/>
-      <c r="HX46" s="0"/>
-      <c r="HY46" s="0"/>
-      <c r="HZ46" s="0"/>
-      <c r="IA46" s="0"/>
-      <c r="IB46" s="0"/>
-      <c r="IC46" s="0"/>
-      <c r="ID46" s="0"/>
-      <c r="IE46" s="0"/>
-      <c r="IF46" s="0"/>
-      <c r="IG46" s="0"/>
-      <c r="IH46" s="0"/>
-      <c r="II46" s="0"/>
-      <c r="IJ46" s="0"/>
-      <c r="IK46" s="0"/>
-      <c r="IL46" s="0"/>
-      <c r="IM46" s="0"/>
-      <c r="IN46" s="0"/>
-      <c r="IO46" s="0"/>
-      <c r="IP46" s="0"/>
-      <c r="IQ46" s="0"/>
-      <c r="IR46" s="0"/>
-      <c r="IS46" s="0"/>
-      <c r="IT46" s="0"/>
-      <c r="IU46" s="0"/>
-      <c r="IV46" s="0"/>
-      <c r="IW46" s="0"/>
-      <c r="IX46" s="0"/>
-      <c r="IY46" s="0"/>
-      <c r="IZ46" s="0"/>
-      <c r="JA46" s="0"/>
-      <c r="JB46" s="0"/>
-      <c r="JC46" s="0"/>
-      <c r="JD46" s="0"/>
-      <c r="JE46" s="0"/>
-      <c r="JF46" s="0"/>
-      <c r="JG46" s="0"/>
-      <c r="JH46" s="0"/>
-      <c r="JI46" s="0"/>
-      <c r="JJ46" s="0"/>
-      <c r="JK46" s="0"/>
-      <c r="JL46" s="0"/>
-      <c r="JM46" s="0"/>
-      <c r="JN46" s="0"/>
-      <c r="JO46" s="0"/>
-      <c r="JP46" s="0"/>
-      <c r="JQ46" s="0"/>
-      <c r="JR46" s="0"/>
-      <c r="JS46" s="0"/>
-      <c r="JT46" s="0"/>
-      <c r="JU46" s="0"/>
-      <c r="JV46" s="0"/>
-      <c r="JW46" s="0"/>
-      <c r="JX46" s="0"/>
-      <c r="JY46" s="0"/>
-      <c r="JZ46" s="0"/>
-      <c r="KA46" s="0"/>
-      <c r="KB46" s="0"/>
-      <c r="KC46" s="0"/>
-      <c r="KD46" s="0"/>
-      <c r="KE46" s="0"/>
-      <c r="KF46" s="0"/>
-      <c r="KG46" s="0"/>
-      <c r="KH46" s="0"/>
-      <c r="KI46" s="0"/>
-      <c r="KJ46" s="0"/>
-      <c r="KK46" s="0"/>
-      <c r="KL46" s="0"/>
-      <c r="KM46" s="0"/>
-      <c r="KN46" s="0"/>
-      <c r="KO46" s="0"/>
-      <c r="KP46" s="0"/>
-      <c r="KQ46" s="0"/>
-      <c r="KR46" s="0"/>
-      <c r="KS46" s="0"/>
-      <c r="KT46" s="0"/>
-      <c r="KU46" s="0"/>
-      <c r="KV46" s="0"/>
-      <c r="KW46" s="0"/>
-      <c r="KX46" s="0"/>
-      <c r="KY46" s="0"/>
-      <c r="KZ46" s="0"/>
-      <c r="LA46" s="0"/>
-      <c r="LB46" s="0"/>
-      <c r="LC46" s="0"/>
-      <c r="LD46" s="0"/>
-      <c r="LE46" s="0"/>
-      <c r="LF46" s="0"/>
-      <c r="LG46" s="0"/>
-      <c r="LH46" s="0"/>
-      <c r="LI46" s="0"/>
-      <c r="LJ46" s="0"/>
-      <c r="LK46" s="0"/>
-      <c r="LL46" s="0"/>
-      <c r="LM46" s="0"/>
-      <c r="LN46" s="0"/>
-      <c r="LO46" s="0"/>
-      <c r="LP46" s="0"/>
-      <c r="LQ46" s="0"/>
-      <c r="LR46" s="0"/>
-      <c r="LS46" s="0"/>
-      <c r="LT46" s="0"/>
-      <c r="LU46" s="0"/>
-      <c r="LV46" s="0"/>
-      <c r="LW46" s="0"/>
-      <c r="LX46" s="0"/>
-      <c r="LY46" s="0"/>
-      <c r="LZ46" s="0"/>
-      <c r="MA46" s="0"/>
-      <c r="MB46" s="0"/>
-      <c r="MC46" s="0"/>
-      <c r="MD46" s="0"/>
-      <c r="ME46" s="0"/>
-      <c r="MF46" s="0"/>
-      <c r="MG46" s="0"/>
-      <c r="MH46" s="0"/>
-      <c r="MI46" s="0"/>
-      <c r="MJ46" s="0"/>
-      <c r="MK46" s="0"/>
-      <c r="ML46" s="0"/>
-      <c r="MM46" s="0"/>
-      <c r="MN46" s="0"/>
-      <c r="MO46" s="0"/>
-      <c r="MP46" s="0"/>
-      <c r="MQ46" s="0"/>
-      <c r="MR46" s="0"/>
-      <c r="MS46" s="0"/>
-      <c r="MT46" s="0"/>
-      <c r="MU46" s="0"/>
-      <c r="MV46" s="0"/>
-      <c r="MW46" s="0"/>
-      <c r="MX46" s="0"/>
-      <c r="MY46" s="0"/>
-      <c r="MZ46" s="0"/>
-      <c r="NA46" s="0"/>
-      <c r="NB46" s="0"/>
-      <c r="NC46" s="0"/>
-      <c r="ND46" s="0"/>
-      <c r="NE46" s="0"/>
-      <c r="NF46" s="0"/>
-      <c r="NG46" s="0"/>
-      <c r="NH46" s="0"/>
-      <c r="NI46" s="0"/>
-      <c r="NJ46" s="0"/>
-      <c r="NK46" s="0"/>
-      <c r="NL46" s="0"/>
-      <c r="NM46" s="0"/>
-      <c r="NN46" s="0"/>
-      <c r="NO46" s="0"/>
-      <c r="NP46" s="0"/>
-      <c r="NQ46" s="0"/>
-      <c r="NR46" s="0"/>
-      <c r="NS46" s="0"/>
-      <c r="NT46" s="0"/>
-      <c r="NU46" s="0"/>
-      <c r="NV46" s="0"/>
-      <c r="NW46" s="0"/>
-      <c r="NX46" s="0"/>
-      <c r="NY46" s="0"/>
-      <c r="NZ46" s="0"/>
-      <c r="OA46" s="0"/>
-      <c r="OB46" s="0"/>
-      <c r="OC46" s="0"/>
-      <c r="OD46" s="0"/>
-      <c r="OE46" s="0"/>
-      <c r="OF46" s="0"/>
-      <c r="OG46" s="0"/>
-      <c r="OH46" s="0"/>
-      <c r="OI46" s="0"/>
-      <c r="OJ46" s="0"/>
-      <c r="OK46" s="0"/>
-      <c r="OL46" s="0"/>
-      <c r="OM46" s="0"/>
-      <c r="ON46" s="0"/>
-      <c r="OO46" s="0"/>
-      <c r="OP46" s="0"/>
-      <c r="OQ46" s="0"/>
-      <c r="OR46" s="0"/>
-      <c r="OS46" s="0"/>
-      <c r="OT46" s="0"/>
-      <c r="OU46" s="0"/>
-      <c r="OV46" s="0"/>
-      <c r="OW46" s="0"/>
-      <c r="OX46" s="0"/>
-      <c r="OY46" s="0"/>
-      <c r="OZ46" s="0"/>
-      <c r="PA46" s="0"/>
-      <c r="PB46" s="0"/>
-      <c r="PC46" s="0"/>
-      <c r="PD46" s="0"/>
-      <c r="PE46" s="0"/>
-      <c r="PF46" s="0"/>
-      <c r="PG46" s="0"/>
-      <c r="PH46" s="0"/>
-      <c r="PI46" s="0"/>
-      <c r="PJ46" s="0"/>
-      <c r="PK46" s="0"/>
-      <c r="PL46" s="0"/>
-      <c r="PM46" s="0"/>
-      <c r="PN46" s="0"/>
-      <c r="PO46" s="0"/>
-      <c r="PP46" s="0"/>
-      <c r="PQ46" s="0"/>
-      <c r="PR46" s="0"/>
-      <c r="PS46" s="0"/>
-      <c r="PT46" s="0"/>
-      <c r="PU46" s="0"/>
-      <c r="PV46" s="0"/>
-      <c r="PW46" s="0"/>
-      <c r="PX46" s="0"/>
-      <c r="PY46" s="0"/>
-      <c r="PZ46" s="0"/>
-      <c r="QA46" s="0"/>
-      <c r="QB46" s="0"/>
-      <c r="QC46" s="0"/>
-      <c r="QD46" s="0"/>
-      <c r="QE46" s="0"/>
-      <c r="QF46" s="0"/>
-      <c r="QG46" s="0"/>
-      <c r="QH46" s="0"/>
-      <c r="QI46" s="0"/>
-      <c r="QJ46" s="0"/>
-      <c r="QK46" s="0"/>
-      <c r="QL46" s="0"/>
-      <c r="QM46" s="0"/>
-      <c r="QN46" s="0"/>
-      <c r="QO46" s="0"/>
-      <c r="QP46" s="0"/>
-      <c r="QQ46" s="0"/>
-      <c r="QR46" s="0"/>
-      <c r="QS46" s="0"/>
-      <c r="QT46" s="0"/>
-      <c r="QU46" s="0"/>
-      <c r="QV46" s="0"/>
-      <c r="QW46" s="0"/>
-      <c r="QX46" s="0"/>
-      <c r="QY46" s="0"/>
-      <c r="QZ46" s="0"/>
-      <c r="RA46" s="0"/>
-      <c r="RB46" s="0"/>
-      <c r="RC46" s="0"/>
-      <c r="RD46" s="0"/>
-      <c r="RE46" s="0"/>
-      <c r="RF46" s="0"/>
-      <c r="RG46" s="0"/>
-      <c r="RH46" s="0"/>
-      <c r="RI46" s="0"/>
-      <c r="RJ46" s="0"/>
-      <c r="RK46" s="0"/>
-      <c r="RL46" s="0"/>
-      <c r="RM46" s="0"/>
-      <c r="RN46" s="0"/>
-      <c r="RO46" s="0"/>
-      <c r="RP46" s="0"/>
-      <c r="RQ46" s="0"/>
-      <c r="RR46" s="0"/>
-      <c r="RS46" s="0"/>
-      <c r="RT46" s="0"/>
-      <c r="RU46" s="0"/>
-      <c r="RV46" s="0"/>
-      <c r="RW46" s="0"/>
-      <c r="RX46" s="0"/>
-      <c r="RY46" s="0"/>
-      <c r="RZ46" s="0"/>
-      <c r="SA46" s="0"/>
-      <c r="SB46" s="0"/>
-      <c r="SC46" s="0"/>
-      <c r="SD46" s="0"/>
-      <c r="SE46" s="0"/>
-      <c r="SF46" s="0"/>
-      <c r="SG46" s="0"/>
-      <c r="SH46" s="0"/>
-      <c r="SI46" s="0"/>
-      <c r="SJ46" s="0"/>
-      <c r="SK46" s="0"/>
-      <c r="SL46" s="0"/>
-      <c r="SM46" s="0"/>
-      <c r="SN46" s="0"/>
-      <c r="SO46" s="0"/>
-      <c r="SP46" s="0"/>
-      <c r="SQ46" s="0"/>
-      <c r="SR46" s="0"/>
-      <c r="SS46" s="0"/>
-      <c r="ST46" s="0"/>
-      <c r="SU46" s="0"/>
-      <c r="SV46" s="0"/>
-      <c r="SW46" s="0"/>
-      <c r="SX46" s="0"/>
-      <c r="SY46" s="0"/>
-      <c r="SZ46" s="0"/>
-      <c r="TA46" s="0"/>
-      <c r="TB46" s="0"/>
-      <c r="TC46" s="0"/>
-      <c r="TD46" s="0"/>
-      <c r="TE46" s="0"/>
-      <c r="TF46" s="0"/>
-      <c r="TG46" s="0"/>
-      <c r="TH46" s="0"/>
-      <c r="TI46" s="0"/>
-      <c r="TJ46" s="0"/>
-      <c r="TK46" s="0"/>
-      <c r="TL46" s="0"/>
-      <c r="TM46" s="0"/>
-      <c r="TN46" s="0"/>
-      <c r="TO46" s="0"/>
-      <c r="TP46" s="0"/>
-      <c r="TQ46" s="0"/>
-      <c r="TR46" s="0"/>
-      <c r="TS46" s="0"/>
-      <c r="TT46" s="0"/>
-      <c r="TU46" s="0"/>
-      <c r="TV46" s="0"/>
-      <c r="TW46" s="0"/>
-      <c r="TX46" s="0"/>
-      <c r="TY46" s="0"/>
-      <c r="TZ46" s="0"/>
-      <c r="UA46" s="0"/>
-      <c r="UB46" s="0"/>
-      <c r="UC46" s="0"/>
-      <c r="UD46" s="0"/>
-      <c r="UE46" s="0"/>
-      <c r="UF46" s="0"/>
-      <c r="UG46" s="0"/>
-      <c r="UH46" s="0"/>
-      <c r="UI46" s="0"/>
-      <c r="UJ46" s="0"/>
-      <c r="UK46" s="0"/>
-      <c r="UL46" s="0"/>
-      <c r="UM46" s="0"/>
-      <c r="UN46" s="0"/>
-      <c r="UO46" s="0"/>
-      <c r="UP46" s="0"/>
-      <c r="UQ46" s="0"/>
-      <c r="UR46" s="0"/>
-      <c r="US46" s="0"/>
-      <c r="UT46" s="0"/>
-      <c r="UU46" s="0"/>
-      <c r="UV46" s="0"/>
-      <c r="UW46" s="0"/>
-      <c r="UX46" s="0"/>
-      <c r="UY46" s="0"/>
-      <c r="UZ46" s="0"/>
-      <c r="VA46" s="0"/>
-      <c r="VB46" s="0"/>
-      <c r="VC46" s="0"/>
-      <c r="VD46" s="0"/>
-      <c r="VE46" s="0"/>
-      <c r="VF46" s="0"/>
-      <c r="VG46" s="0"/>
-      <c r="VH46" s="0"/>
-      <c r="VI46" s="0"/>
-      <c r="VJ46" s="0"/>
-      <c r="VK46" s="0"/>
-      <c r="VL46" s="0"/>
-      <c r="VM46" s="0"/>
-      <c r="VN46" s="0"/>
-      <c r="VO46" s="0"/>
-      <c r="VP46" s="0"/>
-      <c r="VQ46" s="0"/>
-      <c r="VR46" s="0"/>
-      <c r="VS46" s="0"/>
-      <c r="VT46" s="0"/>
-      <c r="VU46" s="0"/>
-      <c r="VV46" s="0"/>
-      <c r="VW46" s="0"/>
-      <c r="VX46" s="0"/>
-      <c r="VY46" s="0"/>
-      <c r="VZ46" s="0"/>
-      <c r="WA46" s="0"/>
-      <c r="WB46" s="0"/>
-      <c r="WC46" s="0"/>
-      <c r="WD46" s="0"/>
-      <c r="WE46" s="0"/>
-      <c r="WF46" s="0"/>
-      <c r="WG46" s="0"/>
-      <c r="WH46" s="0"/>
-      <c r="WI46" s="0"/>
-      <c r="WJ46" s="0"/>
-      <c r="WK46" s="0"/>
-      <c r="WL46" s="0"/>
-      <c r="WM46" s="0"/>
-      <c r="WN46" s="0"/>
-      <c r="WO46" s="0"/>
-      <c r="WP46" s="0"/>
-      <c r="WQ46" s="0"/>
-      <c r="WR46" s="0"/>
-      <c r="WS46" s="0"/>
-      <c r="WT46" s="0"/>
-      <c r="WU46" s="0"/>
-      <c r="WV46" s="0"/>
-      <c r="WW46" s="0"/>
-      <c r="WX46" s="0"/>
-      <c r="WY46" s="0"/>
-      <c r="WZ46" s="0"/>
-      <c r="XA46" s="0"/>
-      <c r="XB46" s="0"/>
-      <c r="XC46" s="0"/>
-      <c r="XD46" s="0"/>
-      <c r="XE46" s="0"/>
-      <c r="XF46" s="0"/>
-      <c r="XG46" s="0"/>
-      <c r="XH46" s="0"/>
-      <c r="XI46" s="0"/>
-      <c r="XJ46" s="0"/>
-      <c r="XK46" s="0"/>
-      <c r="XL46" s="0"/>
-      <c r="XM46" s="0"/>
-      <c r="XN46" s="0"/>
-      <c r="XO46" s="0"/>
-      <c r="XP46" s="0"/>
-      <c r="XQ46" s="0"/>
-      <c r="XR46" s="0"/>
-      <c r="XS46" s="0"/>
-      <c r="XT46" s="0"/>
-      <c r="XU46" s="0"/>
-      <c r="XV46" s="0"/>
-      <c r="XW46" s="0"/>
-      <c r="XX46" s="0"/>
-      <c r="XY46" s="0"/>
-      <c r="XZ46" s="0"/>
-      <c r="YA46" s="0"/>
-      <c r="YB46" s="0"/>
-      <c r="YC46" s="0"/>
-      <c r="YD46" s="0"/>
-      <c r="YE46" s="0"/>
-      <c r="YF46" s="0"/>
-      <c r="YG46" s="0"/>
-      <c r="YH46" s="0"/>
-      <c r="YI46" s="0"/>
-      <c r="YJ46" s="0"/>
-      <c r="YK46" s="0"/>
-      <c r="YL46" s="0"/>
-      <c r="YM46" s="0"/>
-      <c r="YN46" s="0"/>
-      <c r="YO46" s="0"/>
-      <c r="YP46" s="0"/>
-      <c r="YQ46" s="0"/>
-      <c r="YR46" s="0"/>
-      <c r="YS46" s="0"/>
-      <c r="YT46" s="0"/>
-      <c r="YU46" s="0"/>
-      <c r="YV46" s="0"/>
-      <c r="YW46" s="0"/>
-      <c r="YX46" s="0"/>
-      <c r="YY46" s="0"/>
-      <c r="YZ46" s="0"/>
-      <c r="ZA46" s="0"/>
-      <c r="ZB46" s="0"/>
-      <c r="ZC46" s="0"/>
-      <c r="ZD46" s="0"/>
-      <c r="ZE46" s="0"/>
-      <c r="ZF46" s="0"/>
-      <c r="ZG46" s="0"/>
-      <c r="ZH46" s="0"/>
-      <c r="ZI46" s="0"/>
-      <c r="ZJ46" s="0"/>
-      <c r="ZK46" s="0"/>
-      <c r="ZL46" s="0"/>
-      <c r="ZM46" s="0"/>
-      <c r="ZN46" s="0"/>
-      <c r="ZO46" s="0"/>
-      <c r="ZP46" s="0"/>
-      <c r="ZQ46" s="0"/>
-      <c r="ZR46" s="0"/>
-      <c r="ZS46" s="0"/>
-      <c r="ZT46" s="0"/>
-      <c r="ZU46" s="0"/>
-      <c r="ZV46" s="0"/>
-      <c r="ZW46" s="0"/>
-      <c r="ZX46" s="0"/>
-      <c r="ZY46" s="0"/>
-      <c r="ZZ46" s="0"/>
-      <c r="AAA46" s="0"/>
-      <c r="AAB46" s="0"/>
-      <c r="AAC46" s="0"/>
-      <c r="AAD46" s="0"/>
-      <c r="AAE46" s="0"/>
-      <c r="AAF46" s="0"/>
-      <c r="AAG46" s="0"/>
-      <c r="AAH46" s="0"/>
-      <c r="AAI46" s="0"/>
-      <c r="AAJ46" s="0"/>
-      <c r="AAK46" s="0"/>
-      <c r="AAL46" s="0"/>
-      <c r="AAM46" s="0"/>
-      <c r="AAN46" s="0"/>
-      <c r="AAO46" s="0"/>
-      <c r="AAP46" s="0"/>
-      <c r="AAQ46" s="0"/>
-      <c r="AAR46" s="0"/>
-      <c r="AAS46" s="0"/>
-      <c r="AAT46" s="0"/>
-      <c r="AAU46" s="0"/>
-      <c r="AAV46" s="0"/>
-      <c r="AAW46" s="0"/>
-      <c r="AAX46" s="0"/>
-      <c r="AAY46" s="0"/>
-      <c r="AAZ46" s="0"/>
-      <c r="ABA46" s="0"/>
-      <c r="ABB46" s="0"/>
-      <c r="ABC46" s="0"/>
-      <c r="ABD46" s="0"/>
-      <c r="ABE46" s="0"/>
-      <c r="ABF46" s="0"/>
-      <c r="ABG46" s="0"/>
-      <c r="ABH46" s="0"/>
-      <c r="ABI46" s="0"/>
-      <c r="ABJ46" s="0"/>
-      <c r="ABK46" s="0"/>
-      <c r="ABL46" s="0"/>
-      <c r="ABM46" s="0"/>
-      <c r="ABN46" s="0"/>
-      <c r="ABO46" s="0"/>
-      <c r="ABP46" s="0"/>
-      <c r="ABQ46" s="0"/>
-      <c r="ABR46" s="0"/>
-      <c r="ABS46" s="0"/>
-      <c r="ABT46" s="0"/>
-      <c r="ABU46" s="0"/>
-      <c r="ABV46" s="0"/>
-      <c r="ABW46" s="0"/>
-      <c r="ABX46" s="0"/>
-      <c r="ABY46" s="0"/>
-      <c r="ABZ46" s="0"/>
-      <c r="ACA46" s="0"/>
-      <c r="ACB46" s="0"/>
-      <c r="ACC46" s="0"/>
-      <c r="ACD46" s="0"/>
-      <c r="ACE46" s="0"/>
-      <c r="ACF46" s="0"/>
-      <c r="ACG46" s="0"/>
-      <c r="ACH46" s="0"/>
-      <c r="ACI46" s="0"/>
-      <c r="ACJ46" s="0"/>
-      <c r="ACK46" s="0"/>
-      <c r="ACL46" s="0"/>
-      <c r="ACM46" s="0"/>
-      <c r="ACN46" s="0"/>
-      <c r="ACO46" s="0"/>
-      <c r="ACP46" s="0"/>
-      <c r="ACQ46" s="0"/>
-      <c r="ACR46" s="0"/>
-      <c r="ACS46" s="0"/>
-      <c r="ACT46" s="0"/>
-      <c r="ACU46" s="0"/>
-      <c r="ACV46" s="0"/>
-      <c r="ACW46" s="0"/>
-      <c r="ACX46" s="0"/>
-      <c r="ACY46" s="0"/>
-      <c r="ACZ46" s="0"/>
-      <c r="ADA46" s="0"/>
-      <c r="ADB46" s="0"/>
-      <c r="ADC46" s="0"/>
-      <c r="ADD46" s="0"/>
-      <c r="ADE46" s="0"/>
-      <c r="ADF46" s="0"/>
-      <c r="ADG46" s="0"/>
-      <c r="ADH46" s="0"/>
-      <c r="ADI46" s="0"/>
-      <c r="ADJ46" s="0"/>
-      <c r="ADK46" s="0"/>
-      <c r="ADL46" s="0"/>
-      <c r="ADM46" s="0"/>
-      <c r="ADN46" s="0"/>
-      <c r="ADO46" s="0"/>
-      <c r="ADP46" s="0"/>
-      <c r="ADQ46" s="0"/>
-      <c r="ADR46" s="0"/>
-      <c r="ADS46" s="0"/>
-      <c r="ADT46" s="0"/>
-      <c r="ADU46" s="0"/>
-      <c r="ADV46" s="0"/>
-      <c r="ADW46" s="0"/>
-      <c r="ADX46" s="0"/>
-      <c r="ADY46" s="0"/>
-      <c r="ADZ46" s="0"/>
-      <c r="AEA46" s="0"/>
-      <c r="AEB46" s="0"/>
-      <c r="AEC46" s="0"/>
-      <c r="AED46" s="0"/>
-      <c r="AEE46" s="0"/>
-      <c r="AEF46" s="0"/>
-      <c r="AEG46" s="0"/>
-      <c r="AEH46" s="0"/>
-      <c r="AEI46" s="0"/>
-      <c r="AEJ46" s="0"/>
-      <c r="AEK46" s="0"/>
-      <c r="AEL46" s="0"/>
-      <c r="AEM46" s="0"/>
-      <c r="AEN46" s="0"/>
-      <c r="AEO46" s="0"/>
-      <c r="AEP46" s="0"/>
-      <c r="AEQ46" s="0"/>
-      <c r="AER46" s="0"/>
-      <c r="AES46" s="0"/>
-      <c r="AET46" s="0"/>
-      <c r="AEU46" s="0"/>
-      <c r="AEV46" s="0"/>
-      <c r="AEW46" s="0"/>
-      <c r="AEX46" s="0"/>
-      <c r="AEY46" s="0"/>
-      <c r="AEZ46" s="0"/>
-      <c r="AFA46" s="0"/>
-      <c r="AFB46" s="0"/>
-      <c r="AFC46" s="0"/>
-      <c r="AFD46" s="0"/>
-      <c r="AFE46" s="0"/>
-      <c r="AFF46" s="0"/>
-      <c r="AFG46" s="0"/>
-      <c r="AFH46" s="0"/>
-      <c r="AFI46" s="0"/>
-      <c r="AFJ46" s="0"/>
-      <c r="AFK46" s="0"/>
-      <c r="AFL46" s="0"/>
-      <c r="AFM46" s="0"/>
-      <c r="AFN46" s="0"/>
-      <c r="AFO46" s="0"/>
-      <c r="AFP46" s="0"/>
-      <c r="AFQ46" s="0"/>
-      <c r="AFR46" s="0"/>
-      <c r="AFS46" s="0"/>
-      <c r="AFT46" s="0"/>
-      <c r="AFU46" s="0"/>
-      <c r="AFV46" s="0"/>
-      <c r="AFW46" s="0"/>
-      <c r="AFX46" s="0"/>
-      <c r="AFY46" s="0"/>
-      <c r="AFZ46" s="0"/>
-      <c r="AGA46" s="0"/>
-      <c r="AGB46" s="0"/>
-      <c r="AGC46" s="0"/>
-      <c r="AGD46" s="0"/>
-      <c r="AGE46" s="0"/>
-      <c r="AGF46" s="0"/>
-      <c r="AGG46" s="0"/>
-      <c r="AGH46" s="0"/>
-      <c r="AGI46" s="0"/>
-      <c r="AGJ46" s="0"/>
-      <c r="AGK46" s="0"/>
-      <c r="AGL46" s="0"/>
-      <c r="AGM46" s="0"/>
-      <c r="AGN46" s="0"/>
-      <c r="AGO46" s="0"/>
-      <c r="AGP46" s="0"/>
-      <c r="AGQ46" s="0"/>
-      <c r="AGR46" s="0"/>
-      <c r="AGS46" s="0"/>
-      <c r="AGT46" s="0"/>
-      <c r="AGU46" s="0"/>
-      <c r="AGV46" s="0"/>
-      <c r="AGW46" s="0"/>
-      <c r="AGX46" s="0"/>
-      <c r="AGY46" s="0"/>
-      <c r="AGZ46" s="0"/>
-      <c r="AHA46" s="0"/>
-      <c r="AHB46" s="0"/>
-      <c r="AHC46" s="0"/>
-      <c r="AHD46" s="0"/>
-      <c r="AHE46" s="0"/>
-      <c r="AHF46" s="0"/>
-      <c r="AHG46" s="0"/>
-      <c r="AHH46" s="0"/>
-      <c r="AHI46" s="0"/>
-      <c r="AHJ46" s="0"/>
-      <c r="AHK46" s="0"/>
-      <c r="AHL46" s="0"/>
-      <c r="AHM46" s="0"/>
-      <c r="AHN46" s="0"/>
-      <c r="AHO46" s="0"/>
-      <c r="AHP46" s="0"/>
-      <c r="AHQ46" s="0"/>
-      <c r="AHR46" s="0"/>
-      <c r="AHS46" s="0"/>
-      <c r="AHT46" s="0"/>
-      <c r="AHU46" s="0"/>
-      <c r="AHV46" s="0"/>
-      <c r="AHW46" s="0"/>
-      <c r="AHX46" s="0"/>
-      <c r="AHY46" s="0"/>
-      <c r="AHZ46" s="0"/>
-      <c r="AIA46" s="0"/>
-      <c r="AIB46" s="0"/>
-      <c r="AIC46" s="0"/>
-      <c r="AID46" s="0"/>
-      <c r="AIE46" s="0"/>
-      <c r="AIF46" s="0"/>
-      <c r="AIG46" s="0"/>
-      <c r="AIH46" s="0"/>
-      <c r="AII46" s="0"/>
-      <c r="AIJ46" s="0"/>
-      <c r="AIK46" s="0"/>
-      <c r="AIL46" s="0"/>
-      <c r="AIM46" s="0"/>
-      <c r="AIN46" s="0"/>
-      <c r="AIO46" s="0"/>
-      <c r="AIP46" s="0"/>
-      <c r="AIQ46" s="0"/>
-      <c r="AIR46" s="0"/>
-      <c r="AIS46" s="0"/>
-      <c r="AIT46" s="0"/>
-      <c r="AIU46" s="0"/>
-      <c r="AIV46" s="0"/>
-      <c r="AIW46" s="0"/>
-      <c r="AIX46" s="0"/>
-      <c r="AIY46" s="0"/>
-      <c r="AIZ46" s="0"/>
-      <c r="AJA46" s="0"/>
-      <c r="AJB46" s="0"/>
-      <c r="AJC46" s="0"/>
-      <c r="AJD46" s="0"/>
-      <c r="AJE46" s="0"/>
-      <c r="AJF46" s="0"/>
-      <c r="AJG46" s="0"/>
-      <c r="AJH46" s="0"/>
-      <c r="AJI46" s="0"/>
-      <c r="AJJ46" s="0"/>
-      <c r="AJK46" s="0"/>
-      <c r="AJL46" s="0"/>
-      <c r="AJM46" s="0"/>
-      <c r="AJN46" s="0"/>
-      <c r="AJO46" s="0"/>
-      <c r="AJP46" s="0"/>
-      <c r="AJQ46" s="0"/>
-      <c r="AJR46" s="0"/>
-      <c r="AJS46" s="0"/>
-      <c r="AJT46" s="0"/>
-      <c r="AJU46" s="0"/>
-      <c r="AJV46" s="0"/>
-      <c r="AJW46" s="0"/>
-      <c r="AJX46" s="0"/>
-      <c r="AJY46" s="0"/>
-      <c r="AJZ46" s="0"/>
-      <c r="AKA46" s="0"/>
-      <c r="AKB46" s="0"/>
-      <c r="AKC46" s="0"/>
-      <c r="AKD46" s="0"/>
-      <c r="AKE46" s="0"/>
-      <c r="AKF46" s="0"/>
-      <c r="AKG46" s="0"/>
-      <c r="AKH46" s="0"/>
-      <c r="AKI46" s="0"/>
-      <c r="AKJ46" s="0"/>
-      <c r="AKK46" s="0"/>
-      <c r="AKL46" s="0"/>
-      <c r="AKM46" s="0"/>
-      <c r="AKN46" s="0"/>
-      <c r="AKO46" s="0"/>
-      <c r="AKP46" s="0"/>
-      <c r="AKQ46" s="0"/>
-      <c r="AKR46" s="0"/>
-      <c r="AKS46" s="0"/>
-      <c r="AKT46" s="0"/>
-      <c r="AKU46" s="0"/>
-      <c r="AKV46" s="0"/>
-      <c r="AKW46" s="0"/>
-      <c r="AKX46" s="0"/>
-      <c r="AKY46" s="0"/>
-      <c r="AKZ46" s="0"/>
-      <c r="ALA46" s="0"/>
-      <c r="ALB46" s="0"/>
-      <c r="ALC46" s="0"/>
-      <c r="ALD46" s="0"/>
-      <c r="ALE46" s="0"/>
-      <c r="ALF46" s="0"/>
-      <c r="ALG46" s="0"/>
-      <c r="ALH46" s="0"/>
-      <c r="ALI46" s="0"/>
-      <c r="ALJ46" s="0"/>
-      <c r="ALK46" s="0"/>
-      <c r="ALL46" s="0"/>
-      <c r="ALM46" s="0"/>
-      <c r="ALN46" s="0"/>
-      <c r="ALO46" s="0"/>
-      <c r="ALP46" s="0"/>
-      <c r="ALQ46" s="0"/>
-      <c r="ALR46" s="0"/>
-      <c r="ALS46" s="0"/>
-      <c r="ALT46" s="0"/>
-      <c r="ALU46" s="0"/>
-      <c r="ALV46" s="0"/>
-      <c r="ALW46" s="0"/>
-      <c r="ALX46" s="0"/>
-      <c r="ALY46" s="0"/>
-      <c r="ALZ46" s="0"/>
-      <c r="AMA46" s="0"/>
-      <c r="AMB46" s="0"/>
-      <c r="AMC46" s="0"/>
-      <c r="AMD46" s="0"/>
-      <c r="AME46" s="0"/>
-      <c r="AMF46" s="0"/>
-      <c r="AMG46" s="0"/>
-      <c r="AMH46" s="0"/>
-      <c r="AMI46" s="0"/>
-      <c r="AMJ46" s="0"/>
+      <c r="A46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="E47" s="14"/>
+      <c r="H47" s="0"/>
+      <c r="I47" s="0"/>
+      <c r="J47" s="0"/>
+      <c r="K47" s="0"/>
+      <c r="L47" s="0"/>
+      <c r="M47" s="0"/>
+      <c r="N47" s="0"/>
+      <c r="O47" s="0"/>
+      <c r="P47" s="0"/>
+      <c r="Q47" s="0"/>
+      <c r="R47" s="0"/>
+      <c r="S47" s="0"/>
+      <c r="T47" s="0"/>
+      <c r="U47" s="0"/>
+      <c r="V47" s="0"/>
+      <c r="W47" s="0"/>
+      <c r="X47" s="0"/>
+      <c r="Y47" s="0"/>
+      <c r="Z47" s="0"/>
+      <c r="AA47" s="0"/>
+      <c r="AB47" s="0"/>
+      <c r="AC47" s="0"/>
+      <c r="AD47" s="0"/>
+      <c r="AE47" s="0"/>
+      <c r="AF47" s="0"/>
+      <c r="AG47" s="0"/>
+      <c r="AH47" s="0"/>
+      <c r="AI47" s="0"/>
+      <c r="AJ47" s="0"/>
+      <c r="AK47" s="0"/>
+      <c r="AL47" s="0"/>
+      <c r="AM47" s="0"/>
+      <c r="AN47" s="0"/>
+      <c r="AO47" s="0"/>
+      <c r="AP47" s="0"/>
+      <c r="AQ47" s="0"/>
+      <c r="AR47" s="0"/>
+      <c r="AS47" s="0"/>
+      <c r="AT47" s="0"/>
+      <c r="AU47" s="0"/>
+      <c r="AV47" s="0"/>
+      <c r="AW47" s="0"/>
+      <c r="AX47" s="0"/>
+      <c r="AY47" s="0"/>
+      <c r="AZ47" s="0"/>
+      <c r="BA47" s="0"/>
+      <c r="BB47" s="0"/>
+      <c r="BC47" s="0"/>
+      <c r="BD47" s="0"/>
+      <c r="BE47" s="0"/>
+      <c r="BF47" s="0"/>
+      <c r="BG47" s="0"/>
+      <c r="BH47" s="0"/>
+      <c r="BI47" s="0"/>
+      <c r="BJ47" s="0"/>
+      <c r="BK47" s="0"/>
+      <c r="BL47" s="0"/>
+      <c r="BM47" s="0"/>
+      <c r="BN47" s="0"/>
+      <c r="BO47" s="0"/>
+      <c r="BP47" s="0"/>
+      <c r="BQ47" s="0"/>
+      <c r="BR47" s="0"/>
+      <c r="BS47" s="0"/>
+      <c r="BT47" s="0"/>
+      <c r="BU47" s="0"/>
+      <c r="BV47" s="0"/>
+      <c r="BW47" s="0"/>
+      <c r="BX47" s="0"/>
+      <c r="BY47" s="0"/>
+      <c r="BZ47" s="0"/>
+      <c r="CA47" s="0"/>
+      <c r="CB47" s="0"/>
+      <c r="CC47" s="0"/>
+      <c r="CD47" s="0"/>
+      <c r="CE47" s="0"/>
+      <c r="CF47" s="0"/>
+      <c r="CG47" s="0"/>
+      <c r="CH47" s="0"/>
+      <c r="CI47" s="0"/>
+      <c r="CJ47" s="0"/>
+      <c r="CK47" s="0"/>
+      <c r="CL47" s="0"/>
+      <c r="CM47" s="0"/>
+      <c r="CN47" s="0"/>
+      <c r="CO47" s="0"/>
+      <c r="CP47" s="0"/>
+      <c r="CQ47" s="0"/>
+      <c r="CR47" s="0"/>
+      <c r="CS47" s="0"/>
+      <c r="CT47" s="0"/>
+      <c r="CU47" s="0"/>
+      <c r="CV47" s="0"/>
+      <c r="CW47" s="0"/>
+      <c r="CX47" s="0"/>
+      <c r="CY47" s="0"/>
+      <c r="CZ47" s="0"/>
+      <c r="DA47" s="0"/>
+      <c r="DB47" s="0"/>
+      <c r="DC47" s="0"/>
+      <c r="DD47" s="0"/>
+      <c r="DE47" s="0"/>
+      <c r="DF47" s="0"/>
+      <c r="DG47" s="0"/>
+      <c r="DH47" s="0"/>
+      <c r="DI47" s="0"/>
+      <c r="DJ47" s="0"/>
+      <c r="DK47" s="0"/>
+      <c r="DL47" s="0"/>
+      <c r="DM47" s="0"/>
+      <c r="DN47" s="0"/>
+      <c r="DO47" s="0"/>
+      <c r="DP47" s="0"/>
+      <c r="DQ47" s="0"/>
+      <c r="DR47" s="0"/>
+      <c r="DS47" s="0"/>
+      <c r="DT47" s="0"/>
+      <c r="DU47" s="0"/>
+      <c r="DV47" s="0"/>
+      <c r="DW47" s="0"/>
+      <c r="DX47" s="0"/>
+      <c r="DY47" s="0"/>
+      <c r="DZ47" s="0"/>
+      <c r="EA47" s="0"/>
+      <c r="EB47" s="0"/>
+      <c r="EC47" s="0"/>
+      <c r="ED47" s="0"/>
+      <c r="EE47" s="0"/>
+      <c r="EF47" s="0"/>
+      <c r="EG47" s="0"/>
+      <c r="EH47" s="0"/>
+      <c r="EI47" s="0"/>
+      <c r="EJ47" s="0"/>
+      <c r="EK47" s="0"/>
+      <c r="EL47" s="0"/>
+      <c r="EM47" s="0"/>
+      <c r="EN47" s="0"/>
+      <c r="EO47" s="0"/>
+      <c r="EP47" s="0"/>
+      <c r="EQ47" s="0"/>
+      <c r="ER47" s="0"/>
+      <c r="ES47" s="0"/>
+      <c r="ET47" s="0"/>
+      <c r="EU47" s="0"/>
+      <c r="EV47" s="0"/>
+      <c r="EW47" s="0"/>
+      <c r="EX47" s="0"/>
+      <c r="EY47" s="0"/>
+      <c r="EZ47" s="0"/>
+      <c r="FA47" s="0"/>
+      <c r="FB47" s="0"/>
+      <c r="FC47" s="0"/>
+      <c r="FD47" s="0"/>
+      <c r="FE47" s="0"/>
+      <c r="FF47" s="0"/>
+      <c r="FG47" s="0"/>
+      <c r="FH47" s="0"/>
+      <c r="FI47" s="0"/>
+      <c r="FJ47" s="0"/>
+      <c r="FK47" s="0"/>
+      <c r="FL47" s="0"/>
+      <c r="FM47" s="0"/>
+      <c r="FN47" s="0"/>
+      <c r="FO47" s="0"/>
+      <c r="FP47" s="0"/>
+      <c r="FQ47" s="0"/>
+      <c r="FR47" s="0"/>
+      <c r="FS47" s="0"/>
+      <c r="FT47" s="0"/>
+      <c r="FU47" s="0"/>
+      <c r="FV47" s="0"/>
+      <c r="FW47" s="0"/>
+      <c r="FX47" s="0"/>
+      <c r="FY47" s="0"/>
+      <c r="FZ47" s="0"/>
+      <c r="GA47" s="0"/>
+      <c r="GB47" s="0"/>
+      <c r="GC47" s="0"/>
+      <c r="GD47" s="0"/>
+      <c r="GE47" s="0"/>
+      <c r="GF47" s="0"/>
+      <c r="GG47" s="0"/>
+      <c r="GH47" s="0"/>
+      <c r="GI47" s="0"/>
+      <c r="GJ47" s="0"/>
+      <c r="GK47" s="0"/>
+      <c r="GL47" s="0"/>
+      <c r="GM47" s="0"/>
+      <c r="GN47" s="0"/>
+      <c r="GO47" s="0"/>
+      <c r="GP47" s="0"/>
+      <c r="GQ47" s="0"/>
+      <c r="GR47" s="0"/>
+      <c r="GS47" s="0"/>
+      <c r="GT47" s="0"/>
+      <c r="GU47" s="0"/>
+      <c r="GV47" s="0"/>
+      <c r="GW47" s="0"/>
+      <c r="GX47" s="0"/>
+      <c r="GY47" s="0"/>
+      <c r="GZ47" s="0"/>
+      <c r="HA47" s="0"/>
+      <c r="HB47" s="0"/>
+      <c r="HC47" s="0"/>
+      <c r="HD47" s="0"/>
+      <c r="HE47" s="0"/>
+      <c r="HF47" s="0"/>
+      <c r="HG47" s="0"/>
+      <c r="HH47" s="0"/>
+      <c r="HI47" s="0"/>
+      <c r="HJ47" s="0"/>
+      <c r="HK47" s="0"/>
+      <c r="HL47" s="0"/>
+      <c r="HM47" s="0"/>
+      <c r="HN47" s="0"/>
+      <c r="HO47" s="0"/>
+      <c r="HP47" s="0"/>
+      <c r="HQ47" s="0"/>
+      <c r="HR47" s="0"/>
+      <c r="HS47" s="0"/>
+      <c r="HT47" s="0"/>
+      <c r="HU47" s="0"/>
+      <c r="HV47" s="0"/>
+      <c r="HW47" s="0"/>
+      <c r="HX47" s="0"/>
+      <c r="HY47" s="0"/>
+      <c r="HZ47" s="0"/>
+      <c r="IA47" s="0"/>
+      <c r="IB47" s="0"/>
+      <c r="IC47" s="0"/>
+      <c r="ID47" s="0"/>
+      <c r="IE47" s="0"/>
+      <c r="IF47" s="0"/>
+      <c r="IG47" s="0"/>
+      <c r="IH47" s="0"/>
+      <c r="II47" s="0"/>
+      <c r="IJ47" s="0"/>
+      <c r="IK47" s="0"/>
+      <c r="IL47" s="0"/>
+      <c r="IM47" s="0"/>
+      <c r="IN47" s="0"/>
+      <c r="IO47" s="0"/>
+      <c r="IP47" s="0"/>
+      <c r="IQ47" s="0"/>
+      <c r="IR47" s="0"/>
+      <c r="IS47" s="0"/>
+      <c r="IT47" s="0"/>
+      <c r="IU47" s="0"/>
+      <c r="IV47" s="0"/>
+      <c r="IW47" s="0"/>
+      <c r="IX47" s="0"/>
+      <c r="IY47" s="0"/>
+      <c r="IZ47" s="0"/>
+      <c r="JA47" s="0"/>
+      <c r="JB47" s="0"/>
+      <c r="JC47" s="0"/>
+      <c r="JD47" s="0"/>
+      <c r="JE47" s="0"/>
+      <c r="JF47" s="0"/>
+      <c r="JG47" s="0"/>
+      <c r="JH47" s="0"/>
+      <c r="JI47" s="0"/>
+      <c r="JJ47" s="0"/>
+      <c r="JK47" s="0"/>
+      <c r="JL47" s="0"/>
+      <c r="JM47" s="0"/>
+      <c r="JN47" s="0"/>
+      <c r="JO47" s="0"/>
+      <c r="JP47" s="0"/>
+      <c r="JQ47" s="0"/>
+      <c r="JR47" s="0"/>
+      <c r="JS47" s="0"/>
+      <c r="JT47" s="0"/>
+      <c r="JU47" s="0"/>
+      <c r="JV47" s="0"/>
+      <c r="JW47" s="0"/>
+      <c r="JX47" s="0"/>
+      <c r="JY47" s="0"/>
+      <c r="JZ47" s="0"/>
+      <c r="KA47" s="0"/>
+      <c r="KB47" s="0"/>
+      <c r="KC47" s="0"/>
+      <c r="KD47" s="0"/>
+      <c r="KE47" s="0"/>
+      <c r="KF47" s="0"/>
+      <c r="KG47" s="0"/>
+      <c r="KH47" s="0"/>
+      <c r="KI47" s="0"/>
+      <c r="KJ47" s="0"/>
+      <c r="KK47" s="0"/>
+      <c r="KL47" s="0"/>
+      <c r="KM47" s="0"/>
+      <c r="KN47" s="0"/>
+      <c r="KO47" s="0"/>
+      <c r="KP47" s="0"/>
+      <c r="KQ47" s="0"/>
+      <c r="KR47" s="0"/>
+      <c r="KS47" s="0"/>
+      <c r="KT47" s="0"/>
+      <c r="KU47" s="0"/>
+      <c r="KV47" s="0"/>
+      <c r="KW47" s="0"/>
+      <c r="KX47" s="0"/>
+      <c r="KY47" s="0"/>
+      <c r="KZ47" s="0"/>
+      <c r="LA47" s="0"/>
+      <c r="LB47" s="0"/>
+      <c r="LC47" s="0"/>
+      <c r="LD47" s="0"/>
+      <c r="LE47" s="0"/>
+      <c r="LF47" s="0"/>
+      <c r="LG47" s="0"/>
+      <c r="LH47" s="0"/>
+      <c r="LI47" s="0"/>
+      <c r="LJ47" s="0"/>
+      <c r="LK47" s="0"/>
+      <c r="LL47" s="0"/>
+      <c r="LM47" s="0"/>
+      <c r="LN47" s="0"/>
+      <c r="LO47" s="0"/>
+      <c r="LP47" s="0"/>
+      <c r="LQ47" s="0"/>
+      <c r="LR47" s="0"/>
+      <c r="LS47" s="0"/>
+      <c r="LT47" s="0"/>
+      <c r="LU47" s="0"/>
+      <c r="LV47" s="0"/>
+      <c r="LW47" s="0"/>
+      <c r="LX47" s="0"/>
+      <c r="LY47" s="0"/>
+      <c r="LZ47" s="0"/>
+      <c r="MA47" s="0"/>
+      <c r="MB47" s="0"/>
+      <c r="MC47" s="0"/>
+      <c r="MD47" s="0"/>
+      <c r="ME47" s="0"/>
+      <c r="MF47" s="0"/>
+      <c r="MG47" s="0"/>
+      <c r="MH47" s="0"/>
+      <c r="MI47" s="0"/>
+      <c r="MJ47" s="0"/>
+      <c r="MK47" s="0"/>
+      <c r="ML47" s="0"/>
+      <c r="MM47" s="0"/>
+      <c r="MN47" s="0"/>
+      <c r="MO47" s="0"/>
+      <c r="MP47" s="0"/>
+      <c r="MQ47" s="0"/>
+      <c r="MR47" s="0"/>
+      <c r="MS47" s="0"/>
+      <c r="MT47" s="0"/>
+      <c r="MU47" s="0"/>
+      <c r="MV47" s="0"/>
+      <c r="MW47" s="0"/>
+      <c r="MX47" s="0"/>
+      <c r="MY47" s="0"/>
+      <c r="MZ47" s="0"/>
+      <c r="NA47" s="0"/>
+      <c r="NB47" s="0"/>
+      <c r="NC47" s="0"/>
+      <c r="ND47" s="0"/>
+      <c r="NE47" s="0"/>
+      <c r="NF47" s="0"/>
+      <c r="NG47" s="0"/>
+      <c r="NH47" s="0"/>
+      <c r="NI47" s="0"/>
+      <c r="NJ47" s="0"/>
+      <c r="NK47" s="0"/>
+      <c r="NL47" s="0"/>
+      <c r="NM47" s="0"/>
+      <c r="NN47" s="0"/>
+      <c r="NO47" s="0"/>
+      <c r="NP47" s="0"/>
+      <c r="NQ47" s="0"/>
+      <c r="NR47" s="0"/>
+      <c r="NS47" s="0"/>
+      <c r="NT47" s="0"/>
+      <c r="NU47" s="0"/>
+      <c r="NV47" s="0"/>
+      <c r="NW47" s="0"/>
+      <c r="NX47" s="0"/>
+      <c r="NY47" s="0"/>
+      <c r="NZ47" s="0"/>
+      <c r="OA47" s="0"/>
+      <c r="OB47" s="0"/>
+      <c r="OC47" s="0"/>
+      <c r="OD47" s="0"/>
+      <c r="OE47" s="0"/>
+      <c r="OF47" s="0"/>
+      <c r="OG47" s="0"/>
+      <c r="OH47" s="0"/>
+      <c r="OI47" s="0"/>
+      <c r="OJ47" s="0"/>
+      <c r="OK47" s="0"/>
+      <c r="OL47" s="0"/>
+      <c r="OM47" s="0"/>
+      <c r="ON47" s="0"/>
+      <c r="OO47" s="0"/>
+      <c r="OP47" s="0"/>
+      <c r="OQ47" s="0"/>
+      <c r="OR47" s="0"/>
+      <c r="OS47" s="0"/>
+      <c r="OT47" s="0"/>
+      <c r="OU47" s="0"/>
+      <c r="OV47" s="0"/>
+      <c r="OW47" s="0"/>
+      <c r="OX47" s="0"/>
+      <c r="OY47" s="0"/>
+      <c r="OZ47" s="0"/>
+      <c r="PA47" s="0"/>
+      <c r="PB47" s="0"/>
+      <c r="PC47" s="0"/>
+      <c r="PD47" s="0"/>
+      <c r="PE47" s="0"/>
+      <c r="PF47" s="0"/>
+      <c r="PG47" s="0"/>
+      <c r="PH47" s="0"/>
+      <c r="PI47" s="0"/>
+      <c r="PJ47" s="0"/>
+      <c r="PK47" s="0"/>
+      <c r="PL47" s="0"/>
+      <c r="PM47" s="0"/>
+      <c r="PN47" s="0"/>
+      <c r="PO47" s="0"/>
+      <c r="PP47" s="0"/>
+      <c r="PQ47" s="0"/>
+      <c r="PR47" s="0"/>
+      <c r="PS47" s="0"/>
+      <c r="PT47" s="0"/>
+      <c r="PU47" s="0"/>
+      <c r="PV47" s="0"/>
+      <c r="PW47" s="0"/>
+      <c r="PX47" s="0"/>
+      <c r="PY47" s="0"/>
+      <c r="PZ47" s="0"/>
+      <c r="QA47" s="0"/>
+      <c r="QB47" s="0"/>
+      <c r="QC47" s="0"/>
+      <c r="QD47" s="0"/>
+      <c r="QE47" s="0"/>
+      <c r="QF47" s="0"/>
+      <c r="QG47" s="0"/>
+      <c r="QH47" s="0"/>
+      <c r="QI47" s="0"/>
+      <c r="QJ47" s="0"/>
+      <c r="QK47" s="0"/>
+      <c r="QL47" s="0"/>
+      <c r="QM47" s="0"/>
+      <c r="QN47" s="0"/>
+      <c r="QO47" s="0"/>
+      <c r="QP47" s="0"/>
+      <c r="QQ47" s="0"/>
+      <c r="QR47" s="0"/>
+      <c r="QS47" s="0"/>
+      <c r="QT47" s="0"/>
+      <c r="QU47" s="0"/>
+      <c r="QV47" s="0"/>
+      <c r="QW47" s="0"/>
+      <c r="QX47" s="0"/>
+      <c r="QY47" s="0"/>
+      <c r="QZ47" s="0"/>
+      <c r="RA47" s="0"/>
+      <c r="RB47" s="0"/>
+      <c r="RC47" s="0"/>
+      <c r="RD47" s="0"/>
+      <c r="RE47" s="0"/>
+      <c r="RF47" s="0"/>
+      <c r="RG47" s="0"/>
+      <c r="RH47" s="0"/>
+      <c r="RI47" s="0"/>
+      <c r="RJ47" s="0"/>
+      <c r="RK47" s="0"/>
+      <c r="RL47" s="0"/>
+      <c r="RM47" s="0"/>
+      <c r="RN47" s="0"/>
+      <c r="RO47" s="0"/>
+      <c r="RP47" s="0"/>
+      <c r="RQ47" s="0"/>
+      <c r="RR47" s="0"/>
+      <c r="RS47" s="0"/>
+      <c r="RT47" s="0"/>
+      <c r="RU47" s="0"/>
+      <c r="RV47" s="0"/>
+      <c r="RW47" s="0"/>
+      <c r="RX47" s="0"/>
+      <c r="RY47" s="0"/>
+      <c r="RZ47" s="0"/>
+      <c r="SA47" s="0"/>
+      <c r="SB47" s="0"/>
+      <c r="SC47" s="0"/>
+      <c r="SD47" s="0"/>
+      <c r="SE47" s="0"/>
+      <c r="SF47" s="0"/>
+      <c r="SG47" s="0"/>
+      <c r="SH47" s="0"/>
+      <c r="SI47" s="0"/>
+      <c r="SJ47" s="0"/>
+      <c r="SK47" s="0"/>
+      <c r="SL47" s="0"/>
+      <c r="SM47" s="0"/>
+      <c r="SN47" s="0"/>
+      <c r="SO47" s="0"/>
+      <c r="SP47" s="0"/>
+      <c r="SQ47" s="0"/>
+      <c r="SR47" s="0"/>
+      <c r="SS47" s="0"/>
+      <c r="ST47" s="0"/>
+      <c r="SU47" s="0"/>
+      <c r="SV47" s="0"/>
+      <c r="SW47" s="0"/>
+      <c r="SX47" s="0"/>
+      <c r="SY47" s="0"/>
+      <c r="SZ47" s="0"/>
+      <c r="TA47" s="0"/>
+      <c r="TB47" s="0"/>
+      <c r="TC47" s="0"/>
+      <c r="TD47" s="0"/>
+      <c r="TE47" s="0"/>
+      <c r="TF47" s="0"/>
+      <c r="TG47" s="0"/>
+      <c r="TH47" s="0"/>
+      <c r="TI47" s="0"/>
+      <c r="TJ47" s="0"/>
+      <c r="TK47" s="0"/>
+      <c r="TL47" s="0"/>
+      <c r="TM47" s="0"/>
+      <c r="TN47" s="0"/>
+      <c r="TO47" s="0"/>
+      <c r="TP47" s="0"/>
+      <c r="TQ47" s="0"/>
+      <c r="TR47" s="0"/>
+      <c r="TS47" s="0"/>
+      <c r="TT47" s="0"/>
+      <c r="TU47" s="0"/>
+      <c r="TV47" s="0"/>
+      <c r="TW47" s="0"/>
+      <c r="TX47" s="0"/>
+      <c r="TY47" s="0"/>
+      <c r="TZ47" s="0"/>
+      <c r="UA47" s="0"/>
+      <c r="UB47" s="0"/>
+      <c r="UC47" s="0"/>
+      <c r="UD47" s="0"/>
+      <c r="UE47" s="0"/>
+      <c r="UF47" s="0"/>
+      <c r="UG47" s="0"/>
+      <c r="UH47" s="0"/>
+      <c r="UI47" s="0"/>
+      <c r="UJ47" s="0"/>
+      <c r="UK47" s="0"/>
+      <c r="UL47" s="0"/>
+      <c r="UM47" s="0"/>
+      <c r="UN47" s="0"/>
+      <c r="UO47" s="0"/>
+      <c r="UP47" s="0"/>
+      <c r="UQ47" s="0"/>
+      <c r="UR47" s="0"/>
+      <c r="US47" s="0"/>
+      <c r="UT47" s="0"/>
+      <c r="UU47" s="0"/>
+      <c r="UV47" s="0"/>
+      <c r="UW47" s="0"/>
+      <c r="UX47" s="0"/>
+      <c r="UY47" s="0"/>
+      <c r="UZ47" s="0"/>
+      <c r="VA47" s="0"/>
+      <c r="VB47" s="0"/>
+      <c r="VC47" s="0"/>
+      <c r="VD47" s="0"/>
+      <c r="VE47" s="0"/>
+      <c r="VF47" s="0"/>
+      <c r="VG47" s="0"/>
+      <c r="VH47" s="0"/>
+      <c r="VI47" s="0"/>
+      <c r="VJ47" s="0"/>
+      <c r="VK47" s="0"/>
+      <c r="VL47" s="0"/>
+      <c r="VM47" s="0"/>
+      <c r="VN47" s="0"/>
+      <c r="VO47" s="0"/>
+      <c r="VP47" s="0"/>
+      <c r="VQ47" s="0"/>
+      <c r="VR47" s="0"/>
+      <c r="VS47" s="0"/>
+      <c r="VT47" s="0"/>
+      <c r="VU47" s="0"/>
+      <c r="VV47" s="0"/>
+      <c r="VW47" s="0"/>
+      <c r="VX47" s="0"/>
+      <c r="VY47" s="0"/>
+      <c r="VZ47" s="0"/>
+      <c r="WA47" s="0"/>
+      <c r="WB47" s="0"/>
+      <c r="WC47" s="0"/>
+      <c r="WD47" s="0"/>
+      <c r="WE47" s="0"/>
+      <c r="WF47" s="0"/>
+      <c r="WG47" s="0"/>
+      <c r="WH47" s="0"/>
+      <c r="WI47" s="0"/>
+      <c r="WJ47" s="0"/>
+      <c r="WK47" s="0"/>
+      <c r="WL47" s="0"/>
+      <c r="WM47" s="0"/>
+      <c r="WN47" s="0"/>
+      <c r="WO47" s="0"/>
+      <c r="WP47" s="0"/>
+      <c r="WQ47" s="0"/>
+      <c r="WR47" s="0"/>
+      <c r="WS47" s="0"/>
+      <c r="WT47" s="0"/>
+      <c r="WU47" s="0"/>
+      <c r="WV47" s="0"/>
+      <c r="WW47" s="0"/>
+      <c r="WX47" s="0"/>
+      <c r="WY47" s="0"/>
+      <c r="WZ47" s="0"/>
+      <c r="XA47" s="0"/>
+      <c r="XB47" s="0"/>
+      <c r="XC47" s="0"/>
+      <c r="XD47" s="0"/>
+      <c r="XE47" s="0"/>
+      <c r="XF47" s="0"/>
+      <c r="XG47" s="0"/>
+      <c r="XH47" s="0"/>
+      <c r="XI47" s="0"/>
+      <c r="XJ47" s="0"/>
+      <c r="XK47" s="0"/>
+      <c r="XL47" s="0"/>
+      <c r="XM47" s="0"/>
+      <c r="XN47" s="0"/>
+      <c r="XO47" s="0"/>
+      <c r="XP47" s="0"/>
+      <c r="XQ47" s="0"/>
+      <c r="XR47" s="0"/>
+      <c r="XS47" s="0"/>
+      <c r="XT47" s="0"/>
+      <c r="XU47" s="0"/>
+      <c r="XV47" s="0"/>
+      <c r="XW47" s="0"/>
+      <c r="XX47" s="0"/>
+      <c r="XY47" s="0"/>
+      <c r="XZ47" s="0"/>
+      <c r="YA47" s="0"/>
+      <c r="YB47" s="0"/>
+      <c r="YC47" s="0"/>
+      <c r="YD47" s="0"/>
+      <c r="YE47" s="0"/>
+      <c r="YF47" s="0"/>
+      <c r="YG47" s="0"/>
+      <c r="YH47" s="0"/>
+      <c r="YI47" s="0"/>
+      <c r="YJ47" s="0"/>
+      <c r="YK47" s="0"/>
+      <c r="YL47" s="0"/>
+      <c r="YM47" s="0"/>
+      <c r="YN47" s="0"/>
+      <c r="YO47" s="0"/>
+      <c r="YP47" s="0"/>
+      <c r="YQ47" s="0"/>
+      <c r="YR47" s="0"/>
+      <c r="YS47" s="0"/>
+      <c r="YT47" s="0"/>
+      <c r="YU47" s="0"/>
+      <c r="YV47" s="0"/>
+      <c r="YW47" s="0"/>
+      <c r="YX47" s="0"/>
+      <c r="YY47" s="0"/>
+      <c r="YZ47" s="0"/>
+      <c r="ZA47" s="0"/>
+      <c r="ZB47" s="0"/>
+      <c r="ZC47" s="0"/>
+      <c r="ZD47" s="0"/>
+      <c r="ZE47" s="0"/>
+      <c r="ZF47" s="0"/>
+      <c r="ZG47" s="0"/>
+      <c r="ZH47" s="0"/>
+      <c r="ZI47" s="0"/>
+      <c r="ZJ47" s="0"/>
+      <c r="ZK47" s="0"/>
+      <c r="ZL47" s="0"/>
+      <c r="ZM47" s="0"/>
+      <c r="ZN47" s="0"/>
+      <c r="ZO47" s="0"/>
+      <c r="ZP47" s="0"/>
+      <c r="ZQ47" s="0"/>
+      <c r="ZR47" s="0"/>
+      <c r="ZS47" s="0"/>
+      <c r="ZT47" s="0"/>
+      <c r="ZU47" s="0"/>
+      <c r="ZV47" s="0"/>
+      <c r="ZW47" s="0"/>
+      <c r="ZX47" s="0"/>
+      <c r="ZY47" s="0"/>
+      <c r="ZZ47" s="0"/>
+      <c r="AAA47" s="0"/>
+      <c r="AAB47" s="0"/>
+      <c r="AAC47" s="0"/>
+      <c r="AAD47" s="0"/>
+      <c r="AAE47" s="0"/>
+      <c r="AAF47" s="0"/>
+      <c r="AAG47" s="0"/>
+      <c r="AAH47" s="0"/>
+      <c r="AAI47" s="0"/>
+      <c r="AAJ47" s="0"/>
+      <c r="AAK47" s="0"/>
+      <c r="AAL47" s="0"/>
+      <c r="AAM47" s="0"/>
+      <c r="AAN47" s="0"/>
+      <c r="AAO47" s="0"/>
+      <c r="AAP47" s="0"/>
+      <c r="AAQ47" s="0"/>
+      <c r="AAR47" s="0"/>
+      <c r="AAS47" s="0"/>
+      <c r="AAT47" s="0"/>
+      <c r="AAU47" s="0"/>
+      <c r="AAV47" s="0"/>
+      <c r="AAW47" s="0"/>
+      <c r="AAX47" s="0"/>
+      <c r="AAY47" s="0"/>
+      <c r="AAZ47" s="0"/>
+      <c r="ABA47" s="0"/>
+      <c r="ABB47" s="0"/>
+      <c r="ABC47" s="0"/>
+      <c r="ABD47" s="0"/>
+      <c r="ABE47" s="0"/>
+      <c r="ABF47" s="0"/>
+      <c r="ABG47" s="0"/>
+      <c r="ABH47" s="0"/>
+      <c r="ABI47" s="0"/>
+      <c r="ABJ47" s="0"/>
+      <c r="ABK47" s="0"/>
+      <c r="ABL47" s="0"/>
+      <c r="ABM47" s="0"/>
+      <c r="ABN47" s="0"/>
+      <c r="ABO47" s="0"/>
+      <c r="ABP47" s="0"/>
+      <c r="ABQ47" s="0"/>
+      <c r="ABR47" s="0"/>
+      <c r="ABS47" s="0"/>
+      <c r="ABT47" s="0"/>
+      <c r="ABU47" s="0"/>
+      <c r="ABV47" s="0"/>
+      <c r="ABW47" s="0"/>
+      <c r="ABX47" s="0"/>
+      <c r="ABY47" s="0"/>
+      <c r="ABZ47" s="0"/>
+      <c r="ACA47" s="0"/>
+      <c r="ACB47" s="0"/>
+      <c r="ACC47" s="0"/>
+      <c r="ACD47" s="0"/>
+      <c r="ACE47" s="0"/>
+      <c r="ACF47" s="0"/>
+      <c r="ACG47" s="0"/>
+      <c r="ACH47" s="0"/>
+      <c r="ACI47" s="0"/>
+      <c r="ACJ47" s="0"/>
+      <c r="ACK47" s="0"/>
+      <c r="ACL47" s="0"/>
+      <c r="ACM47" s="0"/>
+      <c r="ACN47" s="0"/>
+      <c r="ACO47" s="0"/>
+      <c r="ACP47" s="0"/>
+      <c r="ACQ47" s="0"/>
+      <c r="ACR47" s="0"/>
+      <c r="ACS47" s="0"/>
+      <c r="ACT47" s="0"/>
+      <c r="ACU47" s="0"/>
+      <c r="ACV47" s="0"/>
+      <c r="ACW47" s="0"/>
+      <c r="ACX47" s="0"/>
+      <c r="ACY47" s="0"/>
+      <c r="ACZ47" s="0"/>
+      <c r="ADA47" s="0"/>
+      <c r="ADB47" s="0"/>
+      <c r="ADC47" s="0"/>
+      <c r="ADD47" s="0"/>
+      <c r="ADE47" s="0"/>
+      <c r="ADF47" s="0"/>
+      <c r="ADG47" s="0"/>
+      <c r="ADH47" s="0"/>
+      <c r="ADI47" s="0"/>
+      <c r="ADJ47" s="0"/>
+      <c r="ADK47" s="0"/>
+      <c r="ADL47" s="0"/>
+      <c r="ADM47" s="0"/>
+      <c r="ADN47" s="0"/>
+      <c r="ADO47" s="0"/>
+      <c r="ADP47" s="0"/>
+      <c r="ADQ47" s="0"/>
+      <c r="ADR47" s="0"/>
+      <c r="ADS47" s="0"/>
+      <c r="ADT47" s="0"/>
+      <c r="ADU47" s="0"/>
+      <c r="ADV47" s="0"/>
+      <c r="ADW47" s="0"/>
+      <c r="ADX47" s="0"/>
+      <c r="ADY47" s="0"/>
+      <c r="ADZ47" s="0"/>
+      <c r="AEA47" s="0"/>
+      <c r="AEB47" s="0"/>
+      <c r="AEC47" s="0"/>
+      <c r="AED47" s="0"/>
+      <c r="AEE47" s="0"/>
+      <c r="AEF47" s="0"/>
+      <c r="AEG47" s="0"/>
+      <c r="AEH47" s="0"/>
+      <c r="AEI47" s="0"/>
+      <c r="AEJ47" s="0"/>
+      <c r="AEK47" s="0"/>
+      <c r="AEL47" s="0"/>
+      <c r="AEM47" s="0"/>
+      <c r="AEN47" s="0"/>
+      <c r="AEO47" s="0"/>
+      <c r="AEP47" s="0"/>
+      <c r="AEQ47" s="0"/>
+      <c r="AER47" s="0"/>
+      <c r="AES47" s="0"/>
+      <c r="AET47" s="0"/>
+      <c r="AEU47" s="0"/>
+      <c r="AEV47" s="0"/>
+      <c r="AEW47" s="0"/>
+      <c r="AEX47" s="0"/>
+      <c r="AEY47" s="0"/>
+      <c r="AEZ47" s="0"/>
+      <c r="AFA47" s="0"/>
+      <c r="AFB47" s="0"/>
+      <c r="AFC47" s="0"/>
+      <c r="AFD47" s="0"/>
+      <c r="AFE47" s="0"/>
+      <c r="AFF47" s="0"/>
+      <c r="AFG47" s="0"/>
+      <c r="AFH47" s="0"/>
+      <c r="AFI47" s="0"/>
+      <c r="AFJ47" s="0"/>
+      <c r="AFK47" s="0"/>
+      <c r="AFL47" s="0"/>
+      <c r="AFM47" s="0"/>
+      <c r="AFN47" s="0"/>
+      <c r="AFO47" s="0"/>
+      <c r="AFP47" s="0"/>
+      <c r="AFQ47" s="0"/>
+      <c r="AFR47" s="0"/>
+      <c r="AFS47" s="0"/>
+      <c r="AFT47" s="0"/>
+      <c r="AFU47" s="0"/>
+      <c r="AFV47" s="0"/>
+      <c r="AFW47" s="0"/>
+      <c r="AFX47" s="0"/>
+      <c r="AFY47" s="0"/>
+      <c r="AFZ47" s="0"/>
+      <c r="AGA47" s="0"/>
+      <c r="AGB47" s="0"/>
+      <c r="AGC47" s="0"/>
+      <c r="AGD47" s="0"/>
+      <c r="AGE47" s="0"/>
+      <c r="AGF47" s="0"/>
+      <c r="AGG47" s="0"/>
+      <c r="AGH47" s="0"/>
+      <c r="AGI47" s="0"/>
+      <c r="AGJ47" s="0"/>
+      <c r="AGK47" s="0"/>
+      <c r="AGL47" s="0"/>
+      <c r="AGM47" s="0"/>
+      <c r="AGN47" s="0"/>
+      <c r="AGO47" s="0"/>
+      <c r="AGP47" s="0"/>
+      <c r="AGQ47" s="0"/>
+      <c r="AGR47" s="0"/>
+      <c r="AGS47" s="0"/>
+      <c r="AGT47" s="0"/>
+      <c r="AGU47" s="0"/>
+      <c r="AGV47" s="0"/>
+      <c r="AGW47" s="0"/>
+      <c r="AGX47" s="0"/>
+      <c r="AGY47" s="0"/>
+      <c r="AGZ47" s="0"/>
+      <c r="AHA47" s="0"/>
+      <c r="AHB47" s="0"/>
+      <c r="AHC47" s="0"/>
+      <c r="AHD47" s="0"/>
+      <c r="AHE47" s="0"/>
+      <c r="AHF47" s="0"/>
+      <c r="AHG47" s="0"/>
+      <c r="AHH47" s="0"/>
+      <c r="AHI47" s="0"/>
+      <c r="AHJ47" s="0"/>
+      <c r="AHK47" s="0"/>
+      <c r="AHL47" s="0"/>
+      <c r="AHM47" s="0"/>
+      <c r="AHN47" s="0"/>
+      <c r="AHO47" s="0"/>
+      <c r="AHP47" s="0"/>
+      <c r="AHQ47" s="0"/>
+      <c r="AHR47" s="0"/>
+      <c r="AHS47" s="0"/>
+      <c r="AHT47" s="0"/>
+      <c r="AHU47" s="0"/>
+      <c r="AHV47" s="0"/>
+      <c r="AHW47" s="0"/>
+      <c r="AHX47" s="0"/>
+      <c r="AHY47" s="0"/>
+      <c r="AHZ47" s="0"/>
+      <c r="AIA47" s="0"/>
+      <c r="AIB47" s="0"/>
+      <c r="AIC47" s="0"/>
+      <c r="AID47" s="0"/>
+      <c r="AIE47" s="0"/>
+      <c r="AIF47" s="0"/>
+      <c r="AIG47" s="0"/>
+      <c r="AIH47" s="0"/>
+      <c r="AII47" s="0"/>
+      <c r="AIJ47" s="0"/>
+      <c r="AIK47" s="0"/>
+      <c r="AIL47" s="0"/>
+      <c r="AIM47" s="0"/>
+      <c r="AIN47" s="0"/>
+      <c r="AIO47" s="0"/>
+      <c r="AIP47" s="0"/>
+      <c r="AIQ47" s="0"/>
+      <c r="AIR47" s="0"/>
+      <c r="AIS47" s="0"/>
+      <c r="AIT47" s="0"/>
+      <c r="AIU47" s="0"/>
+      <c r="AIV47" s="0"/>
+      <c r="AIW47" s="0"/>
+      <c r="AIX47" s="0"/>
+      <c r="AIY47" s="0"/>
+      <c r="AIZ47" s="0"/>
+      <c r="AJA47" s="0"/>
+      <c r="AJB47" s="0"/>
+      <c r="AJC47" s="0"/>
+      <c r="AJD47" s="0"/>
+      <c r="AJE47" s="0"/>
+      <c r="AJF47" s="0"/>
+      <c r="AJG47" s="0"/>
+      <c r="AJH47" s="0"/>
+      <c r="AJI47" s="0"/>
+      <c r="AJJ47" s="0"/>
+      <c r="AJK47" s="0"/>
+      <c r="AJL47" s="0"/>
+      <c r="AJM47" s="0"/>
+      <c r="AJN47" s="0"/>
+      <c r="AJO47" s="0"/>
+      <c r="AJP47" s="0"/>
+      <c r="AJQ47" s="0"/>
+      <c r="AJR47" s="0"/>
+      <c r="AJS47" s="0"/>
+      <c r="AJT47" s="0"/>
+      <c r="AJU47" s="0"/>
+      <c r="AJV47" s="0"/>
+      <c r="AJW47" s="0"/>
+      <c r="AJX47" s="0"/>
+      <c r="AJY47" s="0"/>
+      <c r="AJZ47" s="0"/>
+      <c r="AKA47" s="0"/>
+      <c r="AKB47" s="0"/>
+      <c r="AKC47" s="0"/>
+      <c r="AKD47" s="0"/>
+      <c r="AKE47" s="0"/>
+      <c r="AKF47" s="0"/>
+      <c r="AKG47" s="0"/>
+      <c r="AKH47" s="0"/>
+      <c r="AKI47" s="0"/>
+      <c r="AKJ47" s="0"/>
+      <c r="AKK47" s="0"/>
+      <c r="AKL47" s="0"/>
+      <c r="AKM47" s="0"/>
+      <c r="AKN47" s="0"/>
+      <c r="AKO47" s="0"/>
+      <c r="AKP47" s="0"/>
+      <c r="AKQ47" s="0"/>
+      <c r="AKR47" s="0"/>
+      <c r="AKS47" s="0"/>
+      <c r="AKT47" s="0"/>
+      <c r="AKU47" s="0"/>
+      <c r="AKV47" s="0"/>
+      <c r="AKW47" s="0"/>
+      <c r="AKX47" s="0"/>
+      <c r="AKY47" s="0"/>
+      <c r="AKZ47" s="0"/>
+      <c r="ALA47" s="0"/>
+      <c r="ALB47" s="0"/>
+      <c r="ALC47" s="0"/>
+      <c r="ALD47" s="0"/>
+      <c r="ALE47" s="0"/>
+      <c r="ALF47" s="0"/>
+      <c r="ALG47" s="0"/>
+      <c r="ALH47" s="0"/>
+      <c r="ALI47" s="0"/>
+      <c r="ALJ47" s="0"/>
+      <c r="ALK47" s="0"/>
+      <c r="ALL47" s="0"/>
+      <c r="ALM47" s="0"/>
+      <c r="ALN47" s="0"/>
+      <c r="ALO47" s="0"/>
+      <c r="ALP47" s="0"/>
+      <c r="ALQ47" s="0"/>
+      <c r="ALR47" s="0"/>
+      <c r="ALS47" s="0"/>
+      <c r="ALT47" s="0"/>
+      <c r="ALU47" s="0"/>
+      <c r="ALV47" s="0"/>
+      <c r="ALW47" s="0"/>
+      <c r="ALX47" s="0"/>
+      <c r="ALY47" s="0"/>
+      <c r="ALZ47" s="0"/>
+      <c r="AMA47" s="0"/>
+      <c r="AMB47" s="0"/>
+      <c r="AMC47" s="0"/>
+      <c r="AMD47" s="0"/>
+      <c r="AME47" s="0"/>
+      <c r="AMF47" s="0"/>
+      <c r="AMG47" s="0"/>
+      <c r="AMH47" s="0"/>
+      <c r="AMI47" s="0"/>
+      <c r="AMJ47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="E48" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H48" s="0"/>
+      <c r="I48" s="0"/>
+      <c r="J48" s="0"/>
+      <c r="K48" s="0"/>
+      <c r="L48" s="0"/>
+      <c r="M48" s="0"/>
+      <c r="N48" s="0"/>
+      <c r="O48" s="0"/>
+      <c r="P48" s="0"/>
+      <c r="Q48" s="0"/>
+      <c r="R48" s="0"/>
+      <c r="S48" s="0"/>
+      <c r="T48" s="0"/>
+      <c r="U48" s="0"/>
+      <c r="V48" s="0"/>
+      <c r="W48" s="0"/>
+      <c r="X48" s="0"/>
+      <c r="Y48" s="0"/>
+      <c r="Z48" s="0"/>
+      <c r="AA48" s="0"/>
+      <c r="AB48" s="0"/>
+      <c r="AC48" s="0"/>
+      <c r="AD48" s="0"/>
+      <c r="AE48" s="0"/>
+      <c r="AF48" s="0"/>
+      <c r="AG48" s="0"/>
+      <c r="AH48" s="0"/>
+      <c r="AI48" s="0"/>
+      <c r="AJ48" s="0"/>
+      <c r="AK48" s="0"/>
+      <c r="AL48" s="0"/>
+      <c r="AM48" s="0"/>
+      <c r="AN48" s="0"/>
+      <c r="AO48" s="0"/>
+      <c r="AP48" s="0"/>
+      <c r="AQ48" s="0"/>
+      <c r="AR48" s="0"/>
+      <c r="AS48" s="0"/>
+      <c r="AT48" s="0"/>
+      <c r="AU48" s="0"/>
+      <c r="AV48" s="0"/>
+      <c r="AW48" s="0"/>
+      <c r="AX48" s="0"/>
+      <c r="AY48" s="0"/>
+      <c r="AZ48" s="0"/>
+      <c r="BA48" s="0"/>
+      <c r="BB48" s="0"/>
+      <c r="BC48" s="0"/>
+      <c r="BD48" s="0"/>
+      <c r="BE48" s="0"/>
+      <c r="BF48" s="0"/>
+      <c r="BG48" s="0"/>
+      <c r="BH48" s="0"/>
+      <c r="BI48" s="0"/>
+      <c r="BJ48" s="0"/>
+      <c r="BK48" s="0"/>
+      <c r="BL48" s="0"/>
+      <c r="BM48" s="0"/>
+      <c r="BN48" s="0"/>
+      <c r="BO48" s="0"/>
+      <c r="BP48" s="0"/>
+      <c r="BQ48" s="0"/>
+      <c r="BR48" s="0"/>
+      <c r="BS48" s="0"/>
+      <c r="BT48" s="0"/>
+      <c r="BU48" s="0"/>
+      <c r="BV48" s="0"/>
+      <c r="BW48" s="0"/>
+      <c r="BX48" s="0"/>
+      <c r="BY48" s="0"/>
+      <c r="BZ48" s="0"/>
+      <c r="CA48" s="0"/>
+      <c r="CB48" s="0"/>
+      <c r="CC48" s="0"/>
+      <c r="CD48" s="0"/>
+      <c r="CE48" s="0"/>
+      <c r="CF48" s="0"/>
+      <c r="CG48" s="0"/>
+      <c r="CH48" s="0"/>
+      <c r="CI48" s="0"/>
+      <c r="CJ48" s="0"/>
+      <c r="CK48" s="0"/>
+      <c r="CL48" s="0"/>
+      <c r="CM48" s="0"/>
+      <c r="CN48" s="0"/>
+      <c r="CO48" s="0"/>
+      <c r="CP48" s="0"/>
+      <c r="CQ48" s="0"/>
+      <c r="CR48" s="0"/>
+      <c r="CS48" s="0"/>
+      <c r="CT48" s="0"/>
+      <c r="CU48" s="0"/>
+      <c r="CV48" s="0"/>
+      <c r="CW48" s="0"/>
+      <c r="CX48" s="0"/>
+      <c r="CY48" s="0"/>
+      <c r="CZ48" s="0"/>
+      <c r="DA48" s="0"/>
+      <c r="DB48" s="0"/>
+      <c r="DC48" s="0"/>
+      <c r="DD48" s="0"/>
+      <c r="DE48" s="0"/>
+      <c r="DF48" s="0"/>
+      <c r="DG48" s="0"/>
+      <c r="DH48" s="0"/>
+      <c r="DI48" s="0"/>
+      <c r="DJ48" s="0"/>
+      <c r="DK48" s="0"/>
+      <c r="DL48" s="0"/>
+      <c r="DM48" s="0"/>
+      <c r="DN48" s="0"/>
+      <c r="DO48" s="0"/>
+      <c r="DP48" s="0"/>
+      <c r="DQ48" s="0"/>
+      <c r="DR48" s="0"/>
+      <c r="DS48" s="0"/>
+      <c r="DT48" s="0"/>
+      <c r="DU48" s="0"/>
+      <c r="DV48" s="0"/>
+      <c r="DW48" s="0"/>
+      <c r="DX48" s="0"/>
+      <c r="DY48" s="0"/>
+      <c r="DZ48" s="0"/>
+      <c r="EA48" s="0"/>
+      <c r="EB48" s="0"/>
+      <c r="EC48" s="0"/>
+      <c r="ED48" s="0"/>
+      <c r="EE48" s="0"/>
+      <c r="EF48" s="0"/>
+      <c r="EG48" s="0"/>
+      <c r="EH48" s="0"/>
+      <c r="EI48" s="0"/>
+      <c r="EJ48" s="0"/>
+      <c r="EK48" s="0"/>
+      <c r="EL48" s="0"/>
+      <c r="EM48" s="0"/>
+      <c r="EN48" s="0"/>
+      <c r="EO48" s="0"/>
+      <c r="EP48" s="0"/>
+      <c r="EQ48" s="0"/>
+      <c r="ER48" s="0"/>
+      <c r="ES48" s="0"/>
+      <c r="ET48" s="0"/>
+      <c r="EU48" s="0"/>
+      <c r="EV48" s="0"/>
+      <c r="EW48" s="0"/>
+      <c r="EX48" s="0"/>
+      <c r="EY48" s="0"/>
+      <c r="EZ48" s="0"/>
+      <c r="FA48" s="0"/>
+      <c r="FB48" s="0"/>
+      <c r="FC48" s="0"/>
+      <c r="FD48" s="0"/>
+      <c r="FE48" s="0"/>
+      <c r="FF48" s="0"/>
+      <c r="FG48" s="0"/>
+      <c r="FH48" s="0"/>
+      <c r="FI48" s="0"/>
+      <c r="FJ48" s="0"/>
+      <c r="FK48" s="0"/>
+      <c r="FL48" s="0"/>
+      <c r="FM48" s="0"/>
+      <c r="FN48" s="0"/>
+      <c r="FO48" s="0"/>
+      <c r="FP48" s="0"/>
+      <c r="FQ48" s="0"/>
+      <c r="FR48" s="0"/>
+      <c r="FS48" s="0"/>
+      <c r="FT48" s="0"/>
+      <c r="FU48" s="0"/>
+      <c r="FV48" s="0"/>
+      <c r="FW48" s="0"/>
+      <c r="FX48" s="0"/>
+      <c r="FY48" s="0"/>
+      <c r="FZ48" s="0"/>
+      <c r="GA48" s="0"/>
+      <c r="GB48" s="0"/>
+      <c r="GC48" s="0"/>
+      <c r="GD48" s="0"/>
+      <c r="GE48" s="0"/>
+      <c r="GF48" s="0"/>
+      <c r="GG48" s="0"/>
+      <c r="GH48" s="0"/>
+      <c r="GI48" s="0"/>
+      <c r="GJ48" s="0"/>
+      <c r="GK48" s="0"/>
+      <c r="GL48" s="0"/>
+      <c r="GM48" s="0"/>
+      <c r="GN48" s="0"/>
+      <c r="GO48" s="0"/>
+      <c r="GP48" s="0"/>
+      <c r="GQ48" s="0"/>
+      <c r="GR48" s="0"/>
+      <c r="GS48" s="0"/>
+      <c r="GT48" s="0"/>
+      <c r="GU48" s="0"/>
+      <c r="GV48" s="0"/>
+      <c r="GW48" s="0"/>
+      <c r="GX48" s="0"/>
+      <c r="GY48" s="0"/>
+      <c r="GZ48" s="0"/>
+      <c r="HA48" s="0"/>
+      <c r="HB48" s="0"/>
+      <c r="HC48" s="0"/>
+      <c r="HD48" s="0"/>
+      <c r="HE48" s="0"/>
+      <c r="HF48" s="0"/>
+      <c r="HG48" s="0"/>
+      <c r="HH48" s="0"/>
+      <c r="HI48" s="0"/>
+      <c r="HJ48" s="0"/>
+      <c r="HK48" s="0"/>
+      <c r="HL48" s="0"/>
+      <c r="HM48" s="0"/>
+      <c r="HN48" s="0"/>
+      <c r="HO48" s="0"/>
+      <c r="HP48" s="0"/>
+      <c r="HQ48" s="0"/>
+      <c r="HR48" s="0"/>
+      <c r="HS48" s="0"/>
+      <c r="HT48" s="0"/>
+      <c r="HU48" s="0"/>
+      <c r="HV48" s="0"/>
+      <c r="HW48" s="0"/>
+      <c r="HX48" s="0"/>
+      <c r="HY48" s="0"/>
+      <c r="HZ48" s="0"/>
+      <c r="IA48" s="0"/>
+      <c r="IB48" s="0"/>
+      <c r="IC48" s="0"/>
+      <c r="ID48" s="0"/>
+      <c r="IE48" s="0"/>
+      <c r="IF48" s="0"/>
+      <c r="IG48" s="0"/>
+      <c r="IH48" s="0"/>
+      <c r="II48" s="0"/>
+      <c r="IJ48" s="0"/>
+      <c r="IK48" s="0"/>
+      <c r="IL48" s="0"/>
+      <c r="IM48" s="0"/>
+      <c r="IN48" s="0"/>
+      <c r="IO48" s="0"/>
+      <c r="IP48" s="0"/>
+      <c r="IQ48" s="0"/>
+      <c r="IR48" s="0"/>
+      <c r="IS48" s="0"/>
+      <c r="IT48" s="0"/>
+      <c r="IU48" s="0"/>
+      <c r="IV48" s="0"/>
+      <c r="IW48" s="0"/>
+      <c r="IX48" s="0"/>
+      <c r="IY48" s="0"/>
+      <c r="IZ48" s="0"/>
+      <c r="JA48" s="0"/>
+      <c r="JB48" s="0"/>
+      <c r="JC48" s="0"/>
+      <c r="JD48" s="0"/>
+      <c r="JE48" s="0"/>
+      <c r="JF48" s="0"/>
+      <c r="JG48" s="0"/>
+      <c r="JH48" s="0"/>
+      <c r="JI48" s="0"/>
+      <c r="JJ48" s="0"/>
+      <c r="JK48" s="0"/>
+      <c r="JL48" s="0"/>
+      <c r="JM48" s="0"/>
+      <c r="JN48" s="0"/>
+      <c r="JO48" s="0"/>
+      <c r="JP48" s="0"/>
+      <c r="JQ48" s="0"/>
+      <c r="JR48" s="0"/>
+      <c r="JS48" s="0"/>
+      <c r="JT48" s="0"/>
+      <c r="JU48" s="0"/>
+      <c r="JV48" s="0"/>
+      <c r="JW48" s="0"/>
+      <c r="JX48" s="0"/>
+      <c r="JY48" s="0"/>
+      <c r="JZ48" s="0"/>
+      <c r="KA48" s="0"/>
+      <c r="KB48" s="0"/>
+      <c r="KC48" s="0"/>
+      <c r="KD48" s="0"/>
+      <c r="KE48" s="0"/>
+      <c r="KF48" s="0"/>
+      <c r="KG48" s="0"/>
+      <c r="KH48" s="0"/>
+      <c r="KI48" s="0"/>
+      <c r="KJ48" s="0"/>
+      <c r="KK48" s="0"/>
+      <c r="KL48" s="0"/>
+      <c r="KM48" s="0"/>
+      <c r="KN48" s="0"/>
+      <c r="KO48" s="0"/>
+      <c r="KP48" s="0"/>
+      <c r="KQ48" s="0"/>
+      <c r="KR48" s="0"/>
+      <c r="KS48" s="0"/>
+      <c r="KT48" s="0"/>
+      <c r="KU48" s="0"/>
+      <c r="KV48" s="0"/>
+      <c r="KW48" s="0"/>
+      <c r="KX48" s="0"/>
+      <c r="KY48" s="0"/>
+      <c r="KZ48" s="0"/>
+      <c r="LA48" s="0"/>
+      <c r="LB48" s="0"/>
+      <c r="LC48" s="0"/>
+      <c r="LD48" s="0"/>
+      <c r="LE48" s="0"/>
+      <c r="LF48" s="0"/>
+      <c r="LG48" s="0"/>
+      <c r="LH48" s="0"/>
+      <c r="LI48" s="0"/>
+      <c r="LJ48" s="0"/>
+      <c r="LK48" s="0"/>
+      <c r="LL48" s="0"/>
+      <c r="LM48" s="0"/>
+      <c r="LN48" s="0"/>
+      <c r="LO48" s="0"/>
+      <c r="LP48" s="0"/>
+      <c r="LQ48" s="0"/>
+      <c r="LR48" s="0"/>
+      <c r="LS48" s="0"/>
+      <c r="LT48" s="0"/>
+      <c r="LU48" s="0"/>
+      <c r="LV48" s="0"/>
+      <c r="LW48" s="0"/>
+      <c r="LX48" s="0"/>
+      <c r="LY48" s="0"/>
+      <c r="LZ48" s="0"/>
+      <c r="MA48" s="0"/>
+      <c r="MB48" s="0"/>
+      <c r="MC48" s="0"/>
+      <c r="MD48" s="0"/>
+      <c r="ME48" s="0"/>
+      <c r="MF48" s="0"/>
+      <c r="MG48" s="0"/>
+      <c r="MH48" s="0"/>
+      <c r="MI48" s="0"/>
+      <c r="MJ48" s="0"/>
+      <c r="MK48" s="0"/>
+      <c r="ML48" s="0"/>
+      <c r="MM48" s="0"/>
+      <c r="MN48" s="0"/>
+      <c r="MO48" s="0"/>
+      <c r="MP48" s="0"/>
+      <c r="MQ48" s="0"/>
+      <c r="MR48" s="0"/>
+      <c r="MS48" s="0"/>
+      <c r="MT48" s="0"/>
+      <c r="MU48" s="0"/>
+      <c r="MV48" s="0"/>
+      <c r="MW48" s="0"/>
+      <c r="MX48" s="0"/>
+      <c r="MY48" s="0"/>
+      <c r="MZ48" s="0"/>
+      <c r="NA48" s="0"/>
+      <c r="NB48" s="0"/>
+      <c r="NC48" s="0"/>
+      <c r="ND48" s="0"/>
+      <c r="NE48" s="0"/>
+      <c r="NF48" s="0"/>
+      <c r="NG48" s="0"/>
+      <c r="NH48" s="0"/>
+      <c r="NI48" s="0"/>
+      <c r="NJ48" s="0"/>
+      <c r="NK48" s="0"/>
+      <c r="NL48" s="0"/>
+      <c r="NM48" s="0"/>
+      <c r="NN48" s="0"/>
+      <c r="NO48" s="0"/>
+      <c r="NP48" s="0"/>
+      <c r="NQ48" s="0"/>
+      <c r="NR48" s="0"/>
+      <c r="NS48" s="0"/>
+      <c r="NT48" s="0"/>
+      <c r="NU48" s="0"/>
+      <c r="NV48" s="0"/>
+      <c r="NW48" s="0"/>
+      <c r="NX48" s="0"/>
+      <c r="NY48" s="0"/>
+      <c r="NZ48" s="0"/>
+      <c r="OA48" s="0"/>
+      <c r="OB48" s="0"/>
+      <c r="OC48" s="0"/>
+      <c r="OD48" s="0"/>
+      <c r="OE48" s="0"/>
+      <c r="OF48" s="0"/>
+      <c r="OG48" s="0"/>
+      <c r="OH48" s="0"/>
+      <c r="OI48" s="0"/>
+      <c r="OJ48" s="0"/>
+      <c r="OK48" s="0"/>
+      <c r="OL48" s="0"/>
+      <c r="OM48" s="0"/>
+      <c r="ON48" s="0"/>
+      <c r="OO48" s="0"/>
+      <c r="OP48" s="0"/>
+      <c r="OQ48" s="0"/>
+      <c r="OR48" s="0"/>
+      <c r="OS48" s="0"/>
+      <c r="OT48" s="0"/>
+      <c r="OU48" s="0"/>
+      <c r="OV48" s="0"/>
+      <c r="OW48" s="0"/>
+      <c r="OX48" s="0"/>
+      <c r="OY48" s="0"/>
+      <c r="OZ48" s="0"/>
+      <c r="PA48" s="0"/>
+      <c r="PB48" s="0"/>
+      <c r="PC48" s="0"/>
+      <c r="PD48" s="0"/>
+      <c r="PE48" s="0"/>
+      <c r="PF48" s="0"/>
+      <c r="PG48" s="0"/>
+      <c r="PH48" s="0"/>
+      <c r="PI48" s="0"/>
+      <c r="PJ48" s="0"/>
+      <c r="PK48" s="0"/>
+      <c r="PL48" s="0"/>
+      <c r="PM48" s="0"/>
+      <c r="PN48" s="0"/>
+      <c r="PO48" s="0"/>
+      <c r="PP48" s="0"/>
+      <c r="PQ48" s="0"/>
+      <c r="PR48" s="0"/>
+      <c r="PS48" s="0"/>
+      <c r="PT48" s="0"/>
+      <c r="PU48" s="0"/>
+      <c r="PV48" s="0"/>
+      <c r="PW48" s="0"/>
+      <c r="PX48" s="0"/>
+      <c r="PY48" s="0"/>
+      <c r="PZ48" s="0"/>
+      <c r="QA48" s="0"/>
+      <c r="QB48" s="0"/>
+      <c r="QC48" s="0"/>
+      <c r="QD48" s="0"/>
+      <c r="QE48" s="0"/>
+      <c r="QF48" s="0"/>
+      <c r="QG48" s="0"/>
+      <c r="QH48" s="0"/>
+      <c r="QI48" s="0"/>
+      <c r="QJ48" s="0"/>
+      <c r="QK48" s="0"/>
+      <c r="QL48" s="0"/>
+      <c r="QM48" s="0"/>
+      <c r="QN48" s="0"/>
+      <c r="QO48" s="0"/>
+      <c r="QP48" s="0"/>
+      <c r="QQ48" s="0"/>
+      <c r="QR48" s="0"/>
+      <c r="QS48" s="0"/>
+      <c r="QT48" s="0"/>
+      <c r="QU48" s="0"/>
+      <c r="QV48" s="0"/>
+      <c r="QW48" s="0"/>
+      <c r="QX48" s="0"/>
+      <c r="QY48" s="0"/>
+      <c r="QZ48" s="0"/>
+      <c r="RA48" s="0"/>
+      <c r="RB48" s="0"/>
+      <c r="RC48" s="0"/>
+      <c r="RD48" s="0"/>
+      <c r="RE48" s="0"/>
+      <c r="RF48" s="0"/>
+      <c r="RG48" s="0"/>
+      <c r="RH48" s="0"/>
+      <c r="RI48" s="0"/>
+      <c r="RJ48" s="0"/>
+      <c r="RK48" s="0"/>
+      <c r="RL48" s="0"/>
+      <c r="RM48" s="0"/>
+      <c r="RN48" s="0"/>
+      <c r="RO48" s="0"/>
+      <c r="RP48" s="0"/>
+      <c r="RQ48" s="0"/>
+      <c r="RR48" s="0"/>
+      <c r="RS48" s="0"/>
+      <c r="RT48" s="0"/>
+      <c r="RU48" s="0"/>
+      <c r="RV48" s="0"/>
+      <c r="RW48" s="0"/>
+      <c r="RX48" s="0"/>
+      <c r="RY48" s="0"/>
+      <c r="RZ48" s="0"/>
+      <c r="SA48" s="0"/>
+      <c r="SB48" s="0"/>
+      <c r="SC48" s="0"/>
+      <c r="SD48" s="0"/>
+      <c r="SE48" s="0"/>
+      <c r="SF48" s="0"/>
+      <c r="SG48" s="0"/>
+      <c r="SH48" s="0"/>
+      <c r="SI48" s="0"/>
+      <c r="SJ48" s="0"/>
+      <c r="SK48" s="0"/>
+      <c r="SL48" s="0"/>
+      <c r="SM48" s="0"/>
+      <c r="SN48" s="0"/>
+      <c r="SO48" s="0"/>
+      <c r="SP48" s="0"/>
+      <c r="SQ48" s="0"/>
+      <c r="SR48" s="0"/>
+      <c r="SS48" s="0"/>
+      <c r="ST48" s="0"/>
+      <c r="SU48" s="0"/>
+      <c r="SV48" s="0"/>
+      <c r="SW48" s="0"/>
+      <c r="SX48" s="0"/>
+      <c r="SY48" s="0"/>
+      <c r="SZ48" s="0"/>
+      <c r="TA48" s="0"/>
+      <c r="TB48" s="0"/>
+      <c r="TC48" s="0"/>
+      <c r="TD48" s="0"/>
+      <c r="TE48" s="0"/>
+      <c r="TF48" s="0"/>
+      <c r="TG48" s="0"/>
+      <c r="TH48" s="0"/>
+      <c r="TI48" s="0"/>
+      <c r="TJ48" s="0"/>
+      <c r="TK48" s="0"/>
+      <c r="TL48" s="0"/>
+      <c r="TM48" s="0"/>
+      <c r="TN48" s="0"/>
+      <c r="TO48" s="0"/>
+      <c r="TP48" s="0"/>
+      <c r="TQ48" s="0"/>
+      <c r="TR48" s="0"/>
+      <c r="TS48" s="0"/>
+      <c r="TT48" s="0"/>
+      <c r="TU48" s="0"/>
+      <c r="TV48" s="0"/>
+      <c r="TW48" s="0"/>
+      <c r="TX48" s="0"/>
+      <c r="TY48" s="0"/>
+      <c r="TZ48" s="0"/>
+      <c r="UA48" s="0"/>
+      <c r="UB48" s="0"/>
+      <c r="UC48" s="0"/>
+      <c r="UD48" s="0"/>
+      <c r="UE48" s="0"/>
+      <c r="UF48" s="0"/>
+      <c r="UG48" s="0"/>
+      <c r="UH48" s="0"/>
+      <c r="UI48" s="0"/>
+      <c r="UJ48" s="0"/>
+      <c r="UK48" s="0"/>
+      <c r="UL48" s="0"/>
+      <c r="UM48" s="0"/>
+      <c r="UN48" s="0"/>
+      <c r="UO48" s="0"/>
+      <c r="UP48" s="0"/>
+      <c r="UQ48" s="0"/>
+      <c r="UR48" s="0"/>
+      <c r="US48" s="0"/>
+      <c r="UT48" s="0"/>
+      <c r="UU48" s="0"/>
+      <c r="UV48" s="0"/>
+      <c r="UW48" s="0"/>
+      <c r="UX48" s="0"/>
+      <c r="UY48" s="0"/>
+      <c r="UZ48" s="0"/>
+      <c r="VA48" s="0"/>
+      <c r="VB48" s="0"/>
+      <c r="VC48" s="0"/>
+      <c r="VD48" s="0"/>
+      <c r="VE48" s="0"/>
+      <c r="VF48" s="0"/>
+      <c r="VG48" s="0"/>
+      <c r="VH48" s="0"/>
+      <c r="VI48" s="0"/>
+      <c r="VJ48" s="0"/>
+      <c r="VK48" s="0"/>
+      <c r="VL48" s="0"/>
+      <c r="VM48" s="0"/>
+      <c r="VN48" s="0"/>
+      <c r="VO48" s="0"/>
+      <c r="VP48" s="0"/>
+      <c r="VQ48" s="0"/>
+      <c r="VR48" s="0"/>
+      <c r="VS48" s="0"/>
+      <c r="VT48" s="0"/>
+      <c r="VU48" s="0"/>
+      <c r="VV48" s="0"/>
+      <c r="VW48" s="0"/>
+      <c r="VX48" s="0"/>
+      <c r="VY48" s="0"/>
+      <c r="VZ48" s="0"/>
+      <c r="WA48" s="0"/>
+      <c r="WB48" s="0"/>
+      <c r="WC48" s="0"/>
+      <c r="WD48" s="0"/>
+      <c r="WE48" s="0"/>
+      <c r="WF48" s="0"/>
+      <c r="WG48" s="0"/>
+      <c r="WH48" s="0"/>
+      <c r="WI48" s="0"/>
+      <c r="WJ48" s="0"/>
+      <c r="WK48" s="0"/>
+      <c r="WL48" s="0"/>
+      <c r="WM48" s="0"/>
+      <c r="WN48" s="0"/>
+      <c r="WO48" s="0"/>
+      <c r="WP48" s="0"/>
+      <c r="WQ48" s="0"/>
+      <c r="WR48" s="0"/>
+      <c r="WS48" s="0"/>
+      <c r="WT48" s="0"/>
+      <c r="WU48" s="0"/>
+      <c r="WV48" s="0"/>
+      <c r="WW48" s="0"/>
+      <c r="WX48" s="0"/>
+      <c r="WY48" s="0"/>
+      <c r="WZ48" s="0"/>
+      <c r="XA48" s="0"/>
+      <c r="XB48" s="0"/>
+      <c r="XC48" s="0"/>
+      <c r="XD48" s="0"/>
+      <c r="XE48" s="0"/>
+      <c r="XF48" s="0"/>
+      <c r="XG48" s="0"/>
+      <c r="XH48" s="0"/>
+      <c r="XI48" s="0"/>
+      <c r="XJ48" s="0"/>
+      <c r="XK48" s="0"/>
+      <c r="XL48" s="0"/>
+      <c r="XM48" s="0"/>
+      <c r="XN48" s="0"/>
+      <c r="XO48" s="0"/>
+      <c r="XP48" s="0"/>
+      <c r="XQ48" s="0"/>
+      <c r="XR48" s="0"/>
+      <c r="XS48" s="0"/>
+      <c r="XT48" s="0"/>
+      <c r="XU48" s="0"/>
+      <c r="XV48" s="0"/>
+      <c r="XW48" s="0"/>
+      <c r="XX48" s="0"/>
+      <c r="XY48" s="0"/>
+      <c r="XZ48" s="0"/>
+      <c r="YA48" s="0"/>
+      <c r="YB48" s="0"/>
+      <c r="YC48" s="0"/>
+      <c r="YD48" s="0"/>
+      <c r="YE48" s="0"/>
+      <c r="YF48" s="0"/>
+      <c r="YG48" s="0"/>
+      <c r="YH48" s="0"/>
+      <c r="YI48" s="0"/>
+      <c r="YJ48" s="0"/>
+      <c r="YK48" s="0"/>
+      <c r="YL48" s="0"/>
+      <c r="YM48" s="0"/>
+      <c r="YN48" s="0"/>
+      <c r="YO48" s="0"/>
+      <c r="YP48" s="0"/>
+      <c r="YQ48" s="0"/>
+      <c r="YR48" s="0"/>
+      <c r="YS48" s="0"/>
+      <c r="YT48" s="0"/>
+      <c r="YU48" s="0"/>
+      <c r="YV48" s="0"/>
+      <c r="YW48" s="0"/>
+      <c r="YX48" s="0"/>
+      <c r="YY48" s="0"/>
+      <c r="YZ48" s="0"/>
+      <c r="ZA48" s="0"/>
+      <c r="ZB48" s="0"/>
+      <c r="ZC48" s="0"/>
+      <c r="ZD48" s="0"/>
+      <c r="ZE48" s="0"/>
+      <c r="ZF48" s="0"/>
+      <c r="ZG48" s="0"/>
+      <c r="ZH48" s="0"/>
+      <c r="ZI48" s="0"/>
+      <c r="ZJ48" s="0"/>
+      <c r="ZK48" s="0"/>
+      <c r="ZL48" s="0"/>
+      <c r="ZM48" s="0"/>
+      <c r="ZN48" s="0"/>
+      <c r="ZO48" s="0"/>
+      <c r="ZP48" s="0"/>
+      <c r="ZQ48" s="0"/>
+      <c r="ZR48" s="0"/>
+      <c r="ZS48" s="0"/>
+      <c r="ZT48" s="0"/>
+      <c r="ZU48" s="0"/>
+      <c r="ZV48" s="0"/>
+      <c r="ZW48" s="0"/>
+      <c r="ZX48" s="0"/>
+      <c r="ZY48" s="0"/>
+      <c r="ZZ48" s="0"/>
+      <c r="AAA48" s="0"/>
+      <c r="AAB48" s="0"/>
+      <c r="AAC48" s="0"/>
+      <c r="AAD48" s="0"/>
+      <c r="AAE48" s="0"/>
+      <c r="AAF48" s="0"/>
+      <c r="AAG48" s="0"/>
+      <c r="AAH48" s="0"/>
+      <c r="AAI48" s="0"/>
+      <c r="AAJ48" s="0"/>
+      <c r="AAK48" s="0"/>
+      <c r="AAL48" s="0"/>
+      <c r="AAM48" s="0"/>
+      <c r="AAN48" s="0"/>
+      <c r="AAO48" s="0"/>
+      <c r="AAP48" s="0"/>
+      <c r="AAQ48" s="0"/>
+      <c r="AAR48" s="0"/>
+      <c r="AAS48" s="0"/>
+      <c r="AAT48" s="0"/>
+      <c r="AAU48" s="0"/>
+      <c r="AAV48" s="0"/>
+      <c r="AAW48" s="0"/>
+      <c r="AAX48" s="0"/>
+      <c r="AAY48" s="0"/>
+      <c r="AAZ48" s="0"/>
+      <c r="ABA48" s="0"/>
+      <c r="ABB48" s="0"/>
+      <c r="ABC48" s="0"/>
+      <c r="ABD48" s="0"/>
+      <c r="ABE48" s="0"/>
+      <c r="ABF48" s="0"/>
+      <c r="ABG48" s="0"/>
+      <c r="ABH48" s="0"/>
+      <c r="ABI48" s="0"/>
+      <c r="ABJ48" s="0"/>
+      <c r="ABK48" s="0"/>
+      <c r="ABL48" s="0"/>
+      <c r="ABM48" s="0"/>
+      <c r="ABN48" s="0"/>
+      <c r="ABO48" s="0"/>
+      <c r="ABP48" s="0"/>
+      <c r="ABQ48" s="0"/>
+      <c r="ABR48" s="0"/>
+      <c r="ABS48" s="0"/>
+      <c r="ABT48" s="0"/>
+      <c r="ABU48" s="0"/>
+      <c r="ABV48" s="0"/>
+      <c r="ABW48" s="0"/>
+      <c r="ABX48" s="0"/>
+      <c r="ABY48" s="0"/>
+      <c r="ABZ48" s="0"/>
+      <c r="ACA48" s="0"/>
+      <c r="ACB48" s="0"/>
+      <c r="ACC48" s="0"/>
+      <c r="ACD48" s="0"/>
+      <c r="ACE48" s="0"/>
+      <c r="ACF48" s="0"/>
+      <c r="ACG48" s="0"/>
+      <c r="ACH48" s="0"/>
+      <c r="ACI48" s="0"/>
+      <c r="ACJ48" s="0"/>
+      <c r="ACK48" s="0"/>
+      <c r="ACL48" s="0"/>
+      <c r="ACM48" s="0"/>
+      <c r="ACN48" s="0"/>
+      <c r="ACO48" s="0"/>
+      <c r="ACP48" s="0"/>
+      <c r="ACQ48" s="0"/>
+      <c r="ACR48" s="0"/>
+      <c r="ACS48" s="0"/>
+      <c r="ACT48" s="0"/>
+      <c r="ACU48" s="0"/>
+      <c r="ACV48" s="0"/>
+      <c r="ACW48" s="0"/>
+      <c r="ACX48" s="0"/>
+      <c r="ACY48" s="0"/>
+      <c r="ACZ48" s="0"/>
+      <c r="ADA48" s="0"/>
+      <c r="ADB48" s="0"/>
+      <c r="ADC48" s="0"/>
+      <c r="ADD48" s="0"/>
+      <c r="ADE48" s="0"/>
+      <c r="ADF48" s="0"/>
+      <c r="ADG48" s="0"/>
+      <c r="ADH48" s="0"/>
+      <c r="ADI48" s="0"/>
+      <c r="ADJ48" s="0"/>
+      <c r="ADK48" s="0"/>
+      <c r="ADL48" s="0"/>
+      <c r="ADM48" s="0"/>
+      <c r="ADN48" s="0"/>
+      <c r="ADO48" s="0"/>
+      <c r="ADP48" s="0"/>
+      <c r="ADQ48" s="0"/>
+      <c r="ADR48" s="0"/>
+      <c r="ADS48" s="0"/>
+      <c r="ADT48" s="0"/>
+      <c r="ADU48" s="0"/>
+      <c r="ADV48" s="0"/>
+      <c r="ADW48" s="0"/>
+      <c r="ADX48" s="0"/>
+      <c r="ADY48" s="0"/>
+      <c r="ADZ48" s="0"/>
+      <c r="AEA48" s="0"/>
+      <c r="AEB48" s="0"/>
+      <c r="AEC48" s="0"/>
+      <c r="AED48" s="0"/>
+      <c r="AEE48" s="0"/>
+      <c r="AEF48" s="0"/>
+      <c r="AEG48" s="0"/>
+      <c r="AEH48" s="0"/>
+      <c r="AEI48" s="0"/>
+      <c r="AEJ48" s="0"/>
+      <c r="AEK48" s="0"/>
+      <c r="AEL48" s="0"/>
+      <c r="AEM48" s="0"/>
+      <c r="AEN48" s="0"/>
+      <c r="AEO48" s="0"/>
+      <c r="AEP48" s="0"/>
+      <c r="AEQ48" s="0"/>
+      <c r="AER48" s="0"/>
+      <c r="AES48" s="0"/>
+      <c r="AET48" s="0"/>
+      <c r="AEU48" s="0"/>
+      <c r="AEV48" s="0"/>
+      <c r="AEW48" s="0"/>
+      <c r="AEX48" s="0"/>
+      <c r="AEY48" s="0"/>
+      <c r="AEZ48" s="0"/>
+      <c r="AFA48" s="0"/>
+      <c r="AFB48" s="0"/>
+      <c r="AFC48" s="0"/>
+      <c r="AFD48" s="0"/>
+      <c r="AFE48" s="0"/>
+      <c r="AFF48" s="0"/>
+      <c r="AFG48" s="0"/>
+      <c r="AFH48" s="0"/>
+      <c r="AFI48" s="0"/>
+      <c r="AFJ48" s="0"/>
+      <c r="AFK48" s="0"/>
+      <c r="AFL48" s="0"/>
+      <c r="AFM48" s="0"/>
+      <c r="AFN48" s="0"/>
+      <c r="AFO48" s="0"/>
+      <c r="AFP48" s="0"/>
+      <c r="AFQ48" s="0"/>
+      <c r="AFR48" s="0"/>
+      <c r="AFS48" s="0"/>
+      <c r="AFT48" s="0"/>
+      <c r="AFU48" s="0"/>
+      <c r="AFV48" s="0"/>
+      <c r="AFW48" s="0"/>
+      <c r="AFX48" s="0"/>
+      <c r="AFY48" s="0"/>
+      <c r="AFZ48" s="0"/>
+      <c r="AGA48" s="0"/>
+      <c r="AGB48" s="0"/>
+      <c r="AGC48" s="0"/>
+      <c r="AGD48" s="0"/>
+      <c r="AGE48" s="0"/>
+      <c r="AGF48" s="0"/>
+      <c r="AGG48" s="0"/>
+      <c r="AGH48" s="0"/>
+      <c r="AGI48" s="0"/>
+      <c r="AGJ48" s="0"/>
+      <c r="AGK48" s="0"/>
+      <c r="AGL48" s="0"/>
+      <c r="AGM48" s="0"/>
+      <c r="AGN48" s="0"/>
+      <c r="AGO48" s="0"/>
+      <c r="AGP48" s="0"/>
+      <c r="AGQ48" s="0"/>
+      <c r="AGR48" s="0"/>
+      <c r="AGS48" s="0"/>
+      <c r="AGT48" s="0"/>
+      <c r="AGU48" s="0"/>
+      <c r="AGV48" s="0"/>
+      <c r="AGW48" s="0"/>
+      <c r="AGX48" s="0"/>
+      <c r="AGY48" s="0"/>
+      <c r="AGZ48" s="0"/>
+      <c r="AHA48" s="0"/>
+      <c r="AHB48" s="0"/>
+      <c r="AHC48" s="0"/>
+      <c r="AHD48" s="0"/>
+      <c r="AHE48" s="0"/>
+      <c r="AHF48" s="0"/>
+      <c r="AHG48" s="0"/>
+      <c r="AHH48" s="0"/>
+      <c r="AHI48" s="0"/>
+      <c r="AHJ48" s="0"/>
+      <c r="AHK48" s="0"/>
+      <c r="AHL48" s="0"/>
+      <c r="AHM48" s="0"/>
+      <c r="AHN48" s="0"/>
+      <c r="AHO48" s="0"/>
+      <c r="AHP48" s="0"/>
+      <c r="AHQ48" s="0"/>
+      <c r="AHR48" s="0"/>
+      <c r="AHS48" s="0"/>
+      <c r="AHT48" s="0"/>
+      <c r="AHU48" s="0"/>
+      <c r="AHV48" s="0"/>
+      <c r="AHW48" s="0"/>
+      <c r="AHX48" s="0"/>
+      <c r="AHY48" s="0"/>
+      <c r="AHZ48" s="0"/>
+      <c r="AIA48" s="0"/>
+      <c r="AIB48" s="0"/>
+      <c r="AIC48" s="0"/>
+      <c r="AID48" s="0"/>
+      <c r="AIE48" s="0"/>
+      <c r="AIF48" s="0"/>
+      <c r="AIG48" s="0"/>
+      <c r="AIH48" s="0"/>
+      <c r="AII48" s="0"/>
+      <c r="AIJ48" s="0"/>
+      <c r="AIK48" s="0"/>
+      <c r="AIL48" s="0"/>
+      <c r="AIM48" s="0"/>
+      <c r="AIN48" s="0"/>
+      <c r="AIO48" s="0"/>
+      <c r="AIP48" s="0"/>
+      <c r="AIQ48" s="0"/>
+      <c r="AIR48" s="0"/>
+      <c r="AIS48" s="0"/>
+      <c r="AIT48" s="0"/>
+      <c r="AIU48" s="0"/>
+      <c r="AIV48" s="0"/>
+      <c r="AIW48" s="0"/>
+      <c r="AIX48" s="0"/>
+      <c r="AIY48" s="0"/>
+      <c r="AIZ48" s="0"/>
+      <c r="AJA48" s="0"/>
+      <c r="AJB48" s="0"/>
+      <c r="AJC48" s="0"/>
+      <c r="AJD48" s="0"/>
+      <c r="AJE48" s="0"/>
+      <c r="AJF48" s="0"/>
+      <c r="AJG48" s="0"/>
+      <c r="AJH48" s="0"/>
+      <c r="AJI48" s="0"/>
+      <c r="AJJ48" s="0"/>
+      <c r="AJK48" s="0"/>
+      <c r="AJL48" s="0"/>
+      <c r="AJM48" s="0"/>
+      <c r="AJN48" s="0"/>
+      <c r="AJO48" s="0"/>
+      <c r="AJP48" s="0"/>
+      <c r="AJQ48" s="0"/>
+      <c r="AJR48" s="0"/>
+      <c r="AJS48" s="0"/>
+      <c r="AJT48" s="0"/>
+      <c r="AJU48" s="0"/>
+      <c r="AJV48" s="0"/>
+      <c r="AJW48" s="0"/>
+      <c r="AJX48" s="0"/>
+      <c r="AJY48" s="0"/>
+      <c r="AJZ48" s="0"/>
+      <c r="AKA48" s="0"/>
+      <c r="AKB48" s="0"/>
+      <c r="AKC48" s="0"/>
+      <c r="AKD48" s="0"/>
+      <c r="AKE48" s="0"/>
+      <c r="AKF48" s="0"/>
+      <c r="AKG48" s="0"/>
+      <c r="AKH48" s="0"/>
+      <c r="AKI48" s="0"/>
+      <c r="AKJ48" s="0"/>
+      <c r="AKK48" s="0"/>
+      <c r="AKL48" s="0"/>
+      <c r="AKM48" s="0"/>
+      <c r="AKN48" s="0"/>
+      <c r="AKO48" s="0"/>
+      <c r="AKP48" s="0"/>
+      <c r="AKQ48" s="0"/>
+      <c r="AKR48" s="0"/>
+      <c r="AKS48" s="0"/>
+      <c r="AKT48" s="0"/>
+      <c r="AKU48" s="0"/>
+      <c r="AKV48" s="0"/>
+      <c r="AKW48" s="0"/>
+      <c r="AKX48" s="0"/>
+      <c r="AKY48" s="0"/>
+      <c r="AKZ48" s="0"/>
+      <c r="ALA48" s="0"/>
+      <c r="ALB48" s="0"/>
+      <c r="ALC48" s="0"/>
+      <c r="ALD48" s="0"/>
+      <c r="ALE48" s="0"/>
+      <c r="ALF48" s="0"/>
+      <c r="ALG48" s="0"/>
+      <c r="ALH48" s="0"/>
+      <c r="ALI48" s="0"/>
+      <c r="ALJ48" s="0"/>
+      <c r="ALK48" s="0"/>
+      <c r="ALL48" s="0"/>
+      <c r="ALM48" s="0"/>
+      <c r="ALN48" s="0"/>
+      <c r="ALO48" s="0"/>
+      <c r="ALP48" s="0"/>
+      <c r="ALQ48" s="0"/>
+      <c r="ALR48" s="0"/>
+      <c r="ALS48" s="0"/>
+      <c r="ALT48" s="0"/>
+      <c r="ALU48" s="0"/>
+      <c r="ALV48" s="0"/>
+      <c r="ALW48" s="0"/>
+      <c r="ALX48" s="0"/>
+      <c r="ALY48" s="0"/>
+      <c r="ALZ48" s="0"/>
+      <c r="AMA48" s="0"/>
+      <c r="AMB48" s="0"/>
+      <c r="AMC48" s="0"/>
+      <c r="AMD48" s="0"/>
+      <c r="AME48" s="0"/>
+      <c r="AMF48" s="0"/>
+      <c r="AMG48" s="0"/>
+      <c r="AMH48" s="0"/>
+      <c r="AMI48" s="0"/>
+      <c r="AMJ48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="1" t="s">
-        <v>124</v>
+      <c r="A49" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="B50" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D50" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="B51" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6602,22 +7629,13 @@
         <v>56</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6625,16 +7643,19 @@
         <v>56</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6642,7 +7663,22 @@
         <v>56</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6650,95 +7686,1153 @@
         <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E55" s="7" t="s">
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E57" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>145</v>
+      <c r="F57" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F60" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F62" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G62" s="1" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>160</v>
       </c>
+      <c r="C64" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="0"/>
+      <c r="G65" s="0"/>
+      <c r="H65" s="0"/>
+      <c r="I65" s="0"/>
+      <c r="J65" s="0"/>
+      <c r="K65" s="0"/>
+      <c r="L65" s="0"/>
+      <c r="M65" s="0"/>
+      <c r="N65" s="0"/>
+      <c r="O65" s="0"/>
+      <c r="P65" s="0"/>
+      <c r="Q65" s="0"/>
+      <c r="R65" s="0"/>
+      <c r="S65" s="0"/>
+      <c r="T65" s="0"/>
+      <c r="U65" s="0"/>
+      <c r="V65" s="0"/>
+      <c r="W65" s="0"/>
+      <c r="X65" s="0"/>
+      <c r="Y65" s="0"/>
+      <c r="Z65" s="0"/>
+      <c r="AA65" s="0"/>
+      <c r="AB65" s="0"/>
+      <c r="AC65" s="0"/>
+      <c r="AD65" s="0"/>
+      <c r="AE65" s="0"/>
+      <c r="AF65" s="0"/>
+      <c r="AG65" s="0"/>
+      <c r="AH65" s="0"/>
+      <c r="AI65" s="0"/>
+      <c r="AJ65" s="0"/>
+      <c r="AK65" s="0"/>
+      <c r="AL65" s="0"/>
+      <c r="AM65" s="0"/>
+      <c r="AN65" s="0"/>
+      <c r="AO65" s="0"/>
+      <c r="AP65" s="0"/>
+      <c r="AQ65" s="0"/>
+      <c r="AR65" s="0"/>
+      <c r="AS65" s="0"/>
+      <c r="AT65" s="0"/>
+      <c r="AU65" s="0"/>
+      <c r="AV65" s="0"/>
+      <c r="AW65" s="0"/>
+      <c r="AX65" s="0"/>
+      <c r="AY65" s="0"/>
+      <c r="AZ65" s="0"/>
+      <c r="BA65" s="0"/>
+      <c r="BB65" s="0"/>
+      <c r="BC65" s="0"/>
+      <c r="BD65" s="0"/>
+      <c r="BE65" s="0"/>
+      <c r="BF65" s="0"/>
+      <c r="BG65" s="0"/>
+      <c r="BH65" s="0"/>
+      <c r="BI65" s="0"/>
+      <c r="BJ65" s="0"/>
+      <c r="BK65" s="0"/>
+      <c r="BL65" s="0"/>
+      <c r="BM65" s="0"/>
+      <c r="BN65" s="0"/>
+      <c r="BO65" s="0"/>
+      <c r="BP65" s="0"/>
+      <c r="BQ65" s="0"/>
+      <c r="BR65" s="0"/>
+      <c r="BS65" s="0"/>
+      <c r="BT65" s="0"/>
+      <c r="BU65" s="0"/>
+      <c r="BV65" s="0"/>
+      <c r="BW65" s="0"/>
+      <c r="BX65" s="0"/>
+      <c r="BY65" s="0"/>
+      <c r="BZ65" s="0"/>
+      <c r="CA65" s="0"/>
+      <c r="CB65" s="0"/>
+      <c r="CC65" s="0"/>
+      <c r="CD65" s="0"/>
+      <c r="CE65" s="0"/>
+      <c r="CF65" s="0"/>
+      <c r="CG65" s="0"/>
+      <c r="CH65" s="0"/>
+      <c r="CI65" s="0"/>
+      <c r="CJ65" s="0"/>
+      <c r="CK65" s="0"/>
+      <c r="CL65" s="0"/>
+      <c r="CM65" s="0"/>
+      <c r="CN65" s="0"/>
+      <c r="CO65" s="0"/>
+      <c r="CP65" s="0"/>
+      <c r="CQ65" s="0"/>
+      <c r="CR65" s="0"/>
+      <c r="CS65" s="0"/>
+      <c r="CT65" s="0"/>
+      <c r="CU65" s="0"/>
+      <c r="CV65" s="0"/>
+      <c r="CW65" s="0"/>
+      <c r="CX65" s="0"/>
+      <c r="CY65" s="0"/>
+      <c r="CZ65" s="0"/>
+      <c r="DA65" s="0"/>
+      <c r="DB65" s="0"/>
+      <c r="DC65" s="0"/>
+      <c r="DD65" s="0"/>
+      <c r="DE65" s="0"/>
+      <c r="DF65" s="0"/>
+      <c r="DG65" s="0"/>
+      <c r="DH65" s="0"/>
+      <c r="DI65" s="0"/>
+      <c r="DJ65" s="0"/>
+      <c r="DK65" s="0"/>
+      <c r="DL65" s="0"/>
+      <c r="DM65" s="0"/>
+      <c r="DN65" s="0"/>
+      <c r="DO65" s="0"/>
+      <c r="DP65" s="0"/>
+      <c r="DQ65" s="0"/>
+      <c r="DR65" s="0"/>
+      <c r="DS65" s="0"/>
+      <c r="DT65" s="0"/>
+      <c r="DU65" s="0"/>
+      <c r="DV65" s="0"/>
+      <c r="DW65" s="0"/>
+      <c r="DX65" s="0"/>
+      <c r="DY65" s="0"/>
+      <c r="DZ65" s="0"/>
+      <c r="EA65" s="0"/>
+      <c r="EB65" s="0"/>
+      <c r="EC65" s="0"/>
+      <c r="ED65" s="0"/>
+      <c r="EE65" s="0"/>
+      <c r="EF65" s="0"/>
+      <c r="EG65" s="0"/>
+      <c r="EH65" s="0"/>
+      <c r="EI65" s="0"/>
+      <c r="EJ65" s="0"/>
+      <c r="EK65" s="0"/>
+      <c r="EL65" s="0"/>
+      <c r="EM65" s="0"/>
+      <c r="EN65" s="0"/>
+      <c r="EO65" s="0"/>
+      <c r="EP65" s="0"/>
+      <c r="EQ65" s="0"/>
+      <c r="ER65" s="0"/>
+      <c r="ES65" s="0"/>
+      <c r="ET65" s="0"/>
+      <c r="EU65" s="0"/>
+      <c r="EV65" s="0"/>
+      <c r="EW65" s="0"/>
+      <c r="EX65" s="0"/>
+      <c r="EY65" s="0"/>
+      <c r="EZ65" s="0"/>
+      <c r="FA65" s="0"/>
+      <c r="FB65" s="0"/>
+      <c r="FC65" s="0"/>
+      <c r="FD65" s="0"/>
+      <c r="FE65" s="0"/>
+      <c r="FF65" s="0"/>
+      <c r="FG65" s="0"/>
+      <c r="FH65" s="0"/>
+      <c r="FI65" s="0"/>
+      <c r="FJ65" s="0"/>
+      <c r="FK65" s="0"/>
+      <c r="FL65" s="0"/>
+      <c r="FM65" s="0"/>
+      <c r="FN65" s="0"/>
+      <c r="FO65" s="0"/>
+      <c r="FP65" s="0"/>
+      <c r="FQ65" s="0"/>
+      <c r="FR65" s="0"/>
+      <c r="FS65" s="0"/>
+      <c r="FT65" s="0"/>
+      <c r="FU65" s="0"/>
+      <c r="FV65" s="0"/>
+      <c r="FW65" s="0"/>
+      <c r="FX65" s="0"/>
+      <c r="FY65" s="0"/>
+      <c r="FZ65" s="0"/>
+      <c r="GA65" s="0"/>
+      <c r="GB65" s="0"/>
+      <c r="GC65" s="0"/>
+      <c r="GD65" s="0"/>
+      <c r="GE65" s="0"/>
+      <c r="GF65" s="0"/>
+      <c r="GG65" s="0"/>
+      <c r="GH65" s="0"/>
+      <c r="GI65" s="0"/>
+      <c r="GJ65" s="0"/>
+      <c r="GK65" s="0"/>
+      <c r="GL65" s="0"/>
+      <c r="GM65" s="0"/>
+      <c r="GN65" s="0"/>
+      <c r="GO65" s="0"/>
+      <c r="GP65" s="0"/>
+      <c r="GQ65" s="0"/>
+      <c r="GR65" s="0"/>
+      <c r="GS65" s="0"/>
+      <c r="GT65" s="0"/>
+      <c r="GU65" s="0"/>
+      <c r="GV65" s="0"/>
+      <c r="GW65" s="0"/>
+      <c r="GX65" s="0"/>
+      <c r="GY65" s="0"/>
+      <c r="GZ65" s="0"/>
+      <c r="HA65" s="0"/>
+      <c r="HB65" s="0"/>
+      <c r="HC65" s="0"/>
+      <c r="HD65" s="0"/>
+      <c r="HE65" s="0"/>
+      <c r="HF65" s="0"/>
+      <c r="HG65" s="0"/>
+      <c r="HH65" s="0"/>
+      <c r="HI65" s="0"/>
+      <c r="HJ65" s="0"/>
+      <c r="HK65" s="0"/>
+      <c r="HL65" s="0"/>
+      <c r="HM65" s="0"/>
+      <c r="HN65" s="0"/>
+      <c r="HO65" s="0"/>
+      <c r="HP65" s="0"/>
+      <c r="HQ65" s="0"/>
+      <c r="HR65" s="0"/>
+      <c r="HS65" s="0"/>
+      <c r="HT65" s="0"/>
+      <c r="HU65" s="0"/>
+      <c r="HV65" s="0"/>
+      <c r="HW65" s="0"/>
+      <c r="HX65" s="0"/>
+      <c r="HY65" s="0"/>
+      <c r="HZ65" s="0"/>
+      <c r="IA65" s="0"/>
+      <c r="IB65" s="0"/>
+      <c r="IC65" s="0"/>
+      <c r="ID65" s="0"/>
+      <c r="IE65" s="0"/>
+      <c r="IF65" s="0"/>
+      <c r="IG65" s="0"/>
+      <c r="IH65" s="0"/>
+      <c r="II65" s="0"/>
+      <c r="IJ65" s="0"/>
+      <c r="IK65" s="0"/>
+      <c r="IL65" s="0"/>
+      <c r="IM65" s="0"/>
+      <c r="IN65" s="0"/>
+      <c r="IO65" s="0"/>
+      <c r="IP65" s="0"/>
+      <c r="IQ65" s="0"/>
+      <c r="IR65" s="0"/>
+      <c r="IS65" s="0"/>
+      <c r="IT65" s="0"/>
+      <c r="IU65" s="0"/>
+      <c r="IV65" s="0"/>
+      <c r="IW65" s="0"/>
+      <c r="IX65" s="0"/>
+      <c r="IY65" s="0"/>
+      <c r="IZ65" s="0"/>
+      <c r="JA65" s="0"/>
+      <c r="JB65" s="0"/>
+      <c r="JC65" s="0"/>
+      <c r="JD65" s="0"/>
+      <c r="JE65" s="0"/>
+      <c r="JF65" s="0"/>
+      <c r="JG65" s="0"/>
+      <c r="JH65" s="0"/>
+      <c r="JI65" s="0"/>
+      <c r="JJ65" s="0"/>
+      <c r="JK65" s="0"/>
+      <c r="JL65" s="0"/>
+      <c r="JM65" s="0"/>
+      <c r="JN65" s="0"/>
+      <c r="JO65" s="0"/>
+      <c r="JP65" s="0"/>
+      <c r="JQ65" s="0"/>
+      <c r="JR65" s="0"/>
+      <c r="JS65" s="0"/>
+      <c r="JT65" s="0"/>
+      <c r="JU65" s="0"/>
+      <c r="JV65" s="0"/>
+      <c r="JW65" s="0"/>
+      <c r="JX65" s="0"/>
+      <c r="JY65" s="0"/>
+      <c r="JZ65" s="0"/>
+      <c r="KA65" s="0"/>
+      <c r="KB65" s="0"/>
+      <c r="KC65" s="0"/>
+      <c r="KD65" s="0"/>
+      <c r="KE65" s="0"/>
+      <c r="KF65" s="0"/>
+      <c r="KG65" s="0"/>
+      <c r="KH65" s="0"/>
+      <c r="KI65" s="0"/>
+      <c r="KJ65" s="0"/>
+      <c r="KK65" s="0"/>
+      <c r="KL65" s="0"/>
+      <c r="KM65" s="0"/>
+      <c r="KN65" s="0"/>
+      <c r="KO65" s="0"/>
+      <c r="KP65" s="0"/>
+      <c r="KQ65" s="0"/>
+      <c r="KR65" s="0"/>
+      <c r="KS65" s="0"/>
+      <c r="KT65" s="0"/>
+      <c r="KU65" s="0"/>
+      <c r="KV65" s="0"/>
+      <c r="KW65" s="0"/>
+      <c r="KX65" s="0"/>
+      <c r="KY65" s="0"/>
+      <c r="KZ65" s="0"/>
+      <c r="LA65" s="0"/>
+      <c r="LB65" s="0"/>
+      <c r="LC65" s="0"/>
+      <c r="LD65" s="0"/>
+      <c r="LE65" s="0"/>
+      <c r="LF65" s="0"/>
+      <c r="LG65" s="0"/>
+      <c r="LH65" s="0"/>
+      <c r="LI65" s="0"/>
+      <c r="LJ65" s="0"/>
+      <c r="LK65" s="0"/>
+      <c r="LL65" s="0"/>
+      <c r="LM65" s="0"/>
+      <c r="LN65" s="0"/>
+      <c r="LO65" s="0"/>
+      <c r="LP65" s="0"/>
+      <c r="LQ65" s="0"/>
+      <c r="LR65" s="0"/>
+      <c r="LS65" s="0"/>
+      <c r="LT65" s="0"/>
+      <c r="LU65" s="0"/>
+      <c r="LV65" s="0"/>
+      <c r="LW65" s="0"/>
+      <c r="LX65" s="0"/>
+      <c r="LY65" s="0"/>
+      <c r="LZ65" s="0"/>
+      <c r="MA65" s="0"/>
+      <c r="MB65" s="0"/>
+      <c r="MC65" s="0"/>
+      <c r="MD65" s="0"/>
+      <c r="ME65" s="0"/>
+      <c r="MF65" s="0"/>
+      <c r="MG65" s="0"/>
+      <c r="MH65" s="0"/>
+      <c r="MI65" s="0"/>
+      <c r="MJ65" s="0"/>
+      <c r="MK65" s="0"/>
+      <c r="ML65" s="0"/>
+      <c r="MM65" s="0"/>
+      <c r="MN65" s="0"/>
+      <c r="MO65" s="0"/>
+      <c r="MP65" s="0"/>
+      <c r="MQ65" s="0"/>
+      <c r="MR65" s="0"/>
+      <c r="MS65" s="0"/>
+      <c r="MT65" s="0"/>
+      <c r="MU65" s="0"/>
+      <c r="MV65" s="0"/>
+      <c r="MW65" s="0"/>
+      <c r="MX65" s="0"/>
+      <c r="MY65" s="0"/>
+      <c r="MZ65" s="0"/>
+      <c r="NA65" s="0"/>
+      <c r="NB65" s="0"/>
+      <c r="NC65" s="0"/>
+      <c r="ND65" s="0"/>
+      <c r="NE65" s="0"/>
+      <c r="NF65" s="0"/>
+      <c r="NG65" s="0"/>
+      <c r="NH65" s="0"/>
+      <c r="NI65" s="0"/>
+      <c r="NJ65" s="0"/>
+      <c r="NK65" s="0"/>
+      <c r="NL65" s="0"/>
+      <c r="NM65" s="0"/>
+      <c r="NN65" s="0"/>
+      <c r="NO65" s="0"/>
+      <c r="NP65" s="0"/>
+      <c r="NQ65" s="0"/>
+      <c r="NR65" s="0"/>
+      <c r="NS65" s="0"/>
+      <c r="NT65" s="0"/>
+      <c r="NU65" s="0"/>
+      <c r="NV65" s="0"/>
+      <c r="NW65" s="0"/>
+      <c r="NX65" s="0"/>
+      <c r="NY65" s="0"/>
+      <c r="NZ65" s="0"/>
+      <c r="OA65" s="0"/>
+      <c r="OB65" s="0"/>
+      <c r="OC65" s="0"/>
+      <c r="OD65" s="0"/>
+      <c r="OE65" s="0"/>
+      <c r="OF65" s="0"/>
+      <c r="OG65" s="0"/>
+      <c r="OH65" s="0"/>
+      <c r="OI65" s="0"/>
+      <c r="OJ65" s="0"/>
+      <c r="OK65" s="0"/>
+      <c r="OL65" s="0"/>
+      <c r="OM65" s="0"/>
+      <c r="ON65" s="0"/>
+      <c r="OO65" s="0"/>
+      <c r="OP65" s="0"/>
+      <c r="OQ65" s="0"/>
+      <c r="OR65" s="0"/>
+      <c r="OS65" s="0"/>
+      <c r="OT65" s="0"/>
+      <c r="OU65" s="0"/>
+      <c r="OV65" s="0"/>
+      <c r="OW65" s="0"/>
+      <c r="OX65" s="0"/>
+      <c r="OY65" s="0"/>
+      <c r="OZ65" s="0"/>
+      <c r="PA65" s="0"/>
+      <c r="PB65" s="0"/>
+      <c r="PC65" s="0"/>
+      <c r="PD65" s="0"/>
+      <c r="PE65" s="0"/>
+      <c r="PF65" s="0"/>
+      <c r="PG65" s="0"/>
+      <c r="PH65" s="0"/>
+      <c r="PI65" s="0"/>
+      <c r="PJ65" s="0"/>
+      <c r="PK65" s="0"/>
+      <c r="PL65" s="0"/>
+      <c r="PM65" s="0"/>
+      <c r="PN65" s="0"/>
+      <c r="PO65" s="0"/>
+      <c r="PP65" s="0"/>
+      <c r="PQ65" s="0"/>
+      <c r="PR65" s="0"/>
+      <c r="PS65" s="0"/>
+      <c r="PT65" s="0"/>
+      <c r="PU65" s="0"/>
+      <c r="PV65" s="0"/>
+      <c r="PW65" s="0"/>
+      <c r="PX65" s="0"/>
+      <c r="PY65" s="0"/>
+      <c r="PZ65" s="0"/>
+      <c r="QA65" s="0"/>
+      <c r="QB65" s="0"/>
+      <c r="QC65" s="0"/>
+      <c r="QD65" s="0"/>
+      <c r="QE65" s="0"/>
+      <c r="QF65" s="0"/>
+      <c r="QG65" s="0"/>
+      <c r="QH65" s="0"/>
+      <c r="QI65" s="0"/>
+      <c r="QJ65" s="0"/>
+      <c r="QK65" s="0"/>
+      <c r="QL65" s="0"/>
+      <c r="QM65" s="0"/>
+      <c r="QN65" s="0"/>
+      <c r="QO65" s="0"/>
+      <c r="QP65" s="0"/>
+      <c r="QQ65" s="0"/>
+      <c r="QR65" s="0"/>
+      <c r="QS65" s="0"/>
+      <c r="QT65" s="0"/>
+      <c r="QU65" s="0"/>
+      <c r="QV65" s="0"/>
+      <c r="QW65" s="0"/>
+      <c r="QX65" s="0"/>
+      <c r="QY65" s="0"/>
+      <c r="QZ65" s="0"/>
+      <c r="RA65" s="0"/>
+      <c r="RB65" s="0"/>
+      <c r="RC65" s="0"/>
+      <c r="RD65" s="0"/>
+      <c r="RE65" s="0"/>
+      <c r="RF65" s="0"/>
+      <c r="RG65" s="0"/>
+      <c r="RH65" s="0"/>
+      <c r="RI65" s="0"/>
+      <c r="RJ65" s="0"/>
+      <c r="RK65" s="0"/>
+      <c r="RL65" s="0"/>
+      <c r="RM65" s="0"/>
+      <c r="RN65" s="0"/>
+      <c r="RO65" s="0"/>
+      <c r="RP65" s="0"/>
+      <c r="RQ65" s="0"/>
+      <c r="RR65" s="0"/>
+      <c r="RS65" s="0"/>
+      <c r="RT65" s="0"/>
+      <c r="RU65" s="0"/>
+      <c r="RV65" s="0"/>
+      <c r="RW65" s="0"/>
+      <c r="RX65" s="0"/>
+      <c r="RY65" s="0"/>
+      <c r="RZ65" s="0"/>
+      <c r="SA65" s="0"/>
+      <c r="SB65" s="0"/>
+      <c r="SC65" s="0"/>
+      <c r="SD65" s="0"/>
+      <c r="SE65" s="0"/>
+      <c r="SF65" s="0"/>
+      <c r="SG65" s="0"/>
+      <c r="SH65" s="0"/>
+      <c r="SI65" s="0"/>
+      <c r="SJ65" s="0"/>
+      <c r="SK65" s="0"/>
+      <c r="SL65" s="0"/>
+      <c r="SM65" s="0"/>
+      <c r="SN65" s="0"/>
+      <c r="SO65" s="0"/>
+      <c r="SP65" s="0"/>
+      <c r="SQ65" s="0"/>
+      <c r="SR65" s="0"/>
+      <c r="SS65" s="0"/>
+      <c r="ST65" s="0"/>
+      <c r="SU65" s="0"/>
+      <c r="SV65" s="0"/>
+      <c r="SW65" s="0"/>
+      <c r="SX65" s="0"/>
+      <c r="SY65" s="0"/>
+      <c r="SZ65" s="0"/>
+      <c r="TA65" s="0"/>
+      <c r="TB65" s="0"/>
+      <c r="TC65" s="0"/>
+      <c r="TD65" s="0"/>
+      <c r="TE65" s="0"/>
+      <c r="TF65" s="0"/>
+      <c r="TG65" s="0"/>
+      <c r="TH65" s="0"/>
+      <c r="TI65" s="0"/>
+      <c r="TJ65" s="0"/>
+      <c r="TK65" s="0"/>
+      <c r="TL65" s="0"/>
+      <c r="TM65" s="0"/>
+      <c r="TN65" s="0"/>
+      <c r="TO65" s="0"/>
+      <c r="TP65" s="0"/>
+      <c r="TQ65" s="0"/>
+      <c r="TR65" s="0"/>
+      <c r="TS65" s="0"/>
+      <c r="TT65" s="0"/>
+      <c r="TU65" s="0"/>
+      <c r="TV65" s="0"/>
+      <c r="TW65" s="0"/>
+      <c r="TX65" s="0"/>
+      <c r="TY65" s="0"/>
+      <c r="TZ65" s="0"/>
+      <c r="UA65" s="0"/>
+      <c r="UB65" s="0"/>
+      <c r="UC65" s="0"/>
+      <c r="UD65" s="0"/>
+      <c r="UE65" s="0"/>
+      <c r="UF65" s="0"/>
+      <c r="UG65" s="0"/>
+      <c r="UH65" s="0"/>
+      <c r="UI65" s="0"/>
+      <c r="UJ65" s="0"/>
+      <c r="UK65" s="0"/>
+      <c r="UL65" s="0"/>
+      <c r="UM65" s="0"/>
+      <c r="UN65" s="0"/>
+      <c r="UO65" s="0"/>
+      <c r="UP65" s="0"/>
+      <c r="UQ65" s="0"/>
+      <c r="UR65" s="0"/>
+      <c r="US65" s="0"/>
+      <c r="UT65" s="0"/>
+      <c r="UU65" s="0"/>
+      <c r="UV65" s="0"/>
+      <c r="UW65" s="0"/>
+      <c r="UX65" s="0"/>
+      <c r="UY65" s="0"/>
+      <c r="UZ65" s="0"/>
+      <c r="VA65" s="0"/>
+      <c r="VB65" s="0"/>
+      <c r="VC65" s="0"/>
+      <c r="VD65" s="0"/>
+      <c r="VE65" s="0"/>
+      <c r="VF65" s="0"/>
+      <c r="VG65" s="0"/>
+      <c r="VH65" s="0"/>
+      <c r="VI65" s="0"/>
+      <c r="VJ65" s="0"/>
+      <c r="VK65" s="0"/>
+      <c r="VL65" s="0"/>
+      <c r="VM65" s="0"/>
+      <c r="VN65" s="0"/>
+      <c r="VO65" s="0"/>
+      <c r="VP65" s="0"/>
+      <c r="VQ65" s="0"/>
+      <c r="VR65" s="0"/>
+      <c r="VS65" s="0"/>
+      <c r="VT65" s="0"/>
+      <c r="VU65" s="0"/>
+      <c r="VV65" s="0"/>
+      <c r="VW65" s="0"/>
+      <c r="VX65" s="0"/>
+      <c r="VY65" s="0"/>
+      <c r="VZ65" s="0"/>
+      <c r="WA65" s="0"/>
+      <c r="WB65" s="0"/>
+      <c r="WC65" s="0"/>
+      <c r="WD65" s="0"/>
+      <c r="WE65" s="0"/>
+      <c r="WF65" s="0"/>
+      <c r="WG65" s="0"/>
+      <c r="WH65" s="0"/>
+      <c r="WI65" s="0"/>
+      <c r="WJ65" s="0"/>
+      <c r="WK65" s="0"/>
+      <c r="WL65" s="0"/>
+      <c r="WM65" s="0"/>
+      <c r="WN65" s="0"/>
+      <c r="WO65" s="0"/>
+      <c r="WP65" s="0"/>
+      <c r="WQ65" s="0"/>
+      <c r="WR65" s="0"/>
+      <c r="WS65" s="0"/>
+      <c r="WT65" s="0"/>
+      <c r="WU65" s="0"/>
+      <c r="WV65" s="0"/>
+      <c r="WW65" s="0"/>
+      <c r="WX65" s="0"/>
+      <c r="WY65" s="0"/>
+      <c r="WZ65" s="0"/>
+      <c r="XA65" s="0"/>
+      <c r="XB65" s="0"/>
+      <c r="XC65" s="0"/>
+      <c r="XD65" s="0"/>
+      <c r="XE65" s="0"/>
+      <c r="XF65" s="0"/>
+      <c r="XG65" s="0"/>
+      <c r="XH65" s="0"/>
+      <c r="XI65" s="0"/>
+      <c r="XJ65" s="0"/>
+      <c r="XK65" s="0"/>
+      <c r="XL65" s="0"/>
+      <c r="XM65" s="0"/>
+      <c r="XN65" s="0"/>
+      <c r="XO65" s="0"/>
+      <c r="XP65" s="0"/>
+      <c r="XQ65" s="0"/>
+      <c r="XR65" s="0"/>
+      <c r="XS65" s="0"/>
+      <c r="XT65" s="0"/>
+      <c r="XU65" s="0"/>
+      <c r="XV65" s="0"/>
+      <c r="XW65" s="0"/>
+      <c r="XX65" s="0"/>
+      <c r="XY65" s="0"/>
+      <c r="XZ65" s="0"/>
+      <c r="YA65" s="0"/>
+      <c r="YB65" s="0"/>
+      <c r="YC65" s="0"/>
+      <c r="YD65" s="0"/>
+      <c r="YE65" s="0"/>
+      <c r="YF65" s="0"/>
+      <c r="YG65" s="0"/>
+      <c r="YH65" s="0"/>
+      <c r="YI65" s="0"/>
+      <c r="YJ65" s="0"/>
+      <c r="YK65" s="0"/>
+      <c r="YL65" s="0"/>
+      <c r="YM65" s="0"/>
+      <c r="YN65" s="0"/>
+      <c r="YO65" s="0"/>
+      <c r="YP65" s="0"/>
+      <c r="YQ65" s="0"/>
+      <c r="YR65" s="0"/>
+      <c r="YS65" s="0"/>
+      <c r="YT65" s="0"/>
+      <c r="YU65" s="0"/>
+      <c r="YV65" s="0"/>
+      <c r="YW65" s="0"/>
+      <c r="YX65" s="0"/>
+      <c r="YY65" s="0"/>
+      <c r="YZ65" s="0"/>
+      <c r="ZA65" s="0"/>
+      <c r="ZB65" s="0"/>
+      <c r="ZC65" s="0"/>
+      <c r="ZD65" s="0"/>
+      <c r="ZE65" s="0"/>
+      <c r="ZF65" s="0"/>
+      <c r="ZG65" s="0"/>
+      <c r="ZH65" s="0"/>
+      <c r="ZI65" s="0"/>
+      <c r="ZJ65" s="0"/>
+      <c r="ZK65" s="0"/>
+      <c r="ZL65" s="0"/>
+      <c r="ZM65" s="0"/>
+      <c r="ZN65" s="0"/>
+      <c r="ZO65" s="0"/>
+      <c r="ZP65" s="0"/>
+      <c r="ZQ65" s="0"/>
+      <c r="ZR65" s="0"/>
+      <c r="ZS65" s="0"/>
+      <c r="ZT65" s="0"/>
+      <c r="ZU65" s="0"/>
+      <c r="ZV65" s="0"/>
+      <c r="ZW65" s="0"/>
+      <c r="ZX65" s="0"/>
+      <c r="ZY65" s="0"/>
+      <c r="ZZ65" s="0"/>
+      <c r="AAA65" s="0"/>
+      <c r="AAB65" s="0"/>
+      <c r="AAC65" s="0"/>
+      <c r="AAD65" s="0"/>
+      <c r="AAE65" s="0"/>
+      <c r="AAF65" s="0"/>
+      <c r="AAG65" s="0"/>
+      <c r="AAH65" s="0"/>
+      <c r="AAI65" s="0"/>
+      <c r="AAJ65" s="0"/>
+      <c r="AAK65" s="0"/>
+      <c r="AAL65" s="0"/>
+      <c r="AAM65" s="0"/>
+      <c r="AAN65" s="0"/>
+      <c r="AAO65" s="0"/>
+      <c r="AAP65" s="0"/>
+      <c r="AAQ65" s="0"/>
+      <c r="AAR65" s="0"/>
+      <c r="AAS65" s="0"/>
+      <c r="AAT65" s="0"/>
+      <c r="AAU65" s="0"/>
+      <c r="AAV65" s="0"/>
+      <c r="AAW65" s="0"/>
+      <c r="AAX65" s="0"/>
+      <c r="AAY65" s="0"/>
+      <c r="AAZ65" s="0"/>
+      <c r="ABA65" s="0"/>
+      <c r="ABB65" s="0"/>
+      <c r="ABC65" s="0"/>
+      <c r="ABD65" s="0"/>
+      <c r="ABE65" s="0"/>
+      <c r="ABF65" s="0"/>
+      <c r="ABG65" s="0"/>
+      <c r="ABH65" s="0"/>
+      <c r="ABI65" s="0"/>
+      <c r="ABJ65" s="0"/>
+      <c r="ABK65" s="0"/>
+      <c r="ABL65" s="0"/>
+      <c r="ABM65" s="0"/>
+      <c r="ABN65" s="0"/>
+      <c r="ABO65" s="0"/>
+      <c r="ABP65" s="0"/>
+      <c r="ABQ65" s="0"/>
+      <c r="ABR65" s="0"/>
+      <c r="ABS65" s="0"/>
+      <c r="ABT65" s="0"/>
+      <c r="ABU65" s="0"/>
+      <c r="ABV65" s="0"/>
+      <c r="ABW65" s="0"/>
+      <c r="ABX65" s="0"/>
+      <c r="ABY65" s="0"/>
+      <c r="ABZ65" s="0"/>
+      <c r="ACA65" s="0"/>
+      <c r="ACB65" s="0"/>
+      <c r="ACC65" s="0"/>
+      <c r="ACD65" s="0"/>
+      <c r="ACE65" s="0"/>
+      <c r="ACF65" s="0"/>
+      <c r="ACG65" s="0"/>
+      <c r="ACH65" s="0"/>
+      <c r="ACI65" s="0"/>
+      <c r="ACJ65" s="0"/>
+      <c r="ACK65" s="0"/>
+      <c r="ACL65" s="0"/>
+      <c r="ACM65" s="0"/>
+      <c r="ACN65" s="0"/>
+      <c r="ACO65" s="0"/>
+      <c r="ACP65" s="0"/>
+      <c r="ACQ65" s="0"/>
+      <c r="ACR65" s="0"/>
+      <c r="ACS65" s="0"/>
+      <c r="ACT65" s="0"/>
+      <c r="ACU65" s="0"/>
+      <c r="ACV65" s="0"/>
+      <c r="ACW65" s="0"/>
+      <c r="ACX65" s="0"/>
+      <c r="ACY65" s="0"/>
+      <c r="ACZ65" s="0"/>
+      <c r="ADA65" s="0"/>
+      <c r="ADB65" s="0"/>
+      <c r="ADC65" s="0"/>
+      <c r="ADD65" s="0"/>
+      <c r="ADE65" s="0"/>
+      <c r="ADF65" s="0"/>
+      <c r="ADG65" s="0"/>
+      <c r="ADH65" s="0"/>
+      <c r="ADI65" s="0"/>
+      <c r="ADJ65" s="0"/>
+      <c r="ADK65" s="0"/>
+      <c r="ADL65" s="0"/>
+      <c r="ADM65" s="0"/>
+      <c r="ADN65" s="0"/>
+      <c r="ADO65" s="0"/>
+      <c r="ADP65" s="0"/>
+      <c r="ADQ65" s="0"/>
+      <c r="ADR65" s="0"/>
+      <c r="ADS65" s="0"/>
+      <c r="ADT65" s="0"/>
+      <c r="ADU65" s="0"/>
+      <c r="ADV65" s="0"/>
+      <c r="ADW65" s="0"/>
+      <c r="ADX65" s="0"/>
+      <c r="ADY65" s="0"/>
+      <c r="ADZ65" s="0"/>
+      <c r="AEA65" s="0"/>
+      <c r="AEB65" s="0"/>
+      <c r="AEC65" s="0"/>
+      <c r="AED65" s="0"/>
+      <c r="AEE65" s="0"/>
+      <c r="AEF65" s="0"/>
+      <c r="AEG65" s="0"/>
+      <c r="AEH65" s="0"/>
+      <c r="AEI65" s="0"/>
+      <c r="AEJ65" s="0"/>
+      <c r="AEK65" s="0"/>
+      <c r="AEL65" s="0"/>
+      <c r="AEM65" s="0"/>
+      <c r="AEN65" s="0"/>
+      <c r="AEO65" s="0"/>
+      <c r="AEP65" s="0"/>
+      <c r="AEQ65" s="0"/>
+      <c r="AER65" s="0"/>
+      <c r="AES65" s="0"/>
+      <c r="AET65" s="0"/>
+      <c r="AEU65" s="0"/>
+      <c r="AEV65" s="0"/>
+      <c r="AEW65" s="0"/>
+      <c r="AEX65" s="0"/>
+      <c r="AEY65" s="0"/>
+      <c r="AEZ65" s="0"/>
+      <c r="AFA65" s="0"/>
+      <c r="AFB65" s="0"/>
+      <c r="AFC65" s="0"/>
+      <c r="AFD65" s="0"/>
+      <c r="AFE65" s="0"/>
+      <c r="AFF65" s="0"/>
+      <c r="AFG65" s="0"/>
+      <c r="AFH65" s="0"/>
+      <c r="AFI65" s="0"/>
+      <c r="AFJ65" s="0"/>
+      <c r="AFK65" s="0"/>
+      <c r="AFL65" s="0"/>
+      <c r="AFM65" s="0"/>
+      <c r="AFN65" s="0"/>
+      <c r="AFO65" s="0"/>
+      <c r="AFP65" s="0"/>
+      <c r="AFQ65" s="0"/>
+      <c r="AFR65" s="0"/>
+      <c r="AFS65" s="0"/>
+      <c r="AFT65" s="0"/>
+      <c r="AFU65" s="0"/>
+      <c r="AFV65" s="0"/>
+      <c r="AFW65" s="0"/>
+      <c r="AFX65" s="0"/>
+      <c r="AFY65" s="0"/>
+      <c r="AFZ65" s="0"/>
+      <c r="AGA65" s="0"/>
+      <c r="AGB65" s="0"/>
+      <c r="AGC65" s="0"/>
+      <c r="AGD65" s="0"/>
+      <c r="AGE65" s="0"/>
+      <c r="AGF65" s="0"/>
+      <c r="AGG65" s="0"/>
+      <c r="AGH65" s="0"/>
+      <c r="AGI65" s="0"/>
+      <c r="AGJ65" s="0"/>
+      <c r="AGK65" s="0"/>
+      <c r="AGL65" s="0"/>
+      <c r="AGM65" s="0"/>
+      <c r="AGN65" s="0"/>
+      <c r="AGO65" s="0"/>
+      <c r="AGP65" s="0"/>
+      <c r="AGQ65" s="0"/>
+      <c r="AGR65" s="0"/>
+      <c r="AGS65" s="0"/>
+      <c r="AGT65" s="0"/>
+      <c r="AGU65" s="0"/>
+      <c r="AGV65" s="0"/>
+      <c r="AGW65" s="0"/>
+      <c r="AGX65" s="0"/>
+      <c r="AGY65" s="0"/>
+      <c r="AGZ65" s="0"/>
+      <c r="AHA65" s="0"/>
+      <c r="AHB65" s="0"/>
+      <c r="AHC65" s="0"/>
+      <c r="AHD65" s="0"/>
+      <c r="AHE65" s="0"/>
+      <c r="AHF65" s="0"/>
+      <c r="AHG65" s="0"/>
+      <c r="AHH65" s="0"/>
+      <c r="AHI65" s="0"/>
+      <c r="AHJ65" s="0"/>
+      <c r="AHK65" s="0"/>
+      <c r="AHL65" s="0"/>
+      <c r="AHM65" s="0"/>
+      <c r="AHN65" s="0"/>
+      <c r="AHO65" s="0"/>
+      <c r="AHP65" s="0"/>
+      <c r="AHQ65" s="0"/>
+      <c r="AHR65" s="0"/>
+      <c r="AHS65" s="0"/>
+      <c r="AHT65" s="0"/>
+      <c r="AHU65" s="0"/>
+      <c r="AHV65" s="0"/>
+      <c r="AHW65" s="0"/>
+      <c r="AHX65" s="0"/>
+      <c r="AHY65" s="0"/>
+      <c r="AHZ65" s="0"/>
+      <c r="AIA65" s="0"/>
+      <c r="AIB65" s="0"/>
+      <c r="AIC65" s="0"/>
+      <c r="AID65" s="0"/>
+      <c r="AIE65" s="0"/>
+      <c r="AIF65" s="0"/>
+      <c r="AIG65" s="0"/>
+      <c r="AIH65" s="0"/>
+      <c r="AII65" s="0"/>
+      <c r="AIJ65" s="0"/>
+      <c r="AIK65" s="0"/>
+      <c r="AIL65" s="0"/>
+      <c r="AIM65" s="0"/>
+      <c r="AIN65" s="0"/>
+      <c r="AIO65" s="0"/>
+      <c r="AIP65" s="0"/>
+      <c r="AIQ65" s="0"/>
+      <c r="AIR65" s="0"/>
+      <c r="AIS65" s="0"/>
+      <c r="AIT65" s="0"/>
+      <c r="AIU65" s="0"/>
+      <c r="AIV65" s="0"/>
+      <c r="AIW65" s="0"/>
+      <c r="AIX65" s="0"/>
+      <c r="AIY65" s="0"/>
+      <c r="AIZ65" s="0"/>
+      <c r="AJA65" s="0"/>
+      <c r="AJB65" s="0"/>
+      <c r="AJC65" s="0"/>
+      <c r="AJD65" s="0"/>
+      <c r="AJE65" s="0"/>
+      <c r="AJF65" s="0"/>
+      <c r="AJG65" s="0"/>
+      <c r="AJH65" s="0"/>
+      <c r="AJI65" s="0"/>
+      <c r="AJJ65" s="0"/>
+      <c r="AJK65" s="0"/>
+      <c r="AJL65" s="0"/>
+      <c r="AJM65" s="0"/>
+      <c r="AJN65" s="0"/>
+      <c r="AJO65" s="0"/>
+      <c r="AJP65" s="0"/>
+      <c r="AJQ65" s="0"/>
+      <c r="AJR65" s="0"/>
+      <c r="AJS65" s="0"/>
+      <c r="AJT65" s="0"/>
+      <c r="AJU65" s="0"/>
+      <c r="AJV65" s="0"/>
+      <c r="AJW65" s="0"/>
+      <c r="AJX65" s="0"/>
+      <c r="AJY65" s="0"/>
+      <c r="AJZ65" s="0"/>
+      <c r="AKA65" s="0"/>
+      <c r="AKB65" s="0"/>
+      <c r="AKC65" s="0"/>
+      <c r="AKD65" s="0"/>
+      <c r="AKE65" s="0"/>
+      <c r="AKF65" s="0"/>
+      <c r="AKG65" s="0"/>
+      <c r="AKH65" s="0"/>
+      <c r="AKI65" s="0"/>
+      <c r="AKJ65" s="0"/>
+      <c r="AKK65" s="0"/>
+      <c r="AKL65" s="0"/>
+      <c r="AKM65" s="0"/>
+      <c r="AKN65" s="0"/>
+      <c r="AKO65" s="0"/>
+      <c r="AKP65" s="0"/>
+      <c r="AKQ65" s="0"/>
+      <c r="AKR65" s="0"/>
+      <c r="AKS65" s="0"/>
+      <c r="AKT65" s="0"/>
+      <c r="AKU65" s="0"/>
+      <c r="AKV65" s="0"/>
+      <c r="AKW65" s="0"/>
+      <c r="AKX65" s="0"/>
+      <c r="AKY65" s="0"/>
+      <c r="AKZ65" s="0"/>
+      <c r="ALA65" s="0"/>
+      <c r="ALB65" s="0"/>
+      <c r="ALC65" s="0"/>
+      <c r="ALD65" s="0"/>
+      <c r="ALE65" s="0"/>
+      <c r="ALF65" s="0"/>
+      <c r="ALG65" s="0"/>
+      <c r="ALH65" s="0"/>
+      <c r="ALI65" s="0"/>
+      <c r="ALJ65" s="0"/>
+      <c r="ALK65" s="0"/>
+      <c r="ALL65" s="0"/>
+      <c r="ALM65" s="0"/>
+      <c r="ALN65" s="0"/>
+      <c r="ALO65" s="0"/>
+      <c r="ALP65" s="0"/>
+      <c r="ALQ65" s="0"/>
+      <c r="ALR65" s="0"/>
+      <c r="ALS65" s="0"/>
+      <c r="ALT65" s="0"/>
+      <c r="ALU65" s="0"/>
+      <c r="ALV65" s="0"/>
+      <c r="ALW65" s="0"/>
+      <c r="ALX65" s="0"/>
+      <c r="ALY65" s="0"/>
+      <c r="ALZ65" s="0"/>
+      <c r="AMA65" s="0"/>
+      <c r="AMB65" s="0"/>
+      <c r="AMC65" s="0"/>
+      <c r="AMD65" s="0"/>
+      <c r="AME65" s="0"/>
+      <c r="AMF65" s="0"/>
+      <c r="AMG65" s="0"/>
+      <c r="AMH65" s="0"/>
+      <c r="AMI65" s="0"/>
+      <c r="AMJ65" s="0"/>
+    </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7680,6 +9774,8 @@
     <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:H36"/>
   <mergeCells count="2">

</xml_diff>